<commit_message>
fear: export/save to single file
</commit_message>
<xml_diff>
--- a/src/assets/sppd.xlsx
+++ b/src/assets/sppd.xlsx
@@ -3,19 +3,20 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4804D25-4953-4096-AD8D-BE543D62625C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0455A82-8B2F-4573-8A2A-D843313B71E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Surat tugas 1 org" sheetId="1" r:id="rId1"/>
-    <sheet name="sppd depan 1" sheetId="2" r:id="rId2"/>
-    <sheet name="sppd blkg 1" sheetId="3" r:id="rId3"/>
+    <sheet name="data" sheetId="4" r:id="rId1"/>
+    <sheet name="surat_tugas" sheetId="1" r:id="rId2"/>
+    <sheet name="sppd_depan" sheetId="2" r:id="rId3"/>
+    <sheet name="sppd_belakang" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="2">'sppd blkg 1'!$A$1:$F$70</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">'sppd depan 1'!$A$1:$E$39</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Surat tugas 1 org'!$A$1:$H$46</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="3">sppd_belakang!$A$1:$F$70</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">sppd_depan!$A$1:$E$39</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">surat_tugas!$A$1:$H$46</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="98">
   <si>
     <t>SURAT TUGAS</t>
   </si>
@@ -99,9 +100,6 @@
   </si>
   <si>
     <t>........................................</t>
-  </si>
-  <si>
-    <t>Nomor : 449.1/      /UKM/2023</t>
   </si>
   <si>
     <t>Berdasarkan : Peraturan Daerah Kabupaten Semarang Nomor 9 tahun  2022 tentang anggaran Pendapatan dan Belanja Daerah Kab.Semarang tahun anggaran 2023 dan Peraturan Bupati Semarang Nomor 118 tahun 2022 Tentang penjabaran anggaran Pendapatan dan belanja daerah Kabupaten Semarang Tahun 2023</t>
@@ -515,14 +513,39 @@
   <si>
     <t>Pada Tanggal</t>
   </si>
+  <si>
+    <t>nama</t>
+  </si>
+  <si>
+    <t>nip</t>
+  </si>
+  <si>
+    <t>golongan</t>
+  </si>
+  <si>
+    <t>jabatan</t>
+  </si>
+  <si>
+    <t>tanggal</t>
+  </si>
+  <si>
+    <t>tujuan</t>
+  </si>
+  <si>
+    <t>tempat</t>
+  </si>
+  <si>
+    <t>nomor</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="[$-421]dd\ mmmm\ yyyy;@"/>
     <numFmt numFmtId="165" formatCode="[$-409]dd\-mmm\-yy;@"/>
+    <numFmt numFmtId="166" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
   <fonts count="30" x14ac:knownFonts="1">
     <font>
@@ -1278,12 +1301,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1292,153 +1309,6 @@
     </xf>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="19" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="23" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="24" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1450,6 +1320,157 @@
     <xf numFmtId="0" fontId="22" fillId="2" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="19" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="23" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="24" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1999,11 +2020,74 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15277BD0-1E06-4977-8B5E-1D678D3D00DE}">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="27.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B5" s="116"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>97</v>
+      </c>
+      <c r="B8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H52"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A14" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2032,28 +2116,28 @@
     <row r="2" spans="1:8" s="6" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="C2" s="7"/>
-      <c r="D2" s="114"/>
-      <c r="E2" s="114"/>
-      <c r="F2" s="114"/>
-      <c r="G2" s="114"/>
+      <c r="D2" s="119"/>
+      <c r="E2" s="119"/>
+      <c r="F2" s="119"/>
+      <c r="G2" s="119"/>
       <c r="H2" s="5"/>
     </row>
     <row r="3" spans="1:8" s="6" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="C3" s="7"/>
-      <c r="D3" s="115"/>
-      <c r="E3" s="115"/>
-      <c r="F3" s="115"/>
-      <c r="G3" s="115"/>
+      <c r="D3" s="120"/>
+      <c r="E3" s="120"/>
+      <c r="F3" s="120"/>
+      <c r="G3" s="120"/>
       <c r="H3" s="8"/>
     </row>
     <row r="4" spans="1:8" s="6" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="C4" s="7"/>
-      <c r="D4" s="116"/>
-      <c r="E4" s="116"/>
-      <c r="F4" s="116"/>
-      <c r="G4" s="116"/>
+      <c r="D4" s="121"/>
+      <c r="E4" s="121"/>
+      <c r="F4" s="121"/>
+      <c r="G4" s="121"/>
       <c r="H4" s="8"/>
     </row>
     <row r="5" spans="1:8" s="9" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2067,25 +2151,26 @@
     </row>
     <row r="6" spans="1:8" s="14" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
-      <c r="B6" s="117" t="s">
+      <c r="B6" s="122" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="117"/>
-      <c r="D6" s="117"/>
-      <c r="E6" s="117"/>
-      <c r="F6" s="117"/>
-      <c r="G6" s="117"/>
+      <c r="C6" s="122"/>
+      <c r="D6" s="122"/>
+      <c r="E6" s="122"/>
+      <c r="F6" s="122"/>
+      <c r="G6" s="122"/>
     </row>
     <row r="7" spans="1:8" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
-      <c r="B7" s="118" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="118"/>
-      <c r="D7" s="118"/>
-      <c r="E7" s="118"/>
-      <c r="F7" s="118"/>
-      <c r="G7" s="118"/>
+      <c r="B7" s="123" t="str">
+        <f>data!B8</f>
+        <v>Nomor : 449.1/        /UKM/2023</v>
+      </c>
+      <c r="C7" s="123"/>
+      <c r="D7" s="123"/>
+      <c r="E7" s="123"/>
+      <c r="F7" s="123"/>
+      <c r="G7" s="123"/>
     </row>
     <row r="8" spans="1:8" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
@@ -2098,34 +2183,34 @@
     </row>
     <row r="9" spans="1:8" s="14" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
-      <c r="B9" s="119" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="119"/>
-      <c r="D9" s="119"/>
-      <c r="E9" s="119"/>
-      <c r="F9" s="119"/>
-      <c r="G9" s="119"/>
+      <c r="B9" s="124" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="124"/>
+      <c r="D9" s="124"/>
+      <c r="E9" s="124"/>
+      <c r="F9" s="124"/>
+      <c r="G9" s="124"/>
     </row>
     <row r="10" spans="1:8" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
-      <c r="B10" s="122"/>
-      <c r="C10" s="122"/>
-      <c r="D10" s="122"/>
-      <c r="E10" s="122"/>
-      <c r="F10" s="122"/>
-      <c r="G10" s="122"/>
+      <c r="B10" s="125"/>
+      <c r="C10" s="125"/>
+      <c r="D10" s="125"/>
+      <c r="E10" s="125"/>
+      <c r="F10" s="125"/>
+      <c r="G10" s="125"/>
     </row>
     <row r="11" spans="1:8" s="17" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="16"/>
-      <c r="B11" s="113" t="s">
+      <c r="B11" s="118" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="113"/>
-      <c r="D11" s="113"/>
-      <c r="E11" s="113"/>
-      <c r="F11" s="113"/>
-      <c r="G11" s="113"/>
+      <c r="C11" s="118"/>
+      <c r="D11" s="118"/>
+      <c r="E11" s="118"/>
+      <c r="F11" s="118"/>
+      <c r="G11" s="118"/>
     </row>
     <row r="12" spans="1:8" s="17" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="16"/>
@@ -2133,8 +2218,8 @@
       <c r="C12" s="16"/>
       <c r="D12" s="19"/>
       <c r="E12" s="20"/>
-      <c r="F12" s="113"/>
-      <c r="G12" s="113"/>
+      <c r="F12" s="118"/>
+      <c r="G12" s="118"/>
     </row>
     <row r="13" spans="1:8" s="17" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="16"/>
@@ -2147,9 +2232,12 @@
       <c r="D13" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="E13" s="107"/>
-      <c r="F13" s="113"/>
-      <c r="G13" s="113"/>
+      <c r="E13" s="107">
+        <f>data!B1</f>
+        <v>0</v>
+      </c>
+      <c r="F13" s="118"/>
+      <c r="G13" s="118"/>
     </row>
     <row r="14" spans="1:8" s="17" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16"/>
@@ -2160,9 +2248,12 @@
       <c r="D14" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="E14" s="108"/>
-      <c r="F14" s="113"/>
-      <c r="G14" s="113"/>
+      <c r="E14" s="107">
+        <f>data!B2</f>
+        <v>0</v>
+      </c>
+      <c r="F14" s="118"/>
+      <c r="G14" s="118"/>
     </row>
     <row r="15" spans="1:8" s="17" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="16"/>
@@ -2173,7 +2264,10 @@
       <c r="D15" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="E15" s="109"/>
+      <c r="E15" s="107">
+        <f>data!B3</f>
+        <v>0</v>
+      </c>
       <c r="F15" s="19"/>
       <c r="G15" s="22" t="s">
         <v>7</v>
@@ -2188,7 +2282,10 @@
       <c r="D16" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="E16" s="109"/>
+      <c r="E16" s="107">
+        <f>data!B4</f>
+        <v>0</v>
+      </c>
       <c r="F16" s="3"/>
       <c r="G16" s="4"/>
     </row>
@@ -2204,10 +2301,10 @@
         <v>4</v>
       </c>
       <c r="E17" s="20"/>
-      <c r="F17" s="113" t="s">
+      <c r="F17" s="118" t="s">
         <v>10</v>
       </c>
-      <c r="G17" s="113"/>
+      <c r="G17" s="118"/>
     </row>
     <row r="18" spans="1:7" s="17" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="16"/>
@@ -2219,8 +2316,8 @@
         <v>4</v>
       </c>
       <c r="E18" s="20"/>
-      <c r="F18" s="113"/>
-      <c r="G18" s="113"/>
+      <c r="F18" s="118"/>
+      <c r="G18" s="118"/>
     </row>
     <row r="19" spans="1:7" s="17" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="16"/>
@@ -2292,9 +2389,12 @@
       <c r="D24" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="E24" s="20"/>
+      <c r="E24" s="117">
+        <f>data!B6</f>
+        <v>0</v>
+      </c>
       <c r="F24" s="20"/>
-      <c r="G24" s="111"/>
+      <c r="G24" s="109"/>
     </row>
     <row r="25" spans="1:7" s="14" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
@@ -2305,7 +2405,10 @@
       <c r="D25" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="E25" s="20"/>
+      <c r="E25" s="117">
+        <f>data!B7</f>
+        <v>0</v>
+      </c>
       <c r="F25" s="25"/>
       <c r="G25" s="4"/>
     </row>
@@ -2338,10 +2441,10 @@
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
       <c r="E28" s="27"/>
-      <c r="F28" s="118" t="s">
+      <c r="F28" s="123" t="s">
         <v>17</v>
       </c>
-      <c r="G28" s="118"/>
+      <c r="G28" s="123"/>
     </row>
     <row r="29" spans="1:7" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
@@ -2349,10 +2452,10 @@
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
       <c r="E29" s="27"/>
-      <c r="F29" s="118" t="s">
+      <c r="F29" s="123" t="s">
         <v>18</v>
       </c>
-      <c r="G29" s="118"/>
+      <c r="G29" s="123"/>
     </row>
     <row r="30" spans="1:7" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
@@ -2385,10 +2488,10 @@
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
       <c r="E33" s="27"/>
-      <c r="F33" s="121" t="s">
+      <c r="F33" s="127" t="s">
         <v>19</v>
       </c>
-      <c r="G33" s="121"/>
+      <c r="G33" s="127"/>
       <c r="H33" s="31"/>
     </row>
     <row r="34" spans="1:8" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -2397,10 +2500,10 @@
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
       <c r="E34" s="27"/>
-      <c r="F34" s="120" t="s">
+      <c r="F34" s="126" t="s">
         <v>20</v>
       </c>
-      <c r="G34" s="120"/>
+      <c r="G34" s="126"/>
       <c r="H34" s="32"/>
     </row>
     <row r="35" spans="1:8" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -2430,7 +2533,7 @@
       <c r="D37" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="E37" s="162">
+      <c r="E37" s="111">
         <f>E13</f>
         <v>0</v>
       </c>
@@ -2445,7 +2548,7 @@
       <c r="D38" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="E38" s="163">
+      <c r="E38" s="112">
         <f>E14</f>
         <v>0</v>
       </c>
@@ -2523,12 +2626,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K39"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A5" zoomScale="90" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView view="pageBreakPreview" zoomScale="90" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2543,35 +2646,35 @@
   <sheetData>
     <row r="1" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C1" s="35" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D1" s="35"/>
       <c r="E1" s="35"/>
     </row>
     <row r="2" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C2" s="35" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D2" s="35"/>
       <c r="E2" s="35"/>
     </row>
     <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.4">
       <c r="C3" s="36" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D3" s="36"/>
       <c r="E3" s="36"/>
     </row>
     <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
     </row>
     <row r="5" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="37" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B5" s="38"/>
       <c r="C5" s="38"/>
@@ -2582,23 +2685,23 @@
       <c r="B6" s="3"/>
     </row>
     <row r="7" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="141" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7" s="141"/>
-      <c r="C7" s="141"/>
-      <c r="D7" s="141"/>
-      <c r="E7" s="141"/>
+      <c r="A7" s="146" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="146"/>
+      <c r="C7" s="146"/>
+      <c r="D7" s="146"/>
+      <c r="E7" s="146"/>
       <c r="I7" s="39"/>
     </row>
     <row r="8" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="118" t="s">
-        <v>89</v>
-      </c>
-      <c r="B8" s="118"/>
-      <c r="C8" s="118"/>
-      <c r="D8" s="118"/>
-      <c r="E8" s="118"/>
+      <c r="A8" s="123" t="s">
+        <v>88</v>
+      </c>
+      <c r="B8" s="123"/>
+      <c r="C8" s="123"/>
+      <c r="D8" s="123"/>
+      <c r="E8" s="123"/>
       <c r="I8" s="39"/>
     </row>
     <row r="9" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -2613,22 +2716,22 @@
         <v>1</v>
       </c>
       <c r="C10" s="42" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="147" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="142" t="s">
-        <v>32</v>
-      </c>
-      <c r="E10" s="143"/>
+      <c r="E10" s="148"/>
     </row>
     <row r="11" spans="1:11" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="43">
         <v>2</v>
       </c>
       <c r="C11" s="44" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D11" s="45">
-        <f>'Surat tugas 1 org'!E13</f>
+        <f>data!B1</f>
         <v>0</v>
       </c>
       <c r="E11" s="46"/>
@@ -2636,49 +2739,49 @@
     <row r="12" spans="1:11" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="43"/>
       <c r="C12" s="44"/>
-      <c r="D12" s="144"/>
-      <c r="E12" s="145"/>
+      <c r="D12" s="149"/>
+      <c r="E12" s="150"/>
       <c r="H12" s="39"/>
       <c r="K12" s="39"/>
     </row>
     <row r="13" spans="1:11" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="129">
+      <c r="B13" s="134">
         <v>3</v>
       </c>
       <c r="C13" s="47" t="s">
-        <v>34</v>
-      </c>
-      <c r="D13" s="146">
-        <f>'Surat tugas 1 org'!E15</f>
-        <v>0</v>
-      </c>
-      <c r="E13" s="147"/>
+        <v>33</v>
+      </c>
+      <c r="D13" s="151" t="str">
+        <f>data!A3</f>
+        <v>golongan</v>
+      </c>
+      <c r="E13" s="152"/>
       <c r="H13" s="39"/>
       <c r="K13" s="39"/>
     </row>
     <row r="14" spans="1:11" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="129"/>
+      <c r="B14" s="134"/>
       <c r="C14" s="44" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="153"/>
+      <c r="E14" s="154"/>
+    </row>
+    <row r="15" spans="1:11" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="134"/>
+      <c r="C15" s="44" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="148"/>
-      <c r="E14" s="149"/>
-    </row>
-    <row r="15" spans="1:11" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="129"/>
-      <c r="C15" s="44" t="s">
+      <c r="D15" s="48">
+        <f>data!B4</f>
+        <v>0</v>
+      </c>
+      <c r="E15" s="49"/>
+    </row>
+    <row r="16" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="145"/>
+      <c r="C16" s="44" t="s">
         <v>36</v>
-      </c>
-      <c r="D15" s="48">
-        <f>'Surat tugas 1 org'!E16</f>
-        <v>0</v>
-      </c>
-      <c r="E15" s="49"/>
-    </row>
-    <row r="16" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="140"/>
-      <c r="C16" s="44" t="s">
-        <v>37</v>
       </c>
       <c r="D16" s="50"/>
       <c r="E16" s="51"/>
@@ -2689,13 +2792,13 @@
         <v>4</v>
       </c>
       <c r="C17" s="42" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D17" s="102">
-        <f>'Surat tugas 1 org'!E24</f>
+        <f>data!B6</f>
         <v>0</v>
       </c>
-      <c r="E17" s="110"/>
+      <c r="E17" s="108"/>
       <c r="H17" s="39"/>
     </row>
     <row r="18" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -2703,85 +2806,82 @@
         <v>5</v>
       </c>
       <c r="C18" s="52" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" s="141" t="s">
         <v>39</v>
       </c>
-      <c r="D18" s="136" t="s">
+      <c r="E18" s="142"/>
+      <c r="H18" s="39"/>
+    </row>
+    <row r="19" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="134">
+        <v>6</v>
+      </c>
+      <c r="C19" s="47" t="s">
         <v>40</v>
       </c>
-      <c r="E18" s="137"/>
-      <c r="H18" s="39"/>
-    </row>
-    <row r="19" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="129">
-        <v>6</v>
-      </c>
-      <c r="C19" s="47" t="s">
+      <c r="D19" s="131" t="s">
         <v>41</v>
       </c>
-      <c r="D19" s="126" t="s">
+      <c r="E19" s="132"/>
+    </row>
+    <row r="20" spans="2:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="134"/>
+      <c r="C20" s="53" t="s">
         <v>42</v>
       </c>
-      <c r="E19" s="127"/>
-    </row>
-    <row r="20" spans="2:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="129"/>
-      <c r="C20" s="53" t="s">
+      <c r="D20" s="143">
+        <f>data!B7</f>
+        <v>0</v>
+      </c>
+      <c r="E20" s="144"/>
+    </row>
+    <row r="21" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="134">
+        <v>7</v>
+      </c>
+      <c r="C21" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="D20" s="138">
-        <f>'Surat tugas 1 org'!E25</f>
-        <v>0</v>
-      </c>
-      <c r="E20" s="139"/>
-    </row>
-    <row r="21" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="129">
-        <v>7</v>
-      </c>
-      <c r="C21" s="47" t="s">
+      <c r="D21" s="131" t="s">
         <v>44</v>
       </c>
-      <c r="D21" s="126" t="s">
+      <c r="E21" s="132"/>
+    </row>
+    <row r="22" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="134"/>
+      <c r="C22" s="44" t="s">
         <v>45</v>
       </c>
-      <c r="E21" s="127"/>
-    </row>
-    <row r="22" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="129"/>
-      <c r="C22" s="44" t="s">
+      <c r="D22" s="54"/>
+      <c r="E22" s="106"/>
+    </row>
+    <row r="23" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="145"/>
+      <c r="C23" s="44" t="s">
         <v>46</v>
-      </c>
-      <c r="D22" s="54">
-        <f>'Surat tugas 1 org'!E23</f>
-        <v>0</v>
-      </c>
-      <c r="E22" s="106"/>
-    </row>
-    <row r="23" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="140"/>
-      <c r="C23" s="44" t="s">
-        <v>47</v>
       </c>
       <c r="D23" s="54">
         <f>D22</f>
         <v>0</v>
       </c>
-      <c r="E23" s="112"/>
+      <c r="E23" s="110"/>
     </row>
     <row r="24" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="124">
+      <c r="B24" s="129">
         <v>8</v>
       </c>
       <c r="C24" s="56" t="s">
-        <v>48</v>
-      </c>
-      <c r="D24" s="126" t="s">
+        <v>47</v>
+      </c>
+      <c r="D24" s="131" t="s">
         <v>6</v>
       </c>
-      <c r="E24" s="127"/>
+      <c r="E24" s="132"/>
     </row>
     <row r="25" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="125"/>
+      <c r="B25" s="130"/>
       <c r="C25" s="48"/>
       <c r="D25" s="57"/>
       <c r="E25" s="49"/>
@@ -2789,51 +2889,51 @@
     <row r="26" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="58"/>
       <c r="C26" s="59" t="s">
+        <v>48</v>
+      </c>
+      <c r="D26" s="60" t="s">
         <v>49</v>
       </c>
-      <c r="D26" s="60" t="s">
+      <c r="E26" s="49"/>
+    </row>
+    <row r="27" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="133">
+        <v>9</v>
+      </c>
+      <c r="C27" s="61" t="s">
         <v>50</v>
       </c>
-      <c r="E26" s="49"/>
-    </row>
-    <row r="27" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="128">
-        <v>9</v>
-      </c>
-      <c r="C27" s="61" t="s">
+      <c r="D27" s="135" t="s">
         <v>51</v>
       </c>
-      <c r="D27" s="130" t="s">
+      <c r="E27" s="136"/>
+    </row>
+    <row r="28" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="134"/>
+      <c r="C28" s="61" t="s">
         <v>52</v>
       </c>
-      <c r="E27" s="131"/>
-    </row>
-    <row r="28" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="129"/>
-      <c r="C28" s="61" t="s">
+      <c r="D28" s="137" t="s">
         <v>53</v>
       </c>
-      <c r="D28" s="132" t="s">
+      <c r="E28" s="138"/>
+    </row>
+    <row r="29" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="134"/>
+      <c r="C29" s="62" t="s">
         <v>54</v>
       </c>
-      <c r="E28" s="133"/>
-    </row>
-    <row r="29" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="129"/>
-      <c r="C29" s="62" t="s">
+      <c r="D29" s="139" t="s">
         <v>55</v>
       </c>
-      <c r="D29" s="134" t="s">
-        <v>56</v>
-      </c>
-      <c r="E29" s="135"/>
+      <c r="E29" s="140"/>
     </row>
     <row r="30" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="63">
         <v>10</v>
       </c>
       <c r="C30" s="64" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D30" s="42"/>
       <c r="E30" s="65"/>
@@ -2841,12 +2941,12 @@
     <row r="31" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="32" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D32" s="66" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="33" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D33" s="67" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E33" s="55">
         <f>D22</f>
@@ -2857,10 +2957,10 @@
     <row r="34" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="33"/>
       <c r="C34" s="33"/>
-      <c r="D34" s="123" t="s">
-        <v>32</v>
-      </c>
-      <c r="E34" s="123"/>
+      <c r="D34" s="128" t="s">
+        <v>31</v>
+      </c>
+      <c r="E34" s="128"/>
     </row>
     <row r="35" spans="2:6" s="33" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D35" s="68"/>
@@ -2872,16 +2972,16 @@
       <c r="D37" s="68"/>
     </row>
     <row r="38" spans="2:6" s="33" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D38" s="121" t="s">
+      <c r="D38" s="127" t="s">
         <v>19</v>
       </c>
-      <c r="E38" s="121"/>
+      <c r="E38" s="127"/>
     </row>
     <row r="39" spans="2:6" s="33" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D39" s="120" t="s">
+      <c r="D39" s="126" t="s">
         <v>20</v>
       </c>
-      <c r="E39" s="120"/>
+      <c r="E39" s="126"/>
     </row>
   </sheetData>
   <mergeCells count="22">
@@ -2914,12 +3014,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:G82"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A35" zoomScale="86" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C61" sqref="C61:F61"/>
+    <sheetView view="pageBreakPreview" zoomScale="86" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2941,40 +3041,37 @@
     <row r="3" spans="2:7" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="2:7" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="33" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="2:7" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E5" s="33" t="str">
-        <f t="array" ref="E5">'sppd depan 1'!A8:A8</f>
+        <f>data!B8</f>
         <v>Nomor : 449.1/        /UKM/2023</v>
       </c>
     </row>
     <row r="6" spans="2:7" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E6" s="66" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="2:7" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E7" s="66" t="s">
-        <v>90</v>
-      </c>
-      <c r="F7" s="69">
-        <f>'sppd depan 1'!D22</f>
-        <v>0</v>
-      </c>
+        <v>89</v>
+      </c>
+      <c r="F7" s="69"/>
     </row>
     <row r="8" spans="2:7" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C8" s="70"/>
       <c r="D8" s="70"/>
       <c r="E8" s="66" t="s">
-        <v>62</v>
-      </c>
-      <c r="F8" s="158">
-        <f>'Surat tugas 1 org'!E25</f>
+        <v>61</v>
+      </c>
+      <c r="F8" s="163">
+        <f>data!B7</f>
         <v>0</v>
       </c>
-      <c r="G8" s="158"/>
+      <c r="G8" s="163"/>
     </row>
     <row r="9" spans="2:7" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E9" s="71"/>
@@ -2984,29 +3081,29 @@
     </row>
     <row r="11" spans="2:7" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="72" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" s="73" t="s">
         <v>63</v>
-      </c>
-      <c r="C11" s="73" t="s">
-        <v>64</v>
       </c>
       <c r="D11" s="73"/>
       <c r="E11" s="74" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F11" s="75"/>
     </row>
     <row r="12" spans="2:7" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="76"/>
-      <c r="C12" s="159">
-        <f>'Surat tugas 1 org'!E25</f>
+      <c r="C12" s="164">
+        <f>F8</f>
         <v>0</v>
       </c>
-      <c r="D12" s="159"/>
-      <c r="E12" s="160">
+      <c r="D12" s="164"/>
+      <c r="E12" s="165">
         <f>C12</f>
         <v>0</v>
       </c>
-      <c r="F12" s="161"/>
+      <c r="F12" s="166"/>
     </row>
     <row r="13" spans="2:7" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="76"/>
@@ -3015,7 +3112,7 @@
         <v>Pada Tanggal</v>
       </c>
       <c r="D13" s="69">
-        <f>'Surat tugas 1 org'!E23</f>
+        <f>F7</f>
         <v>0</v>
       </c>
       <c r="E13" s="48" t="str">
@@ -3032,20 +3129,20 @@
       <c r="C14" s="66"/>
       <c r="D14" s="66"/>
       <c r="E14" s="48" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F14" s="78"/>
     </row>
     <row r="15" spans="2:7" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="76"/>
-      <c r="C15" s="123" t="s">
-        <v>67</v>
-      </c>
-      <c r="D15" s="123"/>
-      <c r="E15" s="156" t="s">
-        <v>67</v>
-      </c>
-      <c r="F15" s="155"/>
+      <c r="C15" s="128" t="s">
+        <v>66</v>
+      </c>
+      <c r="D15" s="128"/>
+      <c r="E15" s="161" t="s">
+        <v>66</v>
+      </c>
+      <c r="F15" s="160"/>
     </row>
     <row r="16" spans="2:7" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="76"/>
@@ -3067,59 +3164,59 @@
     </row>
     <row r="19" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="76"/>
-      <c r="C19" s="150" t="s">
-        <v>68</v>
-      </c>
-      <c r="D19" s="150"/>
-      <c r="E19" s="157" t="s">
-        <v>68</v>
-      </c>
-      <c r="F19" s="154"/>
+      <c r="C19" s="155" t="s">
+        <v>67</v>
+      </c>
+      <c r="D19" s="155"/>
+      <c r="E19" s="162" t="s">
+        <v>67</v>
+      </c>
+      <c r="F19" s="159"/>
     </row>
     <row r="20" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="80"/>
       <c r="C20" s="81" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D20" s="82"/>
       <c r="E20" s="83" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F20" s="84"/>
     </row>
     <row r="21" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="72" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C21" s="73"/>
       <c r="D21" s="75"/>
       <c r="E21" s="74" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F21" s="75"/>
     </row>
     <row r="22" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="76"/>
       <c r="C22" s="66" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D22" s="85">
         <f>C12</f>
         <v>0</v>
       </c>
-      <c r="E22" s="166" t="s">
-        <v>71</v>
+      <c r="E22" s="115" t="s">
+        <v>70</v>
       </c>
       <c r="F22" s="86"/>
     </row>
     <row r="23" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="76"/>
       <c r="C23" s="66" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D23" s="87"/>
       <c r="E23" s="48" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F23" s="87"/>
     </row>
@@ -3128,20 +3225,20 @@
       <c r="C24" s="66"/>
       <c r="D24" s="78"/>
       <c r="E24" s="48" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F24" s="78"/>
     </row>
     <row r="25" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="76"/>
-      <c r="C25" s="123" t="s">
-        <v>67</v>
-      </c>
-      <c r="D25" s="155"/>
-      <c r="E25" s="156" t="s">
-        <v>67</v>
-      </c>
-      <c r="F25" s="155"/>
+      <c r="C25" s="128" t="s">
+        <v>66</v>
+      </c>
+      <c r="D25" s="160"/>
+      <c r="E25" s="161" t="s">
+        <v>66</v>
+      </c>
+      <c r="F25" s="160"/>
     </row>
     <row r="26" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="76"/>
@@ -3163,56 +3260,56 @@
     </row>
     <row r="29" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="76"/>
-      <c r="C29" s="150" t="s">
-        <v>68</v>
-      </c>
-      <c r="D29" s="154"/>
-      <c r="E29" s="150" t="s">
-        <v>68</v>
-      </c>
-      <c r="F29" s="154"/>
+      <c r="C29" s="155" t="s">
+        <v>67</v>
+      </c>
+      <c r="D29" s="159"/>
+      <c r="E29" s="155" t="s">
+        <v>67</v>
+      </c>
+      <c r="F29" s="159"/>
     </row>
     <row r="30" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="80"/>
       <c r="C30" s="81" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D30" s="84"/>
       <c r="E30" s="83" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F30" s="84"/>
     </row>
     <row r="31" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="72" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C31" s="73"/>
       <c r="D31" s="75"/>
       <c r="E31" s="74" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F31" s="75"/>
     </row>
     <row r="32" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="76"/>
       <c r="C32" s="66" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D32" s="89"/>
-      <c r="E32" s="165" t="s">
-        <v>75</v>
+      <c r="E32" s="114" t="s">
+        <v>74</v>
       </c>
       <c r="F32" s="90"/>
     </row>
     <row r="33" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="76"/>
       <c r="C33" s="66" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D33" s="91"/>
-      <c r="E33" s="164" t="s">
-        <v>72</v>
+      <c r="E33" s="113" t="s">
+        <v>71</v>
       </c>
       <c r="F33" s="91"/>
     </row>
@@ -3220,20 +3317,20 @@
       <c r="B34" s="76"/>
       <c r="C34" s="66"/>
       <c r="E34" s="48" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F34" s="92"/>
     </row>
     <row r="35" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="76"/>
-      <c r="C35" s="123" t="s">
-        <v>67</v>
-      </c>
-      <c r="D35" s="155"/>
-      <c r="E35" s="156" t="s">
-        <v>67</v>
-      </c>
-      <c r="F35" s="155"/>
+      <c r="C35" s="128" t="s">
+        <v>66</v>
+      </c>
+      <c r="D35" s="160"/>
+      <c r="E35" s="161" t="s">
+        <v>66</v>
+      </c>
+      <c r="F35" s="160"/>
     </row>
     <row r="36" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="76"/>
@@ -3255,41 +3352,41 @@
     </row>
     <row r="39" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="76"/>
-      <c r="C39" s="150" t="s">
-        <v>68</v>
-      </c>
-      <c r="D39" s="154"/>
-      <c r="E39" s="150" t="s">
-        <v>68</v>
-      </c>
-      <c r="F39" s="154"/>
+      <c r="C39" s="155" t="s">
+        <v>67</v>
+      </c>
+      <c r="D39" s="159"/>
+      <c r="E39" s="155" t="s">
+        <v>67</v>
+      </c>
+      <c r="F39" s="159"/>
     </row>
     <row r="40" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="80"/>
       <c r="C40" s="81" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D40" s="84"/>
       <c r="E40" s="83" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F40" s="84"/>
     </row>
     <row r="41" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="72" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C41" s="73"/>
       <c r="D41" s="75"/>
       <c r="E41" s="74" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F41" s="75"/>
     </row>
     <row r="42" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="76"/>
       <c r="C42" s="66" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D42" s="93"/>
       <c r="E42" s="94"/>
@@ -3298,7 +3395,7 @@
     <row r="43" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="76"/>
       <c r="C43" s="66" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D43" s="87"/>
       <c r="E43" s="88"/>
@@ -3308,20 +3405,20 @@
       <c r="B44" s="76"/>
       <c r="C44" s="66"/>
       <c r="E44" s="48" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F44" s="92"/>
     </row>
     <row r="45" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="76"/>
-      <c r="C45" s="123" t="s">
-        <v>67</v>
-      </c>
-      <c r="D45" s="155"/>
-      <c r="E45" s="156" t="s">
-        <v>67</v>
-      </c>
-      <c r="F45" s="155"/>
+      <c r="C45" s="128" t="s">
+        <v>66</v>
+      </c>
+      <c r="D45" s="160"/>
+      <c r="E45" s="161" t="s">
+        <v>66</v>
+      </c>
+      <c r="F45" s="160"/>
     </row>
     <row r="46" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="76"/>
@@ -3343,32 +3440,32 @@
     </row>
     <row r="49" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="76"/>
-      <c r="C49" s="150" t="s">
-        <v>68</v>
-      </c>
-      <c r="D49" s="154"/>
-      <c r="E49" s="157" t="s">
-        <v>68</v>
-      </c>
-      <c r="F49" s="154"/>
+      <c r="C49" s="155" t="s">
+        <v>67</v>
+      </c>
+      <c r="D49" s="159"/>
+      <c r="E49" s="162" t="s">
+        <v>67</v>
+      </c>
+      <c r="F49" s="159"/>
     </row>
     <row r="50" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="80"/>
       <c r="C50" s="81" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D50" s="84"/>
       <c r="E50" s="83" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F50" s="84"/>
     </row>
     <row r="51" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="76" t="s">
+        <v>76</v>
+      </c>
+      <c r="C51" s="96" t="s">
         <v>77</v>
-      </c>
-      <c r="C51" s="96" t="s">
-        <v>78</v>
       </c>
       <c r="D51" s="96"/>
       <c r="E51" s="96"/>
@@ -3377,22 +3474,22 @@
     <row r="52" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="76"/>
       <c r="C52" s="33" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F52" s="79"/>
     </row>
     <row r="53" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="76"/>
       <c r="C53" s="33" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F53" s="98"/>
     </row>
     <row r="54" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B54" s="76"/>
-      <c r="C54" s="150"/>
-      <c r="D54" s="150"/>
-      <c r="E54" s="150"/>
+      <c r="C54" s="155"/>
+      <c r="D54" s="155"/>
+      <c r="E54" s="155"/>
       <c r="F54" s="99"/>
     </row>
     <row r="55" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3401,12 +3498,12 @@
     </row>
     <row r="56" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B56" s="76"/>
-      <c r="C56" s="118" t="s">
-        <v>32</v>
-      </c>
-      <c r="D56" s="118"/>
-      <c r="E56" s="118"/>
-      <c r="F56" s="151"/>
+      <c r="C56" s="123" t="s">
+        <v>31</v>
+      </c>
+      <c r="D56" s="123"/>
+      <c r="E56" s="123"/>
+      <c r="F56" s="156"/>
     </row>
     <row r="57" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B57" s="76"/>
@@ -3431,21 +3528,21 @@
     </row>
     <row r="60" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B60" s="76"/>
-      <c r="C60" s="152" t="s">
+      <c r="C60" s="157" t="s">
         <v>19</v>
       </c>
-      <c r="D60" s="152"/>
-      <c r="E60" s="152"/>
-      <c r="F60" s="153"/>
+      <c r="D60" s="157"/>
+      <c r="E60" s="157"/>
+      <c r="F60" s="158"/>
     </row>
     <row r="61" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B61" s="76"/>
-      <c r="C61" s="118" t="s">
+      <c r="C61" s="123" t="s">
         <v>20</v>
       </c>
-      <c r="D61" s="118"/>
-      <c r="E61" s="118"/>
-      <c r="F61" s="151"/>
+      <c r="D61" s="123"/>
+      <c r="E61" s="123"/>
+      <c r="F61" s="156"/>
     </row>
     <row r="62" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B62" s="80"/>
@@ -3456,10 +3553,10 @@
     </row>
     <row r="63" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B63" s="102" t="s">
+        <v>80</v>
+      </c>
+      <c r="C63" s="103" t="s">
         <v>81</v>
-      </c>
-      <c r="C63" s="103" t="s">
-        <v>82</v>
       </c>
       <c r="D63" s="103"/>
       <c r="E63" s="104"/>
@@ -3467,30 +3564,30 @@
     </row>
     <row r="64" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B64" s="33" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="65" spans="2:3" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B65" s="33" t="s">
+        <v>83</v>
+      </c>
+      <c r="C65" s="33" t="s">
         <v>84</v>
-      </c>
-      <c r="C65" s="33" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="66" spans="2:3" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C66" s="33" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="67" spans="2:3" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C67" s="33" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="68" spans="2:3" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C68" s="33" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="69" spans="2:3" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3504,7 +3601,7 @@
     <row r="77" spans="2:3" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="78" spans="2:3" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C78" s="33" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="79" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
feat: support multy field user (orang)
</commit_message>
<xml_diff>
--- a/src/assets/sppd.xlsx
+++ b/src/assets/sppd.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0455A82-8B2F-4573-8A2A-D843313B71E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30D78E03-2762-4087-98A2-9266C1F756B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2760" yWindow="2955" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="4" r:id="rId1"/>
@@ -19,19 +19,11 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">surat_tugas!$A$1:$H$46</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="98">
   <si>
     <t>SURAT TUGAS</t>
   </si>
@@ -1046,7 +1038,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="167">
+  <cellXfs count="164">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1155,9 +1147,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1298,7 +1287,7 @@
     <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1309,10 +1298,6 @@
     </xf>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="2" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1322,8 +1307,26 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1394,47 +1397,29 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="24" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2024,7 +2009,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2056,7 +2041,7 @@
       <c r="A5" t="s">
         <v>94</v>
       </c>
-      <c r="B5" s="116"/>
+      <c r="B5" s="113"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -2086,8 +2071,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H52"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2116,28 +2101,28 @@
     <row r="2" spans="1:8" s="6" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="C2" s="7"/>
-      <c r="D2" s="119"/>
-      <c r="E2" s="119"/>
-      <c r="F2" s="119"/>
-      <c r="G2" s="119"/>
+      <c r="D2" s="122"/>
+      <c r="E2" s="122"/>
+      <c r="F2" s="122"/>
+      <c r="G2" s="122"/>
       <c r="H2" s="5"/>
     </row>
     <row r="3" spans="1:8" s="6" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="C3" s="7"/>
-      <c r="D3" s="120"/>
-      <c r="E3" s="120"/>
-      <c r="F3" s="120"/>
-      <c r="G3" s="120"/>
+      <c r="D3" s="123"/>
+      <c r="E3" s="123"/>
+      <c r="F3" s="123"/>
+      <c r="G3" s="123"/>
       <c r="H3" s="8"/>
     </row>
     <row r="4" spans="1:8" s="6" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="C4" s="7"/>
-      <c r="D4" s="121"/>
-      <c r="E4" s="121"/>
-      <c r="F4" s="121"/>
-      <c r="G4" s="121"/>
+      <c r="D4" s="124"/>
+      <c r="E4" s="124"/>
+      <c r="F4" s="124"/>
+      <c r="G4" s="124"/>
       <c r="H4" s="8"/>
     </row>
     <row r="5" spans="1:8" s="9" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2151,26 +2136,26 @@
     </row>
     <row r="6" spans="1:8" s="14" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
-      <c r="B6" s="122" t="s">
+      <c r="B6" s="125" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="122"/>
-      <c r="D6" s="122"/>
-      <c r="E6" s="122"/>
-      <c r="F6" s="122"/>
-      <c r="G6" s="122"/>
+      <c r="C6" s="125"/>
+      <c r="D6" s="125"/>
+      <c r="E6" s="125"/>
+      <c r="F6" s="125"/>
+      <c r="G6" s="125"/>
     </row>
     <row r="7" spans="1:8" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
-      <c r="B7" s="123" t="str">
+      <c r="B7" s="126" t="str">
         <f>data!B8</f>
         <v>Nomor : 449.1/        /UKM/2023</v>
       </c>
-      <c r="C7" s="123"/>
-      <c r="D7" s="123"/>
-      <c r="E7" s="123"/>
-      <c r="F7" s="123"/>
-      <c r="G7" s="123"/>
+      <c r="C7" s="126"/>
+      <c r="D7" s="126"/>
+      <c r="E7" s="126"/>
+      <c r="F7" s="126"/>
+      <c r="G7" s="126"/>
     </row>
     <row r="8" spans="1:8" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
@@ -2183,34 +2168,34 @@
     </row>
     <row r="9" spans="1:8" s="14" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
-      <c r="B9" s="124" t="s">
+      <c r="B9" s="127" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="124"/>
-      <c r="D9" s="124"/>
-      <c r="E9" s="124"/>
-      <c r="F9" s="124"/>
-      <c r="G9" s="124"/>
+      <c r="C9" s="127"/>
+      <c r="D9" s="127"/>
+      <c r="E9" s="127"/>
+      <c r="F9" s="127"/>
+      <c r="G9" s="127"/>
     </row>
     <row r="10" spans="1:8" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
-      <c r="B10" s="125"/>
-      <c r="C10" s="125"/>
-      <c r="D10" s="125"/>
-      <c r="E10" s="125"/>
-      <c r="F10" s="125"/>
-      <c r="G10" s="125"/>
+      <c r="B10" s="128"/>
+      <c r="C10" s="128"/>
+      <c r="D10" s="128"/>
+      <c r="E10" s="128"/>
+      <c r="F10" s="128"/>
+      <c r="G10" s="128"/>
     </row>
     <row r="11" spans="1:8" s="17" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="16"/>
-      <c r="B11" s="118" t="s">
+      <c r="B11" s="121" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="118"/>
-      <c r="D11" s="118"/>
-      <c r="E11" s="118"/>
-      <c r="F11" s="118"/>
-      <c r="G11" s="118"/>
+      <c r="C11" s="121"/>
+      <c r="D11" s="121"/>
+      <c r="E11" s="121"/>
+      <c r="F11" s="121"/>
+      <c r="G11" s="121"/>
     </row>
     <row r="12" spans="1:8" s="17" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="16"/>
@@ -2218,8 +2203,8 @@
       <c r="C12" s="16"/>
       <c r="D12" s="19"/>
       <c r="E12" s="20"/>
-      <c r="F12" s="118"/>
-      <c r="G12" s="118"/>
+      <c r="F12" s="121"/>
+      <c r="G12" s="121"/>
     </row>
     <row r="13" spans="1:8" s="17" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="16"/>
@@ -2232,12 +2217,12 @@
       <c r="D13" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="E13" s="107">
+      <c r="E13" s="106">
         <f>data!B1</f>
         <v>0</v>
       </c>
-      <c r="F13" s="118"/>
-      <c r="G13" s="118"/>
+      <c r="F13" s="121"/>
+      <c r="G13" s="121"/>
     </row>
     <row r="14" spans="1:8" s="17" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16"/>
@@ -2248,12 +2233,12 @@
       <c r="D14" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="E14" s="107">
+      <c r="E14" s="106">
         <f>data!B2</f>
         <v>0</v>
       </c>
-      <c r="F14" s="118"/>
-      <c r="G14" s="118"/>
+      <c r="F14" s="121"/>
+      <c r="G14" s="121"/>
     </row>
     <row r="15" spans="1:8" s="17" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="16"/>
@@ -2264,7 +2249,7 @@
       <c r="D15" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="E15" s="107">
+      <c r="E15" s="106">
         <f>data!B3</f>
         <v>0</v>
       </c>
@@ -2282,7 +2267,7 @@
       <c r="D16" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="E16" s="107">
+      <c r="E16" s="106">
         <f>data!B4</f>
         <v>0</v>
       </c>
@@ -2300,11 +2285,14 @@
       <c r="D17" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="E17" s="20"/>
-      <c r="F17" s="118" t="s">
+      <c r="E17" s="106">
+        <f>data!C1</f>
+        <v>0</v>
+      </c>
+      <c r="F17" s="121" t="s">
         <v>10</v>
       </c>
-      <c r="G17" s="118"/>
+      <c r="G17" s="121"/>
     </row>
     <row r="18" spans="1:7" s="17" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="16"/>
@@ -2315,9 +2303,12 @@
       <c r="D18" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="E18" s="20"/>
-      <c r="F18" s="118"/>
-      <c r="G18" s="118"/>
+      <c r="E18" s="106">
+        <f>data!C2</f>
+        <v>0</v>
+      </c>
+      <c r="F18" s="121"/>
+      <c r="G18" s="121"/>
     </row>
     <row r="19" spans="1:7" s="17" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="16"/>
@@ -2328,7 +2319,10 @@
       <c r="D19" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="E19" s="20"/>
+      <c r="E19" s="106">
+        <f>data!C3</f>
+        <v>0</v>
+      </c>
       <c r="F19" s="19" t="s">
         <v>11</v>
       </c>
@@ -2343,7 +2337,10 @@
       <c r="D20" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="E20" s="4"/>
+      <c r="E20" s="106">
+        <f>data!C4</f>
+        <v>0</v>
+      </c>
       <c r="F20" s="3"/>
       <c r="G20" s="4"/>
     </row>
@@ -2389,12 +2386,12 @@
       <c r="D24" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="E24" s="117">
+      <c r="E24" s="114">
         <f>data!B6</f>
         <v>0</v>
       </c>
       <c r="F24" s="20"/>
-      <c r="G24" s="109"/>
+      <c r="G24" s="108"/>
     </row>
     <row r="25" spans="1:7" s="14" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
@@ -2405,7 +2402,7 @@
       <c r="D25" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="E25" s="117">
+      <c r="E25" s="114">
         <f>data!B7</f>
         <v>0</v>
       </c>
@@ -2441,10 +2438,10 @@
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
       <c r="E28" s="27"/>
-      <c r="F28" s="123" t="s">
+      <c r="F28" s="126" t="s">
         <v>17</v>
       </c>
-      <c r="G28" s="123"/>
+      <c r="G28" s="126"/>
     </row>
     <row r="29" spans="1:7" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
@@ -2452,10 +2449,10 @@
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
       <c r="E29" s="27"/>
-      <c r="F29" s="123" t="s">
+      <c r="F29" s="126" t="s">
         <v>18</v>
       </c>
-      <c r="G29" s="123"/>
+      <c r="G29" s="126"/>
     </row>
     <row r="30" spans="1:7" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
@@ -2488,10 +2485,10 @@
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
       <c r="E33" s="27"/>
-      <c r="F33" s="127" t="s">
+      <c r="F33" s="130" t="s">
         <v>19</v>
       </c>
-      <c r="G33" s="127"/>
+      <c r="G33" s="130"/>
       <c r="H33" s="31"/>
     </row>
     <row r="34" spans="1:8" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -2500,10 +2497,10 @@
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
       <c r="E34" s="27"/>
-      <c r="F34" s="126" t="s">
+      <c r="F34" s="129" t="s">
         <v>20</v>
       </c>
-      <c r="G34" s="126"/>
+      <c r="G34" s="129"/>
       <c r="H34" s="32"/>
     </row>
     <row r="35" spans="1:8" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -2533,7 +2530,7 @@
       <c r="D37" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="E37" s="111">
+      <c r="E37" s="3">
         <f>E13</f>
         <v>0</v>
       </c>
@@ -2548,7 +2545,7 @@
       <c r="D38" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="E38" s="112">
+      <c r="E38" s="14">
         <f>E14</f>
         <v>0</v>
       </c>
@@ -2558,15 +2555,35 @@
       <c r="G38" s="4"/>
     </row>
     <row r="39" spans="1:8" s="14" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C39" s="16"/>
-      <c r="D39" s="21"/>
-      <c r="E39" s="27"/>
       <c r="G39" s="27"/>
     </row>
     <row r="40" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C40" s="16"/>
-      <c r="D40" s="21"/>
+      <c r="C40" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="D40" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="E40" s="14">
+        <f>E17</f>
+        <v>0</v>
+      </c>
       <c r="F40" s="14"/>
+    </row>
+    <row r="41" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C41" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D41" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="E41" s="14">
+        <f>E18</f>
+        <v>0</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="42" spans="1:8" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
@@ -2630,8 +2647,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K39"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="90" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:E8"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A22" zoomScale="90" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2685,23 +2702,23 @@
       <c r="B6" s="3"/>
     </row>
     <row r="7" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="146" t="s">
+      <c r="A7" s="147" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="146"/>
-      <c r="C7" s="146"/>
-      <c r="D7" s="146"/>
-      <c r="E7" s="146"/>
+      <c r="B7" s="147"/>
+      <c r="C7" s="147"/>
+      <c r="D7" s="147"/>
+      <c r="E7" s="147"/>
       <c r="I7" s="39"/>
     </row>
     <row r="8" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="123" t="s">
+      <c r="A8" s="126" t="s">
         <v>88</v>
       </c>
-      <c r="B8" s="123"/>
-      <c r="C8" s="123"/>
-      <c r="D8" s="123"/>
-      <c r="E8" s="123"/>
+      <c r="B8" s="126"/>
+      <c r="C8" s="126"/>
+      <c r="D8" s="126"/>
+      <c r="E8" s="126"/>
       <c r="I8" s="39"/>
     </row>
     <row r="9" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -2718,10 +2735,10 @@
       <c r="C10" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="147" t="s">
+      <c r="D10" s="148" t="s">
         <v>31</v>
       </c>
-      <c r="E10" s="148"/>
+      <c r="E10" s="149"/>
     </row>
     <row r="11" spans="1:11" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="43">
@@ -2739,36 +2756,42 @@
     <row r="12" spans="1:11" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="43"/>
       <c r="C12" s="44"/>
-      <c r="D12" s="149"/>
-      <c r="E12" s="150"/>
+      <c r="D12" s="120">
+        <f>data!C1</f>
+        <v>0</v>
+      </c>
+      <c r="E12" s="115"/>
       <c r="H12" s="39"/>
       <c r="K12" s="39"/>
     </row>
     <row r="13" spans="1:11" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="134">
+      <c r="B13" s="137">
         <v>3</v>
       </c>
       <c r="C13" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="151" t="str">
-        <f>data!A3</f>
-        <v>golongan</v>
-      </c>
-      <c r="E13" s="152"/>
+      <c r="D13" s="116">
+        <f>data!B3</f>
+        <v>0</v>
+      </c>
+      <c r="E13" s="117"/>
       <c r="H13" s="39"/>
       <c r="K13" s="39"/>
     </row>
     <row r="14" spans="1:11" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="134"/>
+      <c r="B14" s="137"/>
       <c r="C14" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="153"/>
-      <c r="E14" s="154"/>
+      <c r="D14" s="118">
+        <f>data!C3</f>
+        <v>0</v>
+      </c>
+      <c r="E14" s="119"/>
     </row>
     <row r="15" spans="1:11" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="134"/>
+      <c r="B15" s="137"/>
       <c r="C15" s="44" t="s">
         <v>35</v>
       </c>
@@ -2779,12 +2802,15 @@
       <c r="E15" s="49"/>
     </row>
     <row r="16" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="145"/>
+      <c r="B16" s="146"/>
       <c r="C16" s="44" t="s">
         <v>36</v>
       </c>
-      <c r="D16" s="50"/>
-      <c r="E16" s="51"/>
+      <c r="D16" s="48">
+        <f>data!C4</f>
+        <v>0</v>
+      </c>
+      <c r="E16" s="50"/>
       <c r="H16" s="39"/>
     </row>
     <row r="17" spans="2:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2794,204 +2820,201 @@
       <c r="C17" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="D17" s="102">
+      <c r="D17" s="101">
         <f>data!B6</f>
         <v>0</v>
       </c>
-      <c r="E17" s="108"/>
+      <c r="E17" s="107"/>
       <c r="H17" s="39"/>
     </row>
     <row r="18" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="41">
         <v>5</v>
       </c>
-      <c r="C18" s="52" t="s">
+      <c r="C18" s="51" t="s">
         <v>38</v>
       </c>
-      <c r="D18" s="141" t="s">
+      <c r="D18" s="150" t="s">
         <v>39</v>
       </c>
-      <c r="E18" s="142"/>
+      <c r="E18" s="151"/>
       <c r="H18" s="39"/>
     </row>
     <row r="19" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="134">
+      <c r="B19" s="137">
         <v>6</v>
       </c>
       <c r="C19" s="47" t="s">
         <v>40</v>
       </c>
-      <c r="D19" s="131" t="s">
+      <c r="D19" s="134" t="s">
         <v>41</v>
       </c>
-      <c r="E19" s="132"/>
+      <c r="E19" s="135"/>
     </row>
     <row r="20" spans="2:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="134"/>
-      <c r="C20" s="53" t="s">
+      <c r="B20" s="137"/>
+      <c r="C20" s="52" t="s">
         <v>42</v>
       </c>
-      <c r="D20" s="143">
+      <c r="D20" s="144">
         <f>data!B7</f>
         <v>0</v>
       </c>
-      <c r="E20" s="144"/>
+      <c r="E20" s="145"/>
     </row>
     <row r="21" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="134">
+      <c r="B21" s="137">
         <v>7</v>
       </c>
       <c r="C21" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="D21" s="131" t="s">
+      <c r="D21" s="134" t="s">
         <v>44</v>
       </c>
-      <c r="E21" s="132"/>
+      <c r="E21" s="135"/>
     </row>
     <row r="22" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="134"/>
+      <c r="B22" s="137"/>
       <c r="C22" s="44" t="s">
         <v>45</v>
       </c>
-      <c r="D22" s="54"/>
-      <c r="E22" s="106"/>
+      <c r="D22" s="53"/>
+      <c r="E22" s="105"/>
     </row>
     <row r="23" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="145"/>
+      <c r="B23" s="146"/>
       <c r="C23" s="44" t="s">
         <v>46</v>
       </c>
-      <c r="D23" s="54">
+      <c r="D23" s="53">
         <f>D22</f>
         <v>0</v>
       </c>
-      <c r="E23" s="110"/>
+      <c r="E23" s="109"/>
     </row>
     <row r="24" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="129">
+      <c r="B24" s="132">
         <v>8</v>
       </c>
-      <c r="C24" s="56" t="s">
+      <c r="C24" s="55" t="s">
         <v>47</v>
       </c>
-      <c r="D24" s="131" t="s">
+      <c r="D24" s="134" t="s">
         <v>6</v>
       </c>
-      <c r="E24" s="132"/>
+      <c r="E24" s="135"/>
     </row>
     <row r="25" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="130"/>
+      <c r="B25" s="133"/>
       <c r="C25" s="48"/>
-      <c r="D25" s="57"/>
+      <c r="D25" s="56"/>
       <c r="E25" s="49"/>
     </row>
     <row r="26" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="58"/>
-      <c r="C26" s="59" t="s">
+      <c r="B26" s="57"/>
+      <c r="C26" s="58" t="s">
         <v>48</v>
       </c>
-      <c r="D26" s="60" t="s">
+      <c r="D26" s="59" t="s">
         <v>49</v>
       </c>
       <c r="E26" s="49"/>
     </row>
     <row r="27" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="133">
+      <c r="B27" s="136">
         <v>9</v>
       </c>
-      <c r="C27" s="61" t="s">
+      <c r="C27" s="60" t="s">
         <v>50</v>
       </c>
-      <c r="D27" s="135" t="s">
+      <c r="D27" s="138" t="s">
         <v>51</v>
       </c>
-      <c r="E27" s="136"/>
+      <c r="E27" s="139"/>
     </row>
     <row r="28" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="134"/>
-      <c r="C28" s="61" t="s">
+      <c r="B28" s="137"/>
+      <c r="C28" s="60" t="s">
         <v>52</v>
       </c>
-      <c r="D28" s="137" t="s">
+      <c r="D28" s="140" t="s">
         <v>53</v>
       </c>
-      <c r="E28" s="138"/>
+      <c r="E28" s="141"/>
     </row>
     <row r="29" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="134"/>
-      <c r="C29" s="62" t="s">
+      <c r="B29" s="137"/>
+      <c r="C29" s="61" t="s">
         <v>54</v>
       </c>
-      <c r="D29" s="139" t="s">
+      <c r="D29" s="142" t="s">
         <v>55</v>
       </c>
-      <c r="E29" s="140"/>
+      <c r="E29" s="143"/>
     </row>
     <row r="30" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="63">
+      <c r="B30" s="62">
         <v>10</v>
       </c>
-      <c r="C30" s="64" t="s">
+      <c r="C30" s="63" t="s">
         <v>56</v>
       </c>
       <c r="D30" s="42"/>
-      <c r="E30" s="65"/>
+      <c r="E30" s="64"/>
     </row>
     <row r="31" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="32" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D32" s="66" t="s">
+      <c r="D32" s="65" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="33" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D33" s="67" t="s">
+      <c r="D33" s="66" t="s">
         <v>58</v>
       </c>
-      <c r="E33" s="55">
+      <c r="E33" s="54">
         <f>D22</f>
         <v>0</v>
       </c>
-      <c r="F33" s="106"/>
+      <c r="F33" s="105"/>
     </row>
     <row r="34" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="33"/>
       <c r="C34" s="33"/>
-      <c r="D34" s="128" t="s">
+      <c r="D34" s="131" t="s">
         <v>31</v>
       </c>
-      <c r="E34" s="128"/>
+      <c r="E34" s="131"/>
     </row>
     <row r="35" spans="2:6" s="33" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D35" s="68"/>
+      <c r="D35" s="67"/>
     </row>
     <row r="36" spans="2:6" s="33" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D36" s="68"/>
+      <c r="D36" s="67"/>
     </row>
     <row r="37" spans="2:6" s="33" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D37" s="68"/>
+      <c r="D37" s="67"/>
     </row>
     <row r="38" spans="2:6" s="33" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D38" s="127" t="s">
+      <c r="D38" s="130" t="s">
         <v>19</v>
       </c>
-      <c r="E38" s="127"/>
+      <c r="E38" s="130"/>
     </row>
     <row r="39" spans="2:6" s="33" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D39" s="126" t="s">
+      <c r="D39" s="129" t="s">
         <v>20</v>
       </c>
-      <c r="E39" s="126"/>
+      <c r="E39" s="129"/>
     </row>
   </sheetData>
-  <mergeCells count="22">
+  <mergeCells count="19">
     <mergeCell ref="A7:E7"/>
     <mergeCell ref="A8:E8"/>
     <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D12:E12"/>
     <mergeCell ref="B13:B16"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D14:E14"/>
     <mergeCell ref="D18:E18"/>
     <mergeCell ref="B19:B20"/>
     <mergeCell ref="D19:E19"/>
@@ -3019,7 +3042,7 @@
   <dimension ref="B1:G82"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScale="86" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="C7" sqref="C7:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3051,67 +3074,67 @@
       </c>
     </row>
     <row r="6" spans="2:7" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E6" s="66" t="s">
+      <c r="E6" s="65" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="7" spans="2:7" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E7" s="66" t="s">
+      <c r="E7" s="65" t="s">
         <v>89</v>
       </c>
-      <c r="F7" s="69"/>
+      <c r="F7" s="68"/>
     </row>
     <row r="8" spans="2:7" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="70"/>
-      <c r="D8" s="70"/>
-      <c r="E8" s="66" t="s">
+      <c r="C8" s="69"/>
+      <c r="D8" s="69"/>
+      <c r="E8" s="65" t="s">
         <v>61</v>
       </c>
-      <c r="F8" s="163">
+      <c r="F8" s="160">
         <f>data!B7</f>
         <v>0</v>
       </c>
-      <c r="G8" s="163"/>
+      <c r="G8" s="160"/>
     </row>
     <row r="9" spans="2:7" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E9" s="71"/>
+      <c r="E9" s="70"/>
     </row>
     <row r="10" spans="2:7" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E10" s="68"/>
+      <c r="E10" s="67"/>
     </row>
     <row r="11" spans="2:7" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="72" t="s">
+      <c r="B11" s="71" t="s">
         <v>62</v>
       </c>
-      <c r="C11" s="73" t="s">
+      <c r="C11" s="72" t="s">
         <v>63</v>
       </c>
-      <c r="D11" s="73"/>
-      <c r="E11" s="74" t="s">
+      <c r="D11" s="72"/>
+      <c r="E11" s="73" t="s">
         <v>64</v>
       </c>
-      <c r="F11" s="75"/>
+      <c r="F11" s="74"/>
     </row>
     <row r="12" spans="2:7" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="76"/>
-      <c r="C12" s="164">
+      <c r="B12" s="75"/>
+      <c r="C12" s="161">
         <f>F8</f>
         <v>0</v>
       </c>
-      <c r="D12" s="164"/>
-      <c r="E12" s="165">
+      <c r="D12" s="161"/>
+      <c r="E12" s="162">
         <f>C12</f>
         <v>0</v>
       </c>
-      <c r="F12" s="166"/>
+      <c r="F12" s="163"/>
     </row>
     <row r="13" spans="2:7" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="76"/>
-      <c r="C13" s="66" t="str">
+      <c r="B13" s="75"/>
+      <c r="C13" s="65" t="str">
         <f>E7</f>
         <v>Pada Tanggal</v>
       </c>
-      <c r="D13" s="69">
+      <c r="D13" s="68">
         <f>F7</f>
         <v>0</v>
       </c>
@@ -3119,448 +3142,448 @@
         <f>E7</f>
         <v>Pada Tanggal</v>
       </c>
-      <c r="F13" s="77">
+      <c r="F13" s="76">
         <f>D13</f>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="2:7" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="76"/>
-      <c r="C14" s="66"/>
-      <c r="D14" s="66"/>
+      <c r="B14" s="75"/>
+      <c r="C14" s="65"/>
+      <c r="D14" s="65"/>
       <c r="E14" s="48" t="s">
         <v>65</v>
       </c>
-      <c r="F14" s="78"/>
+      <c r="F14" s="77"/>
     </row>
     <row r="15" spans="2:7" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="76"/>
-      <c r="C15" s="128" t="s">
+      <c r="B15" s="75"/>
+      <c r="C15" s="131" t="s">
         <v>66</v>
       </c>
-      <c r="D15" s="128"/>
-      <c r="E15" s="161" t="s">
+      <c r="D15" s="131"/>
+      <c r="E15" s="158" t="s">
         <v>66</v>
       </c>
-      <c r="F15" s="160"/>
+      <c r="F15" s="157"/>
     </row>
     <row r="16" spans="2:7" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="76"/>
+      <c r="B16" s="75"/>
       <c r="E16" s="48"/>
-      <c r="F16" s="79"/>
+      <c r="F16" s="78"/>
     </row>
     <row r="17" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="76"/>
+      <c r="B17" s="75"/>
       <c r="D17" s="33" t="s">
         <v>11</v>
       </c>
       <c r="E17" s="48"/>
-      <c r="F17" s="79"/>
+      <c r="F17" s="78"/>
     </row>
     <row r="18" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="76"/>
+      <c r="B18" s="75"/>
       <c r="E18" s="48"/>
-      <c r="F18" s="79"/>
+      <c r="F18" s="78"/>
     </row>
     <row r="19" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="76"/>
-      <c r="C19" s="155" t="s">
+      <c r="B19" s="75"/>
+      <c r="C19" s="152" t="s">
         <v>67</v>
       </c>
-      <c r="D19" s="155"/>
-      <c r="E19" s="162" t="s">
+      <c r="D19" s="152"/>
+      <c r="E19" s="159" t="s">
         <v>67</v>
       </c>
-      <c r="F19" s="159"/>
+      <c r="F19" s="156"/>
     </row>
     <row r="20" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="80"/>
-      <c r="C20" s="81" t="s">
+      <c r="B20" s="79"/>
+      <c r="C20" s="80" t="s">
         <v>68</v>
       </c>
-      <c r="D20" s="82"/>
-      <c r="E20" s="83" t="s">
+      <c r="D20" s="81"/>
+      <c r="E20" s="82" t="s">
         <v>68</v>
       </c>
-      <c r="F20" s="84"/>
+      <c r="F20" s="83"/>
     </row>
     <row r="21" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="72" t="s">
+      <c r="B21" s="71" t="s">
         <v>69</v>
       </c>
-      <c r="C21" s="73"/>
-      <c r="D21" s="75"/>
-      <c r="E21" s="74" t="s">
+      <c r="C21" s="72"/>
+      <c r="D21" s="74"/>
+      <c r="E21" s="73" t="s">
         <v>64</v>
       </c>
-      <c r="F21" s="75"/>
+      <c r="F21" s="74"/>
     </row>
     <row r="22" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="76"/>
-      <c r="C22" s="66" t="s">
+      <c r="B22" s="75"/>
+      <c r="C22" s="65" t="s">
         <v>70</v>
       </c>
-      <c r="D22" s="85">
+      <c r="D22" s="84">
         <f>C12</f>
         <v>0</v>
       </c>
-      <c r="E22" s="115" t="s">
+      <c r="E22" s="112" t="s">
         <v>70</v>
       </c>
-      <c r="F22" s="86"/>
+      <c r="F22" s="85"/>
     </row>
     <row r="23" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="76"/>
-      <c r="C23" s="66" t="s">
+      <c r="B23" s="75"/>
+      <c r="C23" s="65" t="s">
         <v>71</v>
       </c>
-      <c r="D23" s="87"/>
+      <c r="D23" s="86"/>
       <c r="E23" s="48" t="s">
         <v>71</v>
       </c>
-      <c r="F23" s="87"/>
+      <c r="F23" s="86"/>
     </row>
     <row r="24" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="76"/>
-      <c r="C24" s="66"/>
-      <c r="D24" s="78"/>
+      <c r="B24" s="75"/>
+      <c r="C24" s="65"/>
+      <c r="D24" s="77"/>
       <c r="E24" s="48" t="s">
         <v>72</v>
       </c>
-      <c r="F24" s="78"/>
+      <c r="F24" s="77"/>
     </row>
     <row r="25" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="76"/>
-      <c r="C25" s="128" t="s">
+      <c r="B25" s="75"/>
+      <c r="C25" s="131" t="s">
         <v>66</v>
       </c>
-      <c r="D25" s="160"/>
-      <c r="E25" s="161" t="s">
+      <c r="D25" s="157"/>
+      <c r="E25" s="158" t="s">
         <v>66</v>
       </c>
-      <c r="F25" s="160"/>
+      <c r="F25" s="157"/>
     </row>
     <row r="26" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="76"/>
-      <c r="D26" s="79"/>
+      <c r="B26" s="75"/>
+      <c r="D26" s="78"/>
       <c r="E26" s="48"/>
-      <c r="F26" s="79"/>
+      <c r="F26" s="78"/>
     </row>
     <row r="27" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="76"/>
-      <c r="D27" s="79"/>
+      <c r="B27" s="75"/>
+      <c r="D27" s="78"/>
       <c r="E27" s="48"/>
-      <c r="F27" s="79"/>
+      <c r="F27" s="78"/>
     </row>
     <row r="28" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="76"/>
-      <c r="D28" s="79"/>
+      <c r="B28" s="75"/>
+      <c r="D28" s="78"/>
       <c r="E28" s="48"/>
-      <c r="F28" s="79"/>
+      <c r="F28" s="78"/>
     </row>
     <row r="29" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="76"/>
-      <c r="C29" s="155" t="s">
+      <c r="B29" s="75"/>
+      <c r="C29" s="152" t="s">
         <v>67</v>
       </c>
-      <c r="D29" s="159"/>
-      <c r="E29" s="155" t="s">
+      <c r="D29" s="156"/>
+      <c r="E29" s="152" t="s">
         <v>67</v>
       </c>
-      <c r="F29" s="159"/>
+      <c r="F29" s="156"/>
     </row>
     <row r="30" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="80"/>
-      <c r="C30" s="81" t="s">
+      <c r="B30" s="79"/>
+      <c r="C30" s="80" t="s">
         <v>68</v>
       </c>
-      <c r="D30" s="84"/>
-      <c r="E30" s="83" t="s">
+      <c r="D30" s="83"/>
+      <c r="E30" s="82" t="s">
         <v>68</v>
       </c>
-      <c r="F30" s="84"/>
+      <c r="F30" s="83"/>
     </row>
     <row r="31" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="72" t="s">
+      <c r="B31" s="71" t="s">
         <v>73</v>
       </c>
-      <c r="C31" s="73"/>
-      <c r="D31" s="75"/>
-      <c r="E31" s="74" t="s">
+      <c r="C31" s="72"/>
+      <c r="D31" s="74"/>
+      <c r="E31" s="73" t="s">
         <v>64</v>
       </c>
-      <c r="F31" s="75"/>
+      <c r="F31" s="74"/>
     </row>
     <row r="32" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="76"/>
-      <c r="C32" s="66" t="s">
+      <c r="B32" s="75"/>
+      <c r="C32" s="65" t="s">
         <v>74</v>
       </c>
-      <c r="D32" s="89"/>
-      <c r="E32" s="114" t="s">
+      <c r="D32" s="88"/>
+      <c r="E32" s="111" t="s">
         <v>74</v>
       </c>
-      <c r="F32" s="90"/>
+      <c r="F32" s="89"/>
     </row>
     <row r="33" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="76"/>
-      <c r="C33" s="66" t="s">
+      <c r="B33" s="75"/>
+      <c r="C33" s="65" t="s">
         <v>71</v>
       </c>
-      <c r="D33" s="91"/>
-      <c r="E33" s="113" t="s">
+      <c r="D33" s="90"/>
+      <c r="E33" s="110" t="s">
         <v>71</v>
       </c>
-      <c r="F33" s="91"/>
+      <c r="F33" s="90"/>
     </row>
     <row r="34" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="76"/>
-      <c r="C34" s="66"/>
+      <c r="B34" s="75"/>
+      <c r="C34" s="65"/>
       <c r="E34" s="48" t="s">
         <v>72</v>
       </c>
-      <c r="F34" s="92"/>
+      <c r="F34" s="91"/>
     </row>
     <row r="35" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="76"/>
-      <c r="C35" s="128" t="s">
+      <c r="B35" s="75"/>
+      <c r="C35" s="131" t="s">
         <v>66</v>
       </c>
-      <c r="D35" s="160"/>
-      <c r="E35" s="161" t="s">
+      <c r="D35" s="157"/>
+      <c r="E35" s="158" t="s">
         <v>66</v>
       </c>
-      <c r="F35" s="160"/>
+      <c r="F35" s="157"/>
     </row>
     <row r="36" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="76"/>
-      <c r="D36" s="79"/>
+      <c r="B36" s="75"/>
+      <c r="D36" s="78"/>
       <c r="E36" s="48"/>
-      <c r="F36" s="79"/>
+      <c r="F36" s="78"/>
     </row>
     <row r="37" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="76"/>
-      <c r="D37" s="79"/>
+      <c r="B37" s="75"/>
+      <c r="D37" s="78"/>
       <c r="E37" s="48"/>
-      <c r="F37" s="79"/>
+      <c r="F37" s="78"/>
     </row>
     <row r="38" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="76"/>
-      <c r="D38" s="79"/>
+      <c r="B38" s="75"/>
+      <c r="D38" s="78"/>
       <c r="E38" s="48"/>
-      <c r="F38" s="79"/>
+      <c r="F38" s="78"/>
     </row>
     <row r="39" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="76"/>
-      <c r="C39" s="155" t="s">
+      <c r="B39" s="75"/>
+      <c r="C39" s="152" t="s">
         <v>67</v>
       </c>
-      <c r="D39" s="159"/>
-      <c r="E39" s="155" t="s">
+      <c r="D39" s="156"/>
+      <c r="E39" s="152" t="s">
         <v>67</v>
       </c>
-      <c r="F39" s="159"/>
+      <c r="F39" s="156"/>
     </row>
     <row r="40" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="80"/>
-      <c r="C40" s="81" t="s">
+      <c r="B40" s="79"/>
+      <c r="C40" s="80" t="s">
         <v>68</v>
       </c>
-      <c r="D40" s="84"/>
-      <c r="E40" s="83" t="s">
+      <c r="D40" s="83"/>
+      <c r="E40" s="82" t="s">
         <v>68</v>
       </c>
-      <c r="F40" s="84"/>
+      <c r="F40" s="83"/>
     </row>
     <row r="41" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="72" t="s">
+      <c r="B41" s="71" t="s">
         <v>75</v>
       </c>
-      <c r="C41" s="73"/>
-      <c r="D41" s="75"/>
-      <c r="E41" s="74" t="s">
+      <c r="C41" s="72"/>
+      <c r="D41" s="74"/>
+      <c r="E41" s="73" t="s">
         <v>64</v>
       </c>
-      <c r="F41" s="75"/>
+      <c r="F41" s="74"/>
     </row>
     <row r="42" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="76"/>
-      <c r="C42" s="66" t="s">
+      <c r="B42" s="75"/>
+      <c r="C42" s="65" t="s">
         <v>74</v>
       </c>
-      <c r="D42" s="93"/>
-      <c r="E42" s="94"/>
-      <c r="F42" s="95"/>
+      <c r="D42" s="92"/>
+      <c r="E42" s="93"/>
+      <c r="F42" s="94"/>
     </row>
     <row r="43" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="76"/>
-      <c r="C43" s="66" t="s">
+      <c r="B43" s="75"/>
+      <c r="C43" s="65" t="s">
         <v>71</v>
       </c>
-      <c r="D43" s="87"/>
-      <c r="E43" s="88"/>
-      <c r="F43" s="87"/>
+      <c r="D43" s="86"/>
+      <c r="E43" s="87"/>
+      <c r="F43" s="86"/>
     </row>
     <row r="44" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="76"/>
-      <c r="C44" s="66"/>
+      <c r="B44" s="75"/>
+      <c r="C44" s="65"/>
       <c r="E44" s="48" t="s">
         <v>72</v>
       </c>
-      <c r="F44" s="92"/>
+      <c r="F44" s="91"/>
     </row>
     <row r="45" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="76"/>
-      <c r="C45" s="128" t="s">
+      <c r="B45" s="75"/>
+      <c r="C45" s="131" t="s">
         <v>66</v>
       </c>
-      <c r="D45" s="160"/>
-      <c r="E45" s="161" t="s">
+      <c r="D45" s="157"/>
+      <c r="E45" s="158" t="s">
         <v>66</v>
       </c>
-      <c r="F45" s="160"/>
+      <c r="F45" s="157"/>
     </row>
     <row r="46" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="76"/>
-      <c r="D46" s="79"/>
+      <c r="B46" s="75"/>
+      <c r="D46" s="78"/>
       <c r="E46" s="48"/>
-      <c r="F46" s="79"/>
+      <c r="F46" s="78"/>
     </row>
     <row r="47" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="76"/>
-      <c r="D47" s="79"/>
+      <c r="B47" s="75"/>
+      <c r="D47" s="78"/>
       <c r="E47" s="48"/>
-      <c r="F47" s="79"/>
+      <c r="F47" s="78"/>
     </row>
     <row r="48" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="76"/>
-      <c r="D48" s="79"/>
+      <c r="B48" s="75"/>
+      <c r="D48" s="78"/>
       <c r="E48" s="48"/>
-      <c r="F48" s="79"/>
+      <c r="F48" s="78"/>
     </row>
     <row r="49" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="76"/>
-      <c r="C49" s="155" t="s">
+      <c r="B49" s="75"/>
+      <c r="C49" s="152" t="s">
         <v>67</v>
       </c>
-      <c r="D49" s="159"/>
-      <c r="E49" s="162" t="s">
+      <c r="D49" s="156"/>
+      <c r="E49" s="159" t="s">
         <v>67</v>
       </c>
-      <c r="F49" s="159"/>
+      <c r="F49" s="156"/>
     </row>
     <row r="50" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="80"/>
-      <c r="C50" s="81" t="s">
+      <c r="B50" s="79"/>
+      <c r="C50" s="80" t="s">
         <v>68</v>
       </c>
-      <c r="D50" s="84"/>
-      <c r="E50" s="83" t="s">
+      <c r="D50" s="83"/>
+      <c r="E50" s="82" t="s">
         <v>68</v>
       </c>
-      <c r="F50" s="84"/>
+      <c r="F50" s="83"/>
     </row>
     <row r="51" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="76" t="s">
+      <c r="B51" s="75" t="s">
         <v>76</v>
       </c>
-      <c r="C51" s="96" t="s">
+      <c r="C51" s="95" t="s">
         <v>77</v>
       </c>
-      <c r="D51" s="96"/>
-      <c r="E51" s="96"/>
-      <c r="F51" s="97"/>
+      <c r="D51" s="95"/>
+      <c r="E51" s="95"/>
+      <c r="F51" s="96"/>
     </row>
     <row r="52" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="76"/>
+      <c r="B52" s="75"/>
       <c r="C52" s="33" t="s">
         <v>78</v>
       </c>
-      <c r="F52" s="79"/>
+      <c r="F52" s="78"/>
     </row>
     <row r="53" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="76"/>
+      <c r="B53" s="75"/>
       <c r="C53" s="33" t="s">
         <v>79</v>
       </c>
-      <c r="F53" s="98"/>
+      <c r="F53" s="97"/>
     </row>
     <row r="54" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="76"/>
-      <c r="C54" s="155"/>
-      <c r="D54" s="155"/>
-      <c r="E54" s="155"/>
-      <c r="F54" s="99"/>
+      <c r="B54" s="75"/>
+      <c r="C54" s="152"/>
+      <c r="D54" s="152"/>
+      <c r="E54" s="152"/>
+      <c r="F54" s="98"/>
     </row>
     <row r="55" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="76"/>
-      <c r="F55" s="79"/>
+      <c r="B55" s="75"/>
+      <c r="F55" s="78"/>
     </row>
     <row r="56" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="76"/>
-      <c r="C56" s="123" t="s">
+      <c r="B56" s="75"/>
+      <c r="C56" s="126" t="s">
         <v>31</v>
       </c>
-      <c r="D56" s="123"/>
-      <c r="E56" s="123"/>
-      <c r="F56" s="156"/>
+      <c r="D56" s="126"/>
+      <c r="E56" s="126"/>
+      <c r="F56" s="153"/>
     </row>
     <row r="57" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="76"/>
+      <c r="B57" s="75"/>
       <c r="C57" s="3"/>
       <c r="D57" s="3"/>
       <c r="E57" s="15"/>
-      <c r="F57" s="100"/>
+      <c r="F57" s="99"/>
     </row>
     <row r="58" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="76"/>
+      <c r="B58" s="75"/>
       <c r="C58" s="3"/>
       <c r="D58" s="3"/>
       <c r="E58" s="3"/>
-      <c r="F58" s="100"/>
+      <c r="F58" s="99"/>
     </row>
     <row r="59" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="76"/>
+      <c r="B59" s="75"/>
       <c r="C59" s="3"/>
       <c r="D59" s="3"/>
       <c r="E59" s="3"/>
-      <c r="F59" s="100"/>
+      <c r="F59" s="99"/>
     </row>
     <row r="60" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="76"/>
-      <c r="C60" s="157" t="s">
+      <c r="B60" s="75"/>
+      <c r="C60" s="154" t="s">
         <v>19</v>
       </c>
-      <c r="D60" s="157"/>
-      <c r="E60" s="157"/>
-      <c r="F60" s="158"/>
+      <c r="D60" s="154"/>
+      <c r="E60" s="154"/>
+      <c r="F60" s="155"/>
     </row>
     <row r="61" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="76"/>
-      <c r="C61" s="123" t="s">
+      <c r="B61" s="75"/>
+      <c r="C61" s="126" t="s">
         <v>20</v>
       </c>
-      <c r="D61" s="123"/>
-      <c r="E61" s="123"/>
-      <c r="F61" s="156"/>
+      <c r="D61" s="126"/>
+      <c r="E61" s="126"/>
+      <c r="F61" s="153"/>
     </row>
     <row r="62" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="80"/>
-      <c r="C62" s="81"/>
-      <c r="D62" s="81"/>
-      <c r="E62" s="81"/>
-      <c r="F62" s="101"/>
+      <c r="B62" s="79"/>
+      <c r="C62" s="80"/>
+      <c r="D62" s="80"/>
+      <c r="E62" s="80"/>
+      <c r="F62" s="100"/>
     </row>
     <row r="63" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="102" t="s">
+      <c r="B63" s="101" t="s">
         <v>80</v>
       </c>
-      <c r="C63" s="103" t="s">
+      <c r="C63" s="102" t="s">
         <v>81</v>
       </c>
-      <c r="D63" s="103"/>
-      <c r="E63" s="104"/>
-      <c r="F63" s="105"/>
+      <c r="D63" s="102"/>
+      <c r="E63" s="103"/>
+      <c r="F63" s="104"/>
     </row>
     <row r="64" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B64" s="33" t="s">

</xml_diff>

<commit_message>
fix: default cell fields
</commit_message>
<xml_diff>
--- a/src/assets/sppd.xlsx
+++ b/src/assets/sppd.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30D78E03-2762-4087-98A2-9266C1F756B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45E6B73C-46D6-4BDB-9F6C-CA1A54AAD893}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2760" yWindow="2955" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="4" r:id="rId1"/>
@@ -19,6 +19,14 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">surat_tugas!$A$1:$H$46</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -746,7 +754,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="26">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -1019,9 +1027,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -1031,6 +1037,19 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1038,7 +1057,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="164">
+  <cellXfs count="166">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1166,9 +1185,6 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1328,9 +1344,18 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1344,41 +1369,44 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="19" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1397,65 +1425,62 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="24" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="26" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="20" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="20" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -2008,8 +2033,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15277BD0-1E06-4977-8B5E-1D678D3D00DE}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2041,7 +2066,7 @@
       <c r="A5" t="s">
         <v>94</v>
       </c>
-      <c r="B5" s="113"/>
+      <c r="B5" s="112"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -2101,28 +2126,28 @@
     <row r="2" spans="1:8" s="6" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="C2" s="7"/>
-      <c r="D2" s="122"/>
-      <c r="E2" s="122"/>
-      <c r="F2" s="122"/>
-      <c r="G2" s="122"/>
+      <c r="D2" s="124"/>
+      <c r="E2" s="124"/>
+      <c r="F2" s="124"/>
+      <c r="G2" s="124"/>
       <c r="H2" s="5"/>
     </row>
     <row r="3" spans="1:8" s="6" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="C3" s="7"/>
-      <c r="D3" s="123"/>
-      <c r="E3" s="123"/>
-      <c r="F3" s="123"/>
-      <c r="G3" s="123"/>
+      <c r="D3" s="125"/>
+      <c r="E3" s="125"/>
+      <c r="F3" s="125"/>
+      <c r="G3" s="125"/>
       <c r="H3" s="8"/>
     </row>
     <row r="4" spans="1:8" s="6" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="C4" s="7"/>
-      <c r="D4" s="124"/>
-      <c r="E4" s="124"/>
-      <c r="F4" s="124"/>
-      <c r="G4" s="124"/>
+      <c r="D4" s="126"/>
+      <c r="E4" s="126"/>
+      <c r="F4" s="126"/>
+      <c r="G4" s="126"/>
       <c r="H4" s="8"/>
     </row>
     <row r="5" spans="1:8" s="9" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2136,26 +2161,26 @@
     </row>
     <row r="6" spans="1:8" s="14" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
-      <c r="B6" s="125" t="s">
+      <c r="B6" s="127" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="125"/>
-      <c r="D6" s="125"/>
-      <c r="E6" s="125"/>
-      <c r="F6" s="125"/>
-      <c r="G6" s="125"/>
+      <c r="C6" s="127"/>
+      <c r="D6" s="127"/>
+      <c r="E6" s="127"/>
+      <c r="F6" s="127"/>
+      <c r="G6" s="127"/>
     </row>
     <row r="7" spans="1:8" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
-      <c r="B7" s="126" t="str">
+      <c r="B7" s="122" t="str">
         <f>data!B8</f>
         <v>Nomor : 449.1/        /UKM/2023</v>
       </c>
-      <c r="C7" s="126"/>
-      <c r="D7" s="126"/>
-      <c r="E7" s="126"/>
-      <c r="F7" s="126"/>
-      <c r="G7" s="126"/>
+      <c r="C7" s="122"/>
+      <c r="D7" s="122"/>
+      <c r="E7" s="122"/>
+      <c r="F7" s="122"/>
+      <c r="G7" s="122"/>
     </row>
     <row r="8" spans="1:8" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
@@ -2168,23 +2193,23 @@
     </row>
     <row r="9" spans="1:8" s="14" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
-      <c r="B9" s="127" t="s">
+      <c r="B9" s="128" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="127"/>
-      <c r="D9" s="127"/>
-      <c r="E9" s="127"/>
-      <c r="F9" s="127"/>
-      <c r="G9" s="127"/>
+      <c r="C9" s="128"/>
+      <c r="D9" s="128"/>
+      <c r="E9" s="128"/>
+      <c r="F9" s="128"/>
+      <c r="G9" s="128"/>
     </row>
     <row r="10" spans="1:8" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
-      <c r="B10" s="128"/>
-      <c r="C10" s="128"/>
-      <c r="D10" s="128"/>
-      <c r="E10" s="128"/>
-      <c r="F10" s="128"/>
-      <c r="G10" s="128"/>
+      <c r="B10" s="129"/>
+      <c r="C10" s="129"/>
+      <c r="D10" s="129"/>
+      <c r="E10" s="129"/>
+      <c r="F10" s="129"/>
+      <c r="G10" s="129"/>
     </row>
     <row r="11" spans="1:8" s="17" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="16"/>
@@ -2217,7 +2242,7 @@
       <c r="D13" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="E13" s="106">
+      <c r="E13" s="105">
         <f>data!B1</f>
         <v>0</v>
       </c>
@@ -2233,7 +2258,7 @@
       <c r="D14" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="E14" s="106">
+      <c r="E14" s="105">
         <f>data!B2</f>
         <v>0</v>
       </c>
@@ -2249,7 +2274,7 @@
       <c r="D15" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="E15" s="106">
+      <c r="E15" s="105">
         <f>data!B3</f>
         <v>0</v>
       </c>
@@ -2267,7 +2292,7 @@
       <c r="D16" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="E16" s="106">
+      <c r="E16" s="105">
         <f>data!B4</f>
         <v>0</v>
       </c>
@@ -2285,7 +2310,7 @@
       <c r="D17" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="E17" s="106">
+      <c r="E17" s="105">
         <f>data!C1</f>
         <v>0</v>
       </c>
@@ -2303,7 +2328,7 @@
       <c r="D18" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="E18" s="106">
+      <c r="E18" s="105">
         <f>data!C2</f>
         <v>0</v>
       </c>
@@ -2319,7 +2344,7 @@
       <c r="D19" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="E19" s="106">
+      <c r="E19" s="105">
         <f>data!C3</f>
         <v>0</v>
       </c>
@@ -2337,7 +2362,7 @@
       <c r="D20" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="E20" s="106">
+      <c r="E20" s="105">
         <f>data!C4</f>
         <v>0</v>
       </c>
@@ -2386,12 +2411,12 @@
       <c r="D24" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="E24" s="114">
+      <c r="E24" s="113">
         <f>data!B6</f>
         <v>0</v>
       </c>
       <c r="F24" s="20"/>
-      <c r="G24" s="108"/>
+      <c r="G24" s="107"/>
     </row>
     <row r="25" spans="1:7" s="14" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
@@ -2402,7 +2427,7 @@
       <c r="D25" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="E25" s="114">
+      <c r="E25" s="113">
         <f>data!B7</f>
         <v>0</v>
       </c>
@@ -2438,10 +2463,10 @@
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
       <c r="E28" s="27"/>
-      <c r="F28" s="126" t="s">
+      <c r="F28" s="122" t="s">
         <v>17</v>
       </c>
-      <c r="G28" s="126"/>
+      <c r="G28" s="122"/>
     </row>
     <row r="29" spans="1:7" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
@@ -2449,10 +2474,10 @@
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
       <c r="E29" s="27"/>
-      <c r="F29" s="126" t="s">
+      <c r="F29" s="122" t="s">
         <v>18</v>
       </c>
-      <c r="G29" s="126"/>
+      <c r="G29" s="122"/>
     </row>
     <row r="30" spans="1:7" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
@@ -2485,10 +2510,10 @@
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
       <c r="E33" s="27"/>
-      <c r="F33" s="130" t="s">
+      <c r="F33" s="123" t="s">
         <v>19</v>
       </c>
-      <c r="G33" s="130"/>
+      <c r="G33" s="123"/>
       <c r="H33" s="31"/>
     </row>
     <row r="34" spans="1:8" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -2497,10 +2522,10 @@
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
       <c r="E34" s="27"/>
-      <c r="F34" s="129" t="s">
+      <c r="F34" s="120" t="s">
         <v>20</v>
       </c>
-      <c r="G34" s="129"/>
+      <c r="G34" s="120"/>
       <c r="H34" s="32"/>
     </row>
     <row r="35" spans="1:8" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -2619,11 +2644,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="F33:G33"/>
     <mergeCell ref="F17:G17"/>
     <mergeCell ref="D2:G2"/>
     <mergeCell ref="D3:G3"/>
@@ -2636,6 +2656,11 @@
     <mergeCell ref="F12:G12"/>
     <mergeCell ref="F13:G13"/>
     <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="F33:G33"/>
   </mergeCells>
   <pageMargins left="0.59055118110236227" right="0.39370078740157483" top="0.59055118110236227" bottom="1.7716535433070868" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="5" scale="86" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
@@ -2647,8 +2672,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K39"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A22" zoomScale="90" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A4" zoomScale="90" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21:B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2702,23 +2727,23 @@
       <c r="B6" s="3"/>
     </row>
     <row r="7" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="147" t="s">
+      <c r="A7" s="130" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="147"/>
-      <c r="C7" s="147"/>
-      <c r="D7" s="147"/>
-      <c r="E7" s="147"/>
+      <c r="B7" s="130"/>
+      <c r="C7" s="130"/>
+      <c r="D7" s="130"/>
+      <c r="E7" s="130"/>
       <c r="I7" s="39"/>
     </row>
     <row r="8" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="126" t="s">
+      <c r="A8" s="122" t="s">
         <v>88</v>
       </c>
-      <c r="B8" s="126"/>
-      <c r="C8" s="126"/>
-      <c r="D8" s="126"/>
-      <c r="E8" s="126"/>
+      <c r="B8" s="122"/>
+      <c r="C8" s="122"/>
+      <c r="D8" s="122"/>
+      <c r="E8" s="122"/>
       <c r="I8" s="39"/>
     </row>
     <row r="9" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -2735,10 +2760,10 @@
       <c r="C10" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="148" t="s">
+      <c r="D10" s="131" t="s">
         <v>31</v>
       </c>
-      <c r="E10" s="149"/>
+      <c r="E10" s="132"/>
     </row>
     <row r="11" spans="1:11" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="43">
@@ -2756,42 +2781,45 @@
     <row r="12" spans="1:11" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="43"/>
       <c r="C12" s="44"/>
-      <c r="D12" s="120">
+      <c r="D12" s="119">
         <f>data!C1</f>
         <v>0</v>
       </c>
-      <c r="E12" s="115"/>
+      <c r="E12" s="114"/>
       <c r="H12" s="39"/>
       <c r="K12" s="39"/>
     </row>
     <row r="13" spans="1:11" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="137">
+      <c r="A13" s="49"/>
+      <c r="B13" s="164">
         <v>3</v>
       </c>
       <c r="C13" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="116">
+      <c r="D13" s="115">
         <f>data!B3</f>
         <v>0</v>
       </c>
-      <c r="E13" s="117"/>
+      <c r="E13" s="116"/>
       <c r="H13" s="39"/>
       <c r="K13" s="39"/>
     </row>
     <row r="14" spans="1:11" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="137"/>
+      <c r="A14" s="49"/>
+      <c r="B14" s="164"/>
       <c r="C14" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="118">
+      <c r="D14" s="117">
         <f>data!C3</f>
         <v>0</v>
       </c>
-      <c r="E14" s="119"/>
+      <c r="E14" s="118"/>
     </row>
     <row r="15" spans="1:11" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="137"/>
+      <c r="A15" s="49"/>
+      <c r="B15" s="164"/>
       <c r="C15" s="44" t="s">
         <v>35</v>
       </c>
@@ -2802,7 +2830,8 @@
       <c r="E15" s="49"/>
     </row>
     <row r="16" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="146"/>
+      <c r="A16" s="49"/>
+      <c r="B16" s="159"/>
       <c r="C16" s="44" t="s">
         <v>36</v>
       </c>
@@ -2813,78 +2842,84 @@
       <c r="E16" s="50"/>
       <c r="H16" s="39"/>
     </row>
-    <row r="17" spans="2:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="41">
+    <row r="17" spans="1:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="49"/>
+      <c r="B17" s="165">
         <v>4</v>
       </c>
       <c r="C17" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="D17" s="101">
+      <c r="D17" s="100">
         <f>data!B6</f>
         <v>0</v>
       </c>
-      <c r="E17" s="107"/>
+      <c r="E17" s="106"/>
       <c r="H17" s="39"/>
     </row>
-    <row r="18" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="41">
+    <row r="18" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="49"/>
+      <c r="B18" s="165">
         <v>5</v>
       </c>
       <c r="C18" s="51" t="s">
         <v>38</v>
       </c>
-      <c r="D18" s="150" t="s">
+      <c r="D18" s="134" t="s">
         <v>39</v>
       </c>
-      <c r="E18" s="151"/>
+      <c r="E18" s="135"/>
       <c r="H18" s="39"/>
     </row>
-    <row r="19" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="137">
+    <row r="19" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="49"/>
+      <c r="B19" s="164">
         <v>6</v>
       </c>
       <c r="C19" s="47" t="s">
         <v>40</v>
       </c>
-      <c r="D19" s="134" t="s">
+      <c r="D19" s="136" t="s">
         <v>41</v>
       </c>
-      <c r="E19" s="135"/>
-    </row>
-    <row r="20" spans="2:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="137"/>
+      <c r="E19" s="137"/>
+    </row>
+    <row r="20" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="49"/>
+      <c r="B20" s="164"/>
       <c r="C20" s="52" t="s">
         <v>42</v>
       </c>
-      <c r="D20" s="144">
+      <c r="D20" s="138">
         <f>data!B7</f>
         <v>0</v>
       </c>
-      <c r="E20" s="145"/>
-    </row>
-    <row r="21" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="137">
+      <c r="E20" s="139"/>
+    </row>
+    <row r="21" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="49"/>
+      <c r="B21" s="164">
         <v>7</v>
       </c>
       <c r="C21" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="D21" s="134" t="s">
+      <c r="D21" s="136" t="s">
         <v>44</v>
       </c>
-      <c r="E21" s="135"/>
-    </row>
-    <row r="22" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="137"/>
+      <c r="E21" s="137"/>
+    </row>
+    <row r="22" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="133"/>
       <c r="C22" s="44" t="s">
         <v>45</v>
       </c>
       <c r="D22" s="53"/>
-      <c r="E22" s="105"/>
-    </row>
-    <row r="23" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="146"/>
+      <c r="E22" s="104"/>
+    </row>
+    <row r="23" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="49"/>
+      <c r="B23" s="159"/>
       <c r="C23" s="44" t="s">
         <v>46</v>
       </c>
@@ -2892,135 +2927,131 @@
         <f>D22</f>
         <v>0</v>
       </c>
-      <c r="E23" s="109"/>
-    </row>
-    <row r="24" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="132">
+      <c r="E23" s="108"/>
+    </row>
+    <row r="24" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="49"/>
+      <c r="B24" s="160">
         <v>8</v>
       </c>
       <c r="C24" s="55" t="s">
         <v>47</v>
       </c>
-      <c r="D24" s="134" t="s">
+      <c r="D24" s="136" t="s">
         <v>6</v>
       </c>
-      <c r="E24" s="135"/>
-    </row>
-    <row r="25" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="133"/>
+      <c r="E24" s="137"/>
+    </row>
+    <row r="25" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="49"/>
+      <c r="B25" s="161"/>
       <c r="C25" s="48"/>
       <c r="D25" s="56"/>
       <c r="E25" s="49"/>
     </row>
-    <row r="26" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="57"/>
-      <c r="C26" s="58" t="s">
+    <row r="26" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="49"/>
+      <c r="B26" s="162"/>
+      <c r="C26" s="57" t="s">
         <v>48</v>
       </c>
-      <c r="D26" s="59" t="s">
+      <c r="D26" s="58" t="s">
         <v>49</v>
       </c>
       <c r="E26" s="49"/>
     </row>
-    <row r="27" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="136">
+    <row r="27" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="49"/>
+      <c r="B27" s="163">
         <v>9</v>
       </c>
-      <c r="C27" s="60" t="s">
+      <c r="C27" s="59" t="s">
         <v>50</v>
       </c>
-      <c r="D27" s="138" t="s">
+      <c r="D27" s="141" t="s">
         <v>51</v>
       </c>
-      <c r="E27" s="139"/>
-    </row>
-    <row r="28" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="137"/>
-      <c r="C28" s="60" t="s">
+      <c r="E27" s="142"/>
+    </row>
+    <row r="28" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="49"/>
+      <c r="B28" s="164"/>
+      <c r="C28" s="59" t="s">
         <v>52</v>
       </c>
-      <c r="D28" s="140" t="s">
+      <c r="D28" s="143" t="s">
         <v>53</v>
       </c>
-      <c r="E28" s="141"/>
-    </row>
-    <row r="29" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="137"/>
-      <c r="C29" s="61" t="s">
+      <c r="E28" s="144"/>
+    </row>
+    <row r="29" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="49"/>
+      <c r="B29" s="164"/>
+      <c r="C29" s="60" t="s">
         <v>54</v>
       </c>
-      <c r="D29" s="142" t="s">
+      <c r="D29" s="145" t="s">
         <v>55</v>
       </c>
-      <c r="E29" s="143"/>
-    </row>
-    <row r="30" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="62">
+      <c r="E29" s="146"/>
+    </row>
+    <row r="30" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="61">
         <v>10</v>
       </c>
-      <c r="C30" s="63" t="s">
+      <c r="C30" s="62" t="s">
         <v>56</v>
       </c>
       <c r="D30" s="42"/>
-      <c r="E30" s="64"/>
-    </row>
-    <row r="31" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D32" s="65" t="s">
+      <c r="E30" s="63"/>
+    </row>
+    <row r="31" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D32" s="64" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="33" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D33" s="66" t="s">
+      <c r="D33" s="65" t="s">
         <v>58</v>
       </c>
       <c r="E33" s="54">
         <f>D22</f>
         <v>0</v>
       </c>
-      <c r="F33" s="105"/>
+      <c r="F33" s="104"/>
     </row>
     <row r="34" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="33"/>
       <c r="C34" s="33"/>
-      <c r="D34" s="131" t="s">
+      <c r="D34" s="140" t="s">
         <v>31</v>
       </c>
-      <c r="E34" s="131"/>
+      <c r="E34" s="140"/>
     </row>
     <row r="35" spans="2:6" s="33" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D35" s="67"/>
+      <c r="D35" s="66"/>
     </row>
     <row r="36" spans="2:6" s="33" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D36" s="67"/>
+      <c r="D36" s="66"/>
     </row>
     <row r="37" spans="2:6" s="33" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D37" s="67"/>
+      <c r="D37" s="66"/>
     </row>
     <row r="38" spans="2:6" s="33" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D38" s="130" t="s">
+      <c r="D38" s="123" t="s">
         <v>19</v>
       </c>
-      <c r="E38" s="130"/>
+      <c r="E38" s="123"/>
     </row>
     <row r="39" spans="2:6" s="33" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D39" s="129" t="s">
+      <c r="D39" s="120" t="s">
         <v>20</v>
       </c>
-      <c r="E39" s="129"/>
+      <c r="E39" s="120"/>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="A7:E7"/>
-    <mergeCell ref="A8:E8"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="B13:B16"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="B21:B23"/>
-    <mergeCell ref="D21:E21"/>
     <mergeCell ref="D34:E34"/>
     <mergeCell ref="D38:E38"/>
     <mergeCell ref="D39:E39"/>
@@ -3030,6 +3061,16 @@
     <mergeCell ref="D27:E27"/>
     <mergeCell ref="D28:E28"/>
     <mergeCell ref="D29:E29"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="A7:E7"/>
+    <mergeCell ref="A8:E8"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="B13:B16"/>
+    <mergeCell ref="D18:E18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.45" top="0.25" bottom="1.5" header="0.3" footer="0.3"/>
   <pageSetup paperSize="5" scale="92" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
@@ -3074,67 +3115,67 @@
       </c>
     </row>
     <row r="6" spans="2:7" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E6" s="65" t="s">
+      <c r="E6" s="64" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="7" spans="2:7" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E7" s="65" t="s">
+      <c r="E7" s="64" t="s">
         <v>89</v>
       </c>
-      <c r="F7" s="68"/>
+      <c r="F7" s="67"/>
     </row>
     <row r="8" spans="2:7" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="69"/>
-      <c r="D8" s="69"/>
-      <c r="E8" s="65" t="s">
+      <c r="C8" s="68"/>
+      <c r="D8" s="68"/>
+      <c r="E8" s="64" t="s">
         <v>61</v>
       </c>
-      <c r="F8" s="160">
+      <c r="F8" s="150">
         <f>data!B7</f>
         <v>0</v>
       </c>
-      <c r="G8" s="160"/>
+      <c r="G8" s="150"/>
     </row>
     <row r="9" spans="2:7" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E9" s="70"/>
+      <c r="E9" s="69"/>
     </row>
     <row r="10" spans="2:7" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E10" s="67"/>
+      <c r="E10" s="66"/>
     </row>
     <row r="11" spans="2:7" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="71" t="s">
+      <c r="B11" s="70" t="s">
         <v>62</v>
       </c>
-      <c r="C11" s="72" t="s">
+      <c r="C11" s="71" t="s">
         <v>63</v>
       </c>
-      <c r="D11" s="72"/>
-      <c r="E11" s="73" t="s">
+      <c r="D11" s="71"/>
+      <c r="E11" s="72" t="s">
         <v>64</v>
       </c>
-      <c r="F11" s="74"/>
+      <c r="F11" s="73"/>
     </row>
     <row r="12" spans="2:7" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="75"/>
-      <c r="C12" s="161">
+      <c r="B12" s="74"/>
+      <c r="C12" s="151">
         <f>F8</f>
         <v>0</v>
       </c>
-      <c r="D12" s="161"/>
-      <c r="E12" s="162">
+      <c r="D12" s="151"/>
+      <c r="E12" s="152">
         <f>C12</f>
         <v>0</v>
       </c>
-      <c r="F12" s="163"/>
+      <c r="F12" s="153"/>
     </row>
     <row r="13" spans="2:7" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="75"/>
-      <c r="C13" s="65" t="str">
+      <c r="B13" s="74"/>
+      <c r="C13" s="64" t="str">
         <f>E7</f>
         <v>Pada Tanggal</v>
       </c>
-      <c r="D13" s="68">
+      <c r="D13" s="67">
         <f>F7</f>
         <v>0</v>
       </c>
@@ -3142,448 +3183,448 @@
         <f>E7</f>
         <v>Pada Tanggal</v>
       </c>
-      <c r="F13" s="76">
+      <c r="F13" s="75">
         <f>D13</f>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="2:7" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="75"/>
-      <c r="C14" s="65"/>
-      <c r="D14" s="65"/>
+      <c r="B14" s="74"/>
+      <c r="C14" s="64"/>
+      <c r="D14" s="64"/>
       <c r="E14" s="48" t="s">
         <v>65</v>
       </c>
-      <c r="F14" s="77"/>
+      <c r="F14" s="76"/>
     </row>
     <row r="15" spans="2:7" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="75"/>
-      <c r="C15" s="131" t="s">
+      <c r="B15" s="74"/>
+      <c r="C15" s="140" t="s">
         <v>66</v>
       </c>
-      <c r="D15" s="131"/>
-      <c r="E15" s="158" t="s">
+      <c r="D15" s="140"/>
+      <c r="E15" s="154" t="s">
         <v>66</v>
       </c>
-      <c r="F15" s="157"/>
+      <c r="F15" s="155"/>
     </row>
     <row r="16" spans="2:7" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="75"/>
+      <c r="B16" s="74"/>
       <c r="E16" s="48"/>
-      <c r="F16" s="78"/>
+      <c r="F16" s="77"/>
     </row>
     <row r="17" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="75"/>
+      <c r="B17" s="74"/>
       <c r="D17" s="33" t="s">
         <v>11</v>
       </c>
       <c r="E17" s="48"/>
-      <c r="F17" s="78"/>
+      <c r="F17" s="77"/>
     </row>
     <row r="18" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="75"/>
+      <c r="B18" s="74"/>
       <c r="E18" s="48"/>
-      <c r="F18" s="78"/>
+      <c r="F18" s="77"/>
     </row>
     <row r="19" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="75"/>
-      <c r="C19" s="152" t="s">
+      <c r="B19" s="74"/>
+      <c r="C19" s="147" t="s">
         <v>67</v>
       </c>
-      <c r="D19" s="152"/>
-      <c r="E19" s="159" t="s">
+      <c r="D19" s="147"/>
+      <c r="E19" s="148" t="s">
         <v>67</v>
       </c>
-      <c r="F19" s="156"/>
+      <c r="F19" s="149"/>
     </row>
     <row r="20" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="79"/>
-      <c r="C20" s="80" t="s">
+      <c r="B20" s="78"/>
+      <c r="C20" s="79" t="s">
         <v>68</v>
       </c>
-      <c r="D20" s="81"/>
-      <c r="E20" s="82" t="s">
+      <c r="D20" s="80"/>
+      <c r="E20" s="81" t="s">
         <v>68</v>
       </c>
-      <c r="F20" s="83"/>
+      <c r="F20" s="82"/>
     </row>
     <row r="21" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="71" t="s">
+      <c r="B21" s="70" t="s">
         <v>69</v>
       </c>
-      <c r="C21" s="72"/>
-      <c r="D21" s="74"/>
-      <c r="E21" s="73" t="s">
+      <c r="C21" s="71"/>
+      <c r="D21" s="73"/>
+      <c r="E21" s="72" t="s">
         <v>64</v>
       </c>
-      <c r="F21" s="74"/>
+      <c r="F21" s="73"/>
     </row>
     <row r="22" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="75"/>
-      <c r="C22" s="65" t="s">
+      <c r="B22" s="74"/>
+      <c r="C22" s="64" t="s">
         <v>70</v>
       </c>
-      <c r="D22" s="84">
+      <c r="D22" s="83">
         <f>C12</f>
         <v>0</v>
       </c>
-      <c r="E22" s="112" t="s">
+      <c r="E22" s="111" t="s">
         <v>70</v>
       </c>
-      <c r="F22" s="85"/>
+      <c r="F22" s="84"/>
     </row>
     <row r="23" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="75"/>
-      <c r="C23" s="65" t="s">
+      <c r="B23" s="74"/>
+      <c r="C23" s="64" t="s">
         <v>71</v>
       </c>
-      <c r="D23" s="86"/>
+      <c r="D23" s="85"/>
       <c r="E23" s="48" t="s">
         <v>71</v>
       </c>
-      <c r="F23" s="86"/>
+      <c r="F23" s="85"/>
     </row>
     <row r="24" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="75"/>
-      <c r="C24" s="65"/>
-      <c r="D24" s="77"/>
+      <c r="B24" s="74"/>
+      <c r="C24" s="64"/>
+      <c r="D24" s="76"/>
       <c r="E24" s="48" t="s">
         <v>72</v>
       </c>
-      <c r="F24" s="77"/>
+      <c r="F24" s="76"/>
     </row>
     <row r="25" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="75"/>
-      <c r="C25" s="131" t="s">
+      <c r="B25" s="74"/>
+      <c r="C25" s="140" t="s">
         <v>66</v>
       </c>
-      <c r="D25" s="157"/>
-      <c r="E25" s="158" t="s">
+      <c r="D25" s="155"/>
+      <c r="E25" s="154" t="s">
         <v>66</v>
       </c>
-      <c r="F25" s="157"/>
+      <c r="F25" s="155"/>
     </row>
     <row r="26" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="75"/>
-      <c r="D26" s="78"/>
+      <c r="B26" s="74"/>
+      <c r="D26" s="77"/>
       <c r="E26" s="48"/>
-      <c r="F26" s="78"/>
+      <c r="F26" s="77"/>
     </row>
     <row r="27" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="75"/>
-      <c r="D27" s="78"/>
+      <c r="B27" s="74"/>
+      <c r="D27" s="77"/>
       <c r="E27" s="48"/>
-      <c r="F27" s="78"/>
+      <c r="F27" s="77"/>
     </row>
     <row r="28" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="75"/>
-      <c r="D28" s="78"/>
+      <c r="B28" s="74"/>
+      <c r="D28" s="77"/>
       <c r="E28" s="48"/>
-      <c r="F28" s="78"/>
+      <c r="F28" s="77"/>
     </row>
     <row r="29" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="75"/>
-      <c r="C29" s="152" t="s">
+      <c r="B29" s="74"/>
+      <c r="C29" s="147" t="s">
         <v>67</v>
       </c>
-      <c r="D29" s="156"/>
-      <c r="E29" s="152" t="s">
+      <c r="D29" s="149"/>
+      <c r="E29" s="147" t="s">
         <v>67</v>
       </c>
-      <c r="F29" s="156"/>
+      <c r="F29" s="149"/>
     </row>
     <row r="30" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="79"/>
-      <c r="C30" s="80" t="s">
+      <c r="B30" s="78"/>
+      <c r="C30" s="79" t="s">
         <v>68</v>
       </c>
-      <c r="D30" s="83"/>
-      <c r="E30" s="82" t="s">
+      <c r="D30" s="82"/>
+      <c r="E30" s="81" t="s">
         <v>68</v>
       </c>
-      <c r="F30" s="83"/>
+      <c r="F30" s="82"/>
     </row>
     <row r="31" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="71" t="s">
+      <c r="B31" s="70" t="s">
         <v>73</v>
       </c>
-      <c r="C31" s="72"/>
-      <c r="D31" s="74"/>
-      <c r="E31" s="73" t="s">
+      <c r="C31" s="71"/>
+      <c r="D31" s="73"/>
+      <c r="E31" s="72" t="s">
         <v>64</v>
       </c>
-      <c r="F31" s="74"/>
+      <c r="F31" s="73"/>
     </row>
     <row r="32" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="75"/>
-      <c r="C32" s="65" t="s">
+      <c r="B32" s="74"/>
+      <c r="C32" s="64" t="s">
         <v>74</v>
       </c>
-      <c r="D32" s="88"/>
-      <c r="E32" s="111" t="s">
+      <c r="D32" s="87"/>
+      <c r="E32" s="110" t="s">
         <v>74</v>
       </c>
-      <c r="F32" s="89"/>
+      <c r="F32" s="88"/>
     </row>
     <row r="33" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="75"/>
-      <c r="C33" s="65" t="s">
+      <c r="B33" s="74"/>
+      <c r="C33" s="64" t="s">
         <v>71</v>
       </c>
-      <c r="D33" s="90"/>
-      <c r="E33" s="110" t="s">
+      <c r="D33" s="89"/>
+      <c r="E33" s="109" t="s">
         <v>71</v>
       </c>
-      <c r="F33" s="90"/>
+      <c r="F33" s="89"/>
     </row>
     <row r="34" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="75"/>
-      <c r="C34" s="65"/>
+      <c r="B34" s="74"/>
+      <c r="C34" s="64"/>
       <c r="E34" s="48" t="s">
         <v>72</v>
       </c>
-      <c r="F34" s="91"/>
+      <c r="F34" s="90"/>
     </row>
     <row r="35" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="75"/>
-      <c r="C35" s="131" t="s">
+      <c r="B35" s="74"/>
+      <c r="C35" s="140" t="s">
         <v>66</v>
       </c>
-      <c r="D35" s="157"/>
-      <c r="E35" s="158" t="s">
+      <c r="D35" s="155"/>
+      <c r="E35" s="154" t="s">
         <v>66</v>
       </c>
-      <c r="F35" s="157"/>
+      <c r="F35" s="155"/>
     </row>
     <row r="36" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="75"/>
-      <c r="D36" s="78"/>
+      <c r="B36" s="74"/>
+      <c r="D36" s="77"/>
       <c r="E36" s="48"/>
-      <c r="F36" s="78"/>
+      <c r="F36" s="77"/>
     </row>
     <row r="37" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="75"/>
-      <c r="D37" s="78"/>
+      <c r="B37" s="74"/>
+      <c r="D37" s="77"/>
       <c r="E37" s="48"/>
-      <c r="F37" s="78"/>
+      <c r="F37" s="77"/>
     </row>
     <row r="38" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="75"/>
-      <c r="D38" s="78"/>
+      <c r="B38" s="74"/>
+      <c r="D38" s="77"/>
       <c r="E38" s="48"/>
-      <c r="F38" s="78"/>
+      <c r="F38" s="77"/>
     </row>
     <row r="39" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="75"/>
-      <c r="C39" s="152" t="s">
+      <c r="B39" s="74"/>
+      <c r="C39" s="147" t="s">
         <v>67</v>
       </c>
-      <c r="D39" s="156"/>
-      <c r="E39" s="152" t="s">
+      <c r="D39" s="149"/>
+      <c r="E39" s="147" t="s">
         <v>67</v>
       </c>
-      <c r="F39" s="156"/>
+      <c r="F39" s="149"/>
     </row>
     <row r="40" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="79"/>
-      <c r="C40" s="80" t="s">
+      <c r="B40" s="78"/>
+      <c r="C40" s="79" t="s">
         <v>68</v>
       </c>
-      <c r="D40" s="83"/>
-      <c r="E40" s="82" t="s">
+      <c r="D40" s="82"/>
+      <c r="E40" s="81" t="s">
         <v>68</v>
       </c>
-      <c r="F40" s="83"/>
+      <c r="F40" s="82"/>
     </row>
     <row r="41" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="71" t="s">
+      <c r="B41" s="70" t="s">
         <v>75</v>
       </c>
-      <c r="C41" s="72"/>
-      <c r="D41" s="74"/>
-      <c r="E41" s="73" t="s">
+      <c r="C41" s="71"/>
+      <c r="D41" s="73"/>
+      <c r="E41" s="72" t="s">
         <v>64</v>
       </c>
-      <c r="F41" s="74"/>
+      <c r="F41" s="73"/>
     </row>
     <row r="42" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="75"/>
-      <c r="C42" s="65" t="s">
+      <c r="B42" s="74"/>
+      <c r="C42" s="64" t="s">
         <v>74</v>
       </c>
-      <c r="D42" s="92"/>
-      <c r="E42" s="93"/>
-      <c r="F42" s="94"/>
+      <c r="D42" s="91"/>
+      <c r="E42" s="92"/>
+      <c r="F42" s="93"/>
     </row>
     <row r="43" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="75"/>
-      <c r="C43" s="65" t="s">
+      <c r="B43" s="74"/>
+      <c r="C43" s="64" t="s">
         <v>71</v>
       </c>
-      <c r="D43" s="86"/>
-      <c r="E43" s="87"/>
-      <c r="F43" s="86"/>
+      <c r="D43" s="85"/>
+      <c r="E43" s="86"/>
+      <c r="F43" s="85"/>
     </row>
     <row r="44" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="75"/>
-      <c r="C44" s="65"/>
+      <c r="B44" s="74"/>
+      <c r="C44" s="64"/>
       <c r="E44" s="48" t="s">
         <v>72</v>
       </c>
-      <c r="F44" s="91"/>
+      <c r="F44" s="90"/>
     </row>
     <row r="45" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="75"/>
-      <c r="C45" s="131" t="s">
+      <c r="B45" s="74"/>
+      <c r="C45" s="140" t="s">
         <v>66</v>
       </c>
-      <c r="D45" s="157"/>
-      <c r="E45" s="158" t="s">
+      <c r="D45" s="155"/>
+      <c r="E45" s="154" t="s">
         <v>66</v>
       </c>
-      <c r="F45" s="157"/>
+      <c r="F45" s="155"/>
     </row>
     <row r="46" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="75"/>
-      <c r="D46" s="78"/>
+      <c r="B46" s="74"/>
+      <c r="D46" s="77"/>
       <c r="E46" s="48"/>
-      <c r="F46" s="78"/>
+      <c r="F46" s="77"/>
     </row>
     <row r="47" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="75"/>
-      <c r="D47" s="78"/>
+      <c r="B47" s="74"/>
+      <c r="D47" s="77"/>
       <c r="E47" s="48"/>
-      <c r="F47" s="78"/>
+      <c r="F47" s="77"/>
     </row>
     <row r="48" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="75"/>
-      <c r="D48" s="78"/>
+      <c r="B48" s="74"/>
+      <c r="D48" s="77"/>
       <c r="E48" s="48"/>
-      <c r="F48" s="78"/>
+      <c r="F48" s="77"/>
     </row>
     <row r="49" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="75"/>
-      <c r="C49" s="152" t="s">
+      <c r="B49" s="74"/>
+      <c r="C49" s="147" t="s">
         <v>67</v>
       </c>
-      <c r="D49" s="156"/>
-      <c r="E49" s="159" t="s">
+      <c r="D49" s="149"/>
+      <c r="E49" s="148" t="s">
         <v>67</v>
       </c>
-      <c r="F49" s="156"/>
+      <c r="F49" s="149"/>
     </row>
     <row r="50" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="79"/>
-      <c r="C50" s="80" t="s">
+      <c r="B50" s="78"/>
+      <c r="C50" s="79" t="s">
         <v>68</v>
       </c>
-      <c r="D50" s="83"/>
-      <c r="E50" s="82" t="s">
+      <c r="D50" s="82"/>
+      <c r="E50" s="81" t="s">
         <v>68</v>
       </c>
-      <c r="F50" s="83"/>
+      <c r="F50" s="82"/>
     </row>
     <row r="51" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="75" t="s">
+      <c r="B51" s="74" t="s">
         <v>76</v>
       </c>
-      <c r="C51" s="95" t="s">
+      <c r="C51" s="94" t="s">
         <v>77</v>
       </c>
-      <c r="D51" s="95"/>
-      <c r="E51" s="95"/>
-      <c r="F51" s="96"/>
+      <c r="D51" s="94"/>
+      <c r="E51" s="94"/>
+      <c r="F51" s="95"/>
     </row>
     <row r="52" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="75"/>
+      <c r="B52" s="74"/>
       <c r="C52" s="33" t="s">
         <v>78</v>
       </c>
-      <c r="F52" s="78"/>
+      <c r="F52" s="77"/>
     </row>
     <row r="53" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="75"/>
+      <c r="B53" s="74"/>
       <c r="C53" s="33" t="s">
         <v>79</v>
       </c>
-      <c r="F53" s="97"/>
+      <c r="F53" s="96"/>
     </row>
     <row r="54" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="75"/>
-      <c r="C54" s="152"/>
-      <c r="D54" s="152"/>
-      <c r="E54" s="152"/>
-      <c r="F54" s="98"/>
+      <c r="B54" s="74"/>
+      <c r="C54" s="147"/>
+      <c r="D54" s="147"/>
+      <c r="E54" s="147"/>
+      <c r="F54" s="97"/>
     </row>
     <row r="55" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="75"/>
-      <c r="F55" s="78"/>
+      <c r="B55" s="74"/>
+      <c r="F55" s="77"/>
     </row>
     <row r="56" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="75"/>
-      <c r="C56" s="126" t="s">
+      <c r="B56" s="74"/>
+      <c r="C56" s="122" t="s">
         <v>31</v>
       </c>
-      <c r="D56" s="126"/>
-      <c r="E56" s="126"/>
-      <c r="F56" s="153"/>
+      <c r="D56" s="122"/>
+      <c r="E56" s="122"/>
+      <c r="F56" s="156"/>
     </row>
     <row r="57" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="75"/>
+      <c r="B57" s="74"/>
       <c r="C57" s="3"/>
       <c r="D57" s="3"/>
       <c r="E57" s="15"/>
-      <c r="F57" s="99"/>
+      <c r="F57" s="98"/>
     </row>
     <row r="58" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="75"/>
+      <c r="B58" s="74"/>
       <c r="C58" s="3"/>
       <c r="D58" s="3"/>
       <c r="E58" s="3"/>
-      <c r="F58" s="99"/>
+      <c r="F58" s="98"/>
     </row>
     <row r="59" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="75"/>
+      <c r="B59" s="74"/>
       <c r="C59" s="3"/>
       <c r="D59" s="3"/>
       <c r="E59" s="3"/>
-      <c r="F59" s="99"/>
+      <c r="F59" s="98"/>
     </row>
     <row r="60" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="75"/>
-      <c r="C60" s="154" t="s">
+      <c r="B60" s="74"/>
+      <c r="C60" s="157" t="s">
         <v>19</v>
       </c>
-      <c r="D60" s="154"/>
-      <c r="E60" s="154"/>
-      <c r="F60" s="155"/>
+      <c r="D60" s="157"/>
+      <c r="E60" s="157"/>
+      <c r="F60" s="158"/>
     </row>
     <row r="61" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="75"/>
-      <c r="C61" s="126" t="s">
+      <c r="B61" s="74"/>
+      <c r="C61" s="122" t="s">
         <v>20</v>
       </c>
-      <c r="D61" s="126"/>
-      <c r="E61" s="126"/>
-      <c r="F61" s="153"/>
+      <c r="D61" s="122"/>
+      <c r="E61" s="122"/>
+      <c r="F61" s="156"/>
     </row>
     <row r="62" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="79"/>
-      <c r="C62" s="80"/>
-      <c r="D62" s="80"/>
-      <c r="E62" s="80"/>
-      <c r="F62" s="100"/>
+      <c r="B62" s="78"/>
+      <c r="C62" s="79"/>
+      <c r="D62" s="79"/>
+      <c r="E62" s="79"/>
+      <c r="F62" s="99"/>
     </row>
     <row r="63" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="101" t="s">
+      <c r="B63" s="100" t="s">
         <v>80</v>
       </c>
-      <c r="C63" s="102" t="s">
+      <c r="C63" s="101" t="s">
         <v>81</v>
       </c>
-      <c r="D63" s="102"/>
-      <c r="E63" s="103"/>
-      <c r="F63" s="104"/>
+      <c r="D63" s="101"/>
+      <c r="E63" s="102"/>
+      <c r="F63" s="103"/>
     </row>
     <row r="64" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B64" s="33" t="s">
@@ -3633,19 +3674,6 @@
     <row r="82" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="E35:F35"/>
     <mergeCell ref="C54:E54"/>
     <mergeCell ref="C56:F56"/>
     <mergeCell ref="C60:F60"/>
@@ -3656,6 +3684,19 @@
     <mergeCell ref="E45:F45"/>
     <mergeCell ref="C49:D49"/>
     <mergeCell ref="E49:F49"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="E15:F15"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.43307086614173229" top="0.23622047244094491" bottom="1.4960629921259843" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="5" scale="86" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
refactor: excel source format
</commit_message>
<xml_diff>
--- a/src/assets/sppd.xlsx
+++ b/src/assets/sppd.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45E6B73C-46D6-4BDB-9F6C-CA1A54AAD893}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B25FD93B-D5C1-46DE-98E9-EC463EE860CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="4" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="92">
   <si>
     <t>SURAT TUGAS</t>
   </si>
@@ -102,35 +102,6 @@
     <t>........................................</t>
   </si>
   <si>
-    <t>Berdasarkan : Peraturan Daerah Kabupaten Semarang Nomor 9 tahun  2022 tentang anggaran Pendapatan dan Belanja Daerah Kab.Semarang tahun anggaran 2023 dan Peraturan Bupati Semarang Nomor 118 tahun 2022 Tentang penjabaran anggaran Pendapatan dan belanja daerah Kabupaten Semarang Tahun 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        PEMERINTAH KABUPATEN SEMARANG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                          DINAS KESEHATAN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    UPTD PUSKESMAS LEREP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                  Jl . Yudhistira km 3 Telp. (024) 6923416 Ungaran</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>DHARMOTTAMA SATYA PRAJA</t>
-    </r>
-  </si>
-  <si>
     <t>SURAT PERINTAH PERJALANAN DINAS</t>
   </si>
   <si>
@@ -143,78 +114,6 @@
     <t>Nama pegawai yang diperintahkan</t>
   </si>
   <si>
-    <r>
-      <t>a.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">       </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">Pangkat dan golongan ruang gaji menurut </t>
-    </r>
-  </si>
-  <si>
-    <t>PP no 6 tahun 1997</t>
-  </si>
-  <si>
-    <r>
-      <t>b.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">      </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Jabatan/ Instansi</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>c.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">       </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Tingkat menurut peraturan perjalanan dinas</t>
-    </r>
-  </si>
-  <si>
     <t>Maksud perjalanan dinas</t>
   </si>
   <si>
@@ -224,125 +123,10 @@
     <t>Kendaraan pribadi</t>
   </si>
   <si>
-    <r>
-      <t>a.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">       </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Tempat berangkat</t>
-    </r>
-  </si>
-  <si>
     <t>UPTD Puskesmas Lerep</t>
   </si>
   <si>
-    <r>
-      <t>b.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">      </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Tempat tujuan</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>a.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">       </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Lama perjalanan dinas</t>
-    </r>
-  </si>
-  <si>
     <t>1 (satu) hari</t>
-  </si>
-  <si>
-    <r>
-      <t>b.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">      </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Tanggal berangkat</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>c.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">      </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Tanggal harus kembali</t>
-    </r>
   </si>
   <si>
     <t>Pengikut</t>
@@ -409,9 +193,6 @@
     </r>
   </si>
   <si>
-    <t>b. 1.02.1.02.01.16.55</t>
-  </si>
-  <si>
     <t>Keterangan Lain</t>
   </si>
   <si>
@@ -508,9 +289,6 @@
     <t>kealpaan</t>
   </si>
   <si>
-    <t>Nomor : 449.1/        /UKM/2023</t>
-  </si>
-  <si>
     <t>Pada Tanggal</t>
   </si>
   <si>
@@ -536,6 +314,170 @@
   </si>
   <si>
     <t>nomor</t>
+  </si>
+  <si>
+    <t>Peraturan Daerah Kabupaten Semarang Nomor 14 tahun 2023 tanggal 21 Desember 2023 tentang Anggaran Pendapatan dan Belanja Daerah Kabupaten Semarang tahun anggaran 2024 dan Peraturan Bupati Semarang Nomor 79 tahun 2023 tanggal 22 Desember 2023 tentang penjabaran Anggaran Pendapatan dan Belanja Daerah Kabupaten Semarang Tahun 2024 Berita Daerah Kabupaten Semarang Tahun 2023 No 79</t>
+  </si>
+  <si>
+    <t>Berdasarkan</t>
+  </si>
+  <si>
+    <t>a. Pangkat dan golongan ruang gaji menurut PP no 6 tahun 1997</t>
+  </si>
+  <si>
+    <r>
+      <t>b.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Jabatan/ Instansi</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>c.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Tingkat menurut peraturan perjalanan dinas</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">a. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Tempat berangkat</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>b.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Tempat tujuan</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>a.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Lama perjalanan dinas</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>b.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Tanggal berangkat</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>c.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Tanggal harus kembali</t>
+    </r>
+  </si>
+  <si>
+    <t>Nomor : 449.1/        /UKM/2024</t>
   </si>
 </sst>
 </file>
@@ -547,7 +489,7 @@
     <numFmt numFmtId="165" formatCode="[$-409]dd\-mmm\-yy;@"/>
     <numFmt numFmtId="166" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="30" x14ac:knownFonts="1">
+  <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -599,13 +541,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="24"/>
       <color indexed="8"/>
       <name val="Times New Roman"/>
       <family val="1"/>
@@ -693,13 +628,6 @@
       <family val="1"/>
     </font>
     <font>
-      <b/>
-      <sz val="16"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
@@ -754,21 +682,12 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="27">
+  <borders count="28">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1050,437 +969,486 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="166">
+  <cellXfs count="169">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="12" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="15" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="15" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="19" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="20" xfId="2" applyBorder="1"/>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="2" applyBorder="1"/>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="15" fontId="25" fillId="0" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="23" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="2" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="23" fillId="2" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="2" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="23" fillId="2" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="23" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="15" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="24" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="27" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="26" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="23" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="24" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="26" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="20" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="20" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1506,16 +1474,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>130095</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:rowOff>58510</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1706869</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:rowOff>163287</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1539,14 +1507,12 @@
           </a:extLst>
         </a:blip>
         <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
+        <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="0" y="104775"/>
-          <a:ext cx="7038975" cy="1333500"/>
+          <a:off x="252559" y="58510"/>
+          <a:ext cx="6570596" cy="1383848"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1583,25 +1549,25 @@
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>676275</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:rowOff>74084</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1628775</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:colOff>1606206</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>179917</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2053" name="Picture 3">
+        <xdr:cNvPr id="4" name="Picture 0">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7585836D-8073-4A2E-AC37-108F95096D3C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5882133C-A36C-4D97-80E7-0ACD09DD4A76}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1618,88 +1584,12 @@
           </a:extLst>
         </a:blip>
         <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
+        <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="5162550" y="114300"/>
-          <a:ext cx="952500" cy="1076325"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2054" name="Picture 342">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7F82165C-FE7C-4718-8CF1-CBA229AAE425}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="57150" y="57150"/>
-          <a:ext cx="990600" cy="1038225"/>
+          <a:off x="63500" y="74084"/>
+          <a:ext cx="6030039" cy="1270000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2034,7 +1924,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2044,46 +1934,46 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>90</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>91</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>92</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>93</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>94</v>
-      </c>
-      <c r="B5" s="112"/>
+        <v>77</v>
+      </c>
+      <c r="B5" s="86"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>95</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>97</v>
+        <v>80</v>
       </c>
       <c r="B8" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -2096,8 +1986,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H52"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2126,31 +2016,31 @@
     <row r="2" spans="1:8" s="6" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="C2" s="7"/>
-      <c r="D2" s="124"/>
-      <c r="E2" s="124"/>
-      <c r="F2" s="124"/>
-      <c r="G2" s="124"/>
+      <c r="D2" s="126"/>
+      <c r="E2" s="126"/>
+      <c r="F2" s="126"/>
+      <c r="G2" s="126"/>
       <c r="H2" s="5"/>
     </row>
     <row r="3" spans="1:8" s="6" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="C3" s="7"/>
-      <c r="D3" s="125"/>
-      <c r="E3" s="125"/>
-      <c r="F3" s="125"/>
-      <c r="G3" s="125"/>
+      <c r="D3" s="127"/>
+      <c r="E3" s="127"/>
+      <c r="F3" s="127"/>
+      <c r="G3" s="127"/>
       <c r="H3" s="8"/>
     </row>
     <row r="4" spans="1:8" s="6" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="C4" s="7"/>
-      <c r="D4" s="126"/>
-      <c r="E4" s="126"/>
-      <c r="F4" s="126"/>
-      <c r="G4" s="126"/>
+      <c r="D4" s="128"/>
+      <c r="E4" s="128"/>
+      <c r="F4" s="128"/>
+      <c r="G4" s="128"/>
       <c r="H4" s="8"/>
     </row>
-    <row r="5" spans="1:8" s="9" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" s="9" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="C5" s="10"/>
       <c r="D5" s="10"/>
@@ -2161,66 +2051,70 @@
     </row>
     <row r="6" spans="1:8" s="14" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
-      <c r="B6" s="127" t="s">
+      <c r="B6" s="129" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="127"/>
-      <c r="D6" s="127"/>
-      <c r="E6" s="127"/>
-      <c r="F6" s="127"/>
-      <c r="G6" s="127"/>
-    </row>
-    <row r="7" spans="1:8" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C6" s="129"/>
+      <c r="D6" s="129"/>
+      <c r="E6" s="129"/>
+      <c r="F6" s="129"/>
+      <c r="G6" s="129"/>
+    </row>
+    <row r="7" spans="1:8" s="14" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
-      <c r="B7" s="122" t="str">
+      <c r="B7" s="125" t="str">
         <f>data!B8</f>
-        <v>Nomor : 449.1/        /UKM/2023</v>
-      </c>
-      <c r="C7" s="122"/>
-      <c r="D7" s="122"/>
-      <c r="E7" s="122"/>
-      <c r="F7" s="122"/>
-      <c r="G7" s="122"/>
+        <v>Nomor : 449.1/        /UKM/2024</v>
+      </c>
+      <c r="C7" s="125"/>
+      <c r="D7" s="125"/>
+      <c r="E7" s="125"/>
+      <c r="F7" s="125"/>
+      <c r="G7" s="125"/>
     </row>
     <row r="8" spans="1:8" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="4"/>
-    </row>
-    <row r="9" spans="1:8" s="14" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C8" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" s="131" t="s">
+        <v>81</v>
+      </c>
+      <c r="F8" s="131"/>
+      <c r="G8" s="131"/>
+    </row>
+    <row r="9" spans="1:8" s="14" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
-      <c r="B9" s="128" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" s="128"/>
-      <c r="D9" s="128"/>
-      <c r="E9" s="128"/>
-      <c r="F9" s="128"/>
-      <c r="G9" s="128"/>
+      <c r="B9"/>
+      <c r="C9"/>
+      <c r="D9"/>
+      <c r="E9" s="131"/>
+      <c r="F9" s="131"/>
+      <c r="G9" s="131"/>
     </row>
     <row r="10" spans="1:8" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
-      <c r="B10" s="129"/>
-      <c r="C10" s="129"/>
-      <c r="D10" s="129"/>
-      <c r="E10" s="129"/>
-      <c r="F10" s="129"/>
-      <c r="G10" s="129"/>
+      <c r="B10" s="130"/>
+      <c r="C10" s="130"/>
+      <c r="D10" s="130"/>
+      <c r="E10" s="130"/>
+      <c r="F10" s="130"/>
+      <c r="G10" s="130"/>
     </row>
     <row r="11" spans="1:8" s="17" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="16"/>
-      <c r="B11" s="121" t="s">
+      <c r="B11" s="125" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="121"/>
-      <c r="D11" s="121"/>
-      <c r="E11" s="121"/>
-      <c r="F11" s="121"/>
-      <c r="G11" s="121"/>
+      <c r="C11" s="125"/>
+      <c r="D11" s="125"/>
+      <c r="E11" s="125"/>
+      <c r="F11" s="125"/>
+      <c r="G11" s="125"/>
     </row>
     <row r="12" spans="1:8" s="17" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="16"/>
@@ -2228,8 +2122,8 @@
       <c r="C12" s="16"/>
       <c r="D12" s="19"/>
       <c r="E12" s="20"/>
-      <c r="F12" s="121"/>
-      <c r="G12" s="121"/>
+      <c r="F12" s="125"/>
+      <c r="G12" s="125"/>
     </row>
     <row r="13" spans="1:8" s="17" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="16"/>
@@ -2242,12 +2136,12 @@
       <c r="D13" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="E13" s="105">
+      <c r="E13" s="81">
         <f>data!B1</f>
         <v>0</v>
       </c>
-      <c r="F13" s="121"/>
-      <c r="G13" s="121"/>
+      <c r="F13" s="125"/>
+      <c r="G13" s="125"/>
     </row>
     <row r="14" spans="1:8" s="17" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16"/>
@@ -2258,12 +2152,12 @@
       <c r="D14" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="E14" s="105">
+      <c r="E14" s="81">
         <f>data!B2</f>
         <v>0</v>
       </c>
-      <c r="F14" s="121"/>
-      <c r="G14" s="121"/>
+      <c r="F14" s="125"/>
+      <c r="G14" s="125"/>
     </row>
     <row r="15" spans="1:8" s="17" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="16"/>
@@ -2274,7 +2168,7 @@
       <c r="D15" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="E15" s="105">
+      <c r="E15" s="81">
         <f>data!B3</f>
         <v>0</v>
       </c>
@@ -2292,7 +2186,7 @@
       <c r="D16" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="E16" s="105">
+      <c r="E16" s="81">
         <f>data!B4</f>
         <v>0</v>
       </c>
@@ -2310,14 +2204,14 @@
       <c r="D17" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="E17" s="105">
+      <c r="E17" s="81">
         <f>data!C1</f>
         <v>0</v>
       </c>
-      <c r="F17" s="121" t="s">
+      <c r="F17" s="125" t="s">
         <v>10</v>
       </c>
-      <c r="G17" s="121"/>
+      <c r="G17" s="125"/>
     </row>
     <row r="18" spans="1:7" s="17" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="16"/>
@@ -2328,12 +2222,12 @@
       <c r="D18" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="E18" s="105">
+      <c r="E18" s="81">
         <f>data!C2</f>
         <v>0</v>
       </c>
-      <c r="F18" s="121"/>
-      <c r="G18" s="121"/>
+      <c r="F18" s="125"/>
+      <c r="G18" s="125"/>
     </row>
     <row r="19" spans="1:7" s="17" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="16"/>
@@ -2344,7 +2238,7 @@
       <c r="D19" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="E19" s="105">
+      <c r="E19" s="81">
         <f>data!C3</f>
         <v>0</v>
       </c>
@@ -2362,7 +2256,7 @@
       <c r="D20" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="E20" s="105">
+      <c r="E20" s="81">
         <f>data!C4</f>
         <v>0</v>
       </c>
@@ -2411,12 +2305,12 @@
       <c r="D24" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="E24" s="113">
+      <c r="E24" s="87">
         <f>data!B6</f>
         <v>0</v>
       </c>
       <c r="F24" s="20"/>
-      <c r="G24" s="107"/>
+      <c r="G24" s="82"/>
     </row>
     <row r="25" spans="1:7" s="14" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
@@ -2427,7 +2321,7 @@
       <c r="D25" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="E25" s="113">
+      <c r="E25" s="87">
         <f>data!B7</f>
         <v>0</v>
       </c>
@@ -2463,10 +2357,10 @@
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
       <c r="E28" s="27"/>
-      <c r="F28" s="122" t="s">
+      <c r="F28" s="133" t="s">
         <v>17</v>
       </c>
-      <c r="G28" s="122"/>
+      <c r="G28" s="133"/>
     </row>
     <row r="29" spans="1:7" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
@@ -2474,10 +2368,10 @@
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
       <c r="E29" s="27"/>
-      <c r="F29" s="122" t="s">
+      <c r="F29" s="133" t="s">
         <v>18</v>
       </c>
-      <c r="G29" s="122"/>
+      <c r="G29" s="133"/>
     </row>
     <row r="30" spans="1:7" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
@@ -2510,10 +2404,10 @@
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
       <c r="E33" s="27"/>
-      <c r="F33" s="123" t="s">
+      <c r="F33" s="134" t="s">
         <v>19</v>
       </c>
-      <c r="G33" s="123"/>
+      <c r="G33" s="134"/>
       <c r="H33" s="31"/>
     </row>
     <row r="34" spans="1:8" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -2522,10 +2416,10 @@
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
       <c r="E34" s="27"/>
-      <c r="F34" s="120" t="s">
+      <c r="F34" s="132" t="s">
         <v>20</v>
       </c>
-      <c r="G34" s="120"/>
+      <c r="G34" s="132"/>
       <c r="H34" s="32"/>
     </row>
     <row r="35" spans="1:8" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -2644,23 +2538,23 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="F33:G33"/>
     <mergeCell ref="F17:G17"/>
     <mergeCell ref="D2:G2"/>
     <mergeCell ref="D3:G3"/>
     <mergeCell ref="D4:G4"/>
     <mergeCell ref="B6:G6"/>
     <mergeCell ref="B7:G7"/>
-    <mergeCell ref="B9:G9"/>
     <mergeCell ref="B10:G10"/>
     <mergeCell ref="B11:G11"/>
     <mergeCell ref="F12:G12"/>
     <mergeCell ref="F13:G13"/>
     <mergeCell ref="F14:G14"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="E8:G9"/>
   </mergeCells>
   <pageMargins left="0.59055118110236227" right="0.39370078740157483" top="0.59055118110236227" bottom="1.7716535433070868" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="5" scale="86" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
@@ -2672,386 +2566,392 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K39"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A4" zoomScale="90" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21:B23"/>
+    <sheetView view="pageBreakPreview" zoomScale="90" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.85546875" style="5" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="5.140625" style="96" customWidth="1"/>
     <col min="3" max="3" width="40.7109375" style="5" customWidth="1"/>
     <col min="4" max="4" width="15.5703125" style="5" customWidth="1"/>
     <col min="5" max="5" width="24.85546875" style="5" customWidth="1"/>
     <col min="6" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C1" s="35" t="s">
+    <row r="1" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1"/>
+      <c r="B1" s="94"/>
+      <c r="C1"/>
+      <c r="D1"/>
+      <c r="E1"/>
+    </row>
+    <row r="2" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2"/>
+      <c r="B2" s="94"/>
+      <c r="C2"/>
+      <c r="D2"/>
+      <c r="E2"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3"/>
+      <c r="B3" s="94"/>
+      <c r="C3"/>
+      <c r="D3"/>
+      <c r="E3"/>
+    </row>
+    <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4"/>
+      <c r="B4" s="94"/>
+      <c r="C4"/>
+      <c r="D4"/>
+      <c r="E4"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5"/>
+      <c r="B5" s="94"/>
+      <c r="C5"/>
+      <c r="D5"/>
+      <c r="E5"/>
+    </row>
+    <row r="6" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="95"/>
+    </row>
+    <row r="7" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="152" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="152"/>
+      <c r="C7" s="152"/>
+      <c r="D7" s="152"/>
+      <c r="E7" s="152"/>
+      <c r="I7" s="35"/>
+    </row>
+    <row r="8" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="133" t="str">
+        <f>data!B8</f>
+        <v>Nomor : 449.1/        /UKM/2024</v>
+      </c>
+      <c r="B8" s="133"/>
+      <c r="C8" s="133"/>
+      <c r="D8" s="133"/>
+      <c r="E8" s="133"/>
+      <c r="I8" s="35"/>
+    </row>
+    <row r="9" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="36"/>
+      <c r="B9" s="92"/>
+      <c r="C9" s="36"/>
+      <c r="D9" s="36"/>
+      <c r="I9" s="35"/>
+    </row>
+    <row r="10" spans="1:11" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="89">
+        <v>1</v>
+      </c>
+      <c r="C10" s="99" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-    </row>
-    <row r="2" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="35" t="s">
+      <c r="D10" s="138" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-    </row>
-    <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.4">
-      <c r="C3" s="36" t="s">
+      <c r="E10" s="139"/>
+    </row>
+    <row r="11" spans="1:11" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="93">
+        <v>2</v>
+      </c>
+      <c r="C11" s="100" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-    </row>
-    <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-    </row>
-    <row r="5" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" s="38"/>
-      <c r="C5" s="38"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-    </row>
-    <row r="6" spans="1:11" ht="20.100000000000001" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="3"/>
-    </row>
-    <row r="7" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="130" t="s">
-        <v>29</v>
-      </c>
-      <c r="B7" s="130"/>
-      <c r="C7" s="130"/>
-      <c r="D7" s="130"/>
-      <c r="E7" s="130"/>
-      <c r="I7" s="39"/>
-    </row>
-    <row r="8" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="122" t="s">
-        <v>88</v>
-      </c>
-      <c r="B8" s="122"/>
-      <c r="C8" s="122"/>
-      <c r="D8" s="122"/>
-      <c r="E8" s="122"/>
-      <c r="I8" s="39"/>
-    </row>
-    <row r="9" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="40"/>
-      <c r="B9" s="40"/>
-      <c r="C9" s="40"/>
-      <c r="D9" s="40"/>
-      <c r="I9" s="39"/>
-    </row>
-    <row r="10" spans="1:11" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="41">
-        <v>1</v>
-      </c>
-      <c r="C10" s="42" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" s="131" t="s">
-        <v>31</v>
-      </c>
-      <c r="E10" s="132"/>
-    </row>
-    <row r="11" spans="1:11" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="43">
-        <v>2</v>
-      </c>
-      <c r="C11" s="44" t="s">
-        <v>32</v>
-      </c>
-      <c r="D11" s="45">
+      <c r="D11" s="101">
         <f>data!B1</f>
         <v>0</v>
       </c>
-      <c r="E11" s="46"/>
+      <c r="E11" s="102"/>
     </row>
     <row r="12" spans="1:11" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="43"/>
-      <c r="C12" s="44"/>
-      <c r="D12" s="119">
+      <c r="B12" s="93"/>
+      <c r="C12" s="100"/>
+      <c r="D12" s="103">
         <f>data!C1</f>
         <v>0</v>
       </c>
-      <c r="E12" s="114"/>
-      <c r="H12" s="39"/>
-      <c r="K12" s="39"/>
-    </row>
-    <row r="13" spans="1:11" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="49"/>
-      <c r="B13" s="164">
+      <c r="E12" s="104"/>
+      <c r="H12" s="35"/>
+      <c r="K12" s="35"/>
+    </row>
+    <row r="13" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="38"/>
+      <c r="B13" s="153">
         <v>3</v>
       </c>
-      <c r="C13" s="47" t="s">
-        <v>33</v>
-      </c>
-      <c r="D13" s="115">
+      <c r="C13" s="105" t="s">
+        <v>83</v>
+      </c>
+      <c r="D13" s="106">
         <f>data!B3</f>
         <v>0</v>
       </c>
-      <c r="E13" s="116"/>
-      <c r="H13" s="39"/>
-      <c r="K13" s="39"/>
+      <c r="E13" s="107"/>
+      <c r="H13" s="35"/>
+      <c r="K13" s="35"/>
     </row>
     <row r="14" spans="1:11" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="49"/>
-      <c r="B14" s="164"/>
-      <c r="C14" s="44" t="s">
-        <v>34</v>
-      </c>
-      <c r="D14" s="117">
+      <c r="A14" s="38"/>
+      <c r="B14" s="153"/>
+      <c r="C14" s="100" t="s">
+        <v>84</v>
+      </c>
+      <c r="D14" s="108">
         <f>data!C3</f>
         <v>0</v>
       </c>
-      <c r="E14" s="118"/>
-    </row>
-    <row r="15" spans="1:11" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="49"/>
-      <c r="B15" s="164"/>
-      <c r="C15" s="44" t="s">
-        <v>35</v>
-      </c>
-      <c r="D15" s="48">
+      <c r="E14" s="109"/>
+    </row>
+    <row r="15" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="38"/>
+      <c r="B15" s="154"/>
+      <c r="C15" s="100" t="s">
+        <v>85</v>
+      </c>
+      <c r="D15" s="110">
         <f>data!B4</f>
         <v>0</v>
       </c>
-      <c r="E15" s="49"/>
-    </row>
-    <row r="16" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="49"/>
-      <c r="B16" s="159"/>
-      <c r="C16" s="44" t="s">
-        <v>36</v>
-      </c>
-      <c r="D16" s="48">
-        <f>data!C4</f>
-        <v>0</v>
-      </c>
-      <c r="E16" s="50"/>
-      <c r="H16" s="39"/>
+      <c r="E15" s="111"/>
+    </row>
+    <row r="16" spans="1:11" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="38"/>
+      <c r="B16" s="97"/>
+      <c r="C16" s="100"/>
+      <c r="D16" s="110"/>
+      <c r="E16" s="111"/>
     </row>
     <row r="17" spans="1:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="49"/>
-      <c r="B17" s="165">
+      <c r="A17" s="38"/>
+      <c r="B17" s="91">
         <v>4</v>
       </c>
-      <c r="C17" s="42" t="s">
-        <v>37</v>
-      </c>
-      <c r="D17" s="100">
+      <c r="C17" s="99" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" s="112">
         <f>data!B6</f>
         <v>0</v>
       </c>
-      <c r="E17" s="106"/>
-      <c r="H17" s="39"/>
+      <c r="E17" s="113"/>
+      <c r="H17" s="35"/>
     </row>
     <row r="18" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="49"/>
-      <c r="B18" s="165">
+      <c r="A18" s="38"/>
+      <c r="B18" s="91">
         <v>5</v>
       </c>
-      <c r="C18" s="51" t="s">
-        <v>38</v>
-      </c>
-      <c r="D18" s="134" t="s">
-        <v>39</v>
-      </c>
-      <c r="E18" s="135"/>
-      <c r="H18" s="39"/>
+      <c r="C18" s="99" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" s="155" t="s">
+        <v>29</v>
+      </c>
+      <c r="E18" s="156"/>
+      <c r="H18" s="35"/>
     </row>
     <row r="19" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="49"/>
-      <c r="B19" s="164">
+      <c r="A19" s="38"/>
+      <c r="B19" s="141">
         <v>6</v>
       </c>
-      <c r="C19" s="47" t="s">
-        <v>40</v>
-      </c>
-      <c r="D19" s="136" t="s">
-        <v>41</v>
-      </c>
-      <c r="E19" s="137"/>
+      <c r="C19" s="114" t="s">
+        <v>86</v>
+      </c>
+      <c r="D19" s="138" t="s">
+        <v>30</v>
+      </c>
+      <c r="E19" s="139"/>
     </row>
     <row r="20" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="49"/>
-      <c r="B20" s="164"/>
-      <c r="C20" s="52" t="s">
-        <v>42</v>
-      </c>
-      <c r="D20" s="138">
+      <c r="A20" s="38"/>
+      <c r="B20" s="141"/>
+      <c r="C20" s="115" t="s">
+        <v>87</v>
+      </c>
+      <c r="D20" s="148">
         <f>data!B7</f>
         <v>0</v>
       </c>
-      <c r="E20" s="139"/>
+      <c r="E20" s="149"/>
     </row>
     <row r="21" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="49"/>
-      <c r="B21" s="164">
+      <c r="A21" s="38"/>
+      <c r="B21" s="141">
         <v>7</v>
       </c>
-      <c r="C21" s="47" t="s">
-        <v>43</v>
-      </c>
-      <c r="D21" s="136" t="s">
-        <v>44</v>
-      </c>
-      <c r="E21" s="137"/>
+      <c r="C21" s="114" t="s">
+        <v>88</v>
+      </c>
+      <c r="D21" s="138" t="s">
+        <v>31</v>
+      </c>
+      <c r="E21" s="139"/>
     </row>
     <row r="22" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="133"/>
-      <c r="C22" s="44" t="s">
-        <v>45</v>
-      </c>
-      <c r="D22" s="53"/>
-      <c r="E22" s="104"/>
+      <c r="B22" s="150"/>
+      <c r="C22" s="100" t="s">
+        <v>89</v>
+      </c>
+      <c r="D22" s="98"/>
+      <c r="E22" s="116"/>
     </row>
     <row r="23" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="49"/>
-      <c r="B23" s="159"/>
-      <c r="C23" s="44" t="s">
-        <v>46</v>
-      </c>
-      <c r="D23" s="53">
+      <c r="A23" s="38"/>
+      <c r="B23" s="151"/>
+      <c r="C23" s="100" t="s">
+        <v>90</v>
+      </c>
+      <c r="D23" s="98">
         <f>D22</f>
         <v>0</v>
       </c>
-      <c r="E23" s="108"/>
+      <c r="E23" s="117"/>
     </row>
     <row r="24" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="49"/>
-      <c r="B24" s="160">
+      <c r="A24" s="38"/>
+      <c r="B24" s="136">
         <v>8</v>
       </c>
-      <c r="C24" s="55" t="s">
-        <v>47</v>
-      </c>
-      <c r="D24" s="136" t="s">
+      <c r="C24" s="88" t="s">
+        <v>32</v>
+      </c>
+      <c r="D24" s="138" t="s">
         <v>6</v>
       </c>
-      <c r="E24" s="137"/>
+      <c r="E24" s="139"/>
     </row>
     <row r="25" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="49"/>
-      <c r="B25" s="161"/>
-      <c r="C25" s="48"/>
-      <c r="D25" s="56"/>
-      <c r="E25" s="49"/>
+      <c r="A25" s="38"/>
+      <c r="B25" s="137"/>
+      <c r="C25" s="110"/>
+      <c r="D25" s="118"/>
+      <c r="E25" s="111"/>
     </row>
     <row r="26" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="49"/>
-      <c r="B26" s="162"/>
-      <c r="C26" s="57" t="s">
-        <v>48</v>
-      </c>
-      <c r="D26" s="58" t="s">
-        <v>49</v>
-      </c>
-      <c r="E26" s="49"/>
+      <c r="A26" s="38"/>
+      <c r="B26" s="90"/>
+      <c r="C26" s="119" t="s">
+        <v>33</v>
+      </c>
+      <c r="D26" s="120" t="s">
+        <v>34</v>
+      </c>
+      <c r="E26" s="111"/>
     </row>
     <row r="27" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="49"/>
-      <c r="B27" s="163">
+      <c r="A27" s="38"/>
+      <c r="B27" s="140">
         <v>9</v>
       </c>
-      <c r="C27" s="59" t="s">
-        <v>50</v>
-      </c>
-      <c r="D27" s="141" t="s">
-        <v>51</v>
-      </c>
-      <c r="E27" s="142"/>
+      <c r="C27" s="121" t="s">
+        <v>35</v>
+      </c>
+      <c r="D27" s="142" t="s">
+        <v>36</v>
+      </c>
+      <c r="E27" s="143"/>
     </row>
     <row r="28" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="49"/>
-      <c r="B28" s="164"/>
-      <c r="C28" s="59" t="s">
-        <v>52</v>
-      </c>
-      <c r="D28" s="143" t="s">
-        <v>53</v>
-      </c>
-      <c r="E28" s="144"/>
+      <c r="A28" s="38"/>
+      <c r="B28" s="141"/>
+      <c r="C28" s="121" t="s">
+        <v>37</v>
+      </c>
+      <c r="D28" s="144" t="s">
+        <v>38</v>
+      </c>
+      <c r="E28" s="145"/>
     </row>
     <row r="29" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="49"/>
-      <c r="B29" s="164"/>
-      <c r="C29" s="60" t="s">
-        <v>54</v>
-      </c>
-      <c r="D29" s="145" t="s">
-        <v>55</v>
-      </c>
-      <c r="E29" s="146"/>
+      <c r="A29" s="38"/>
+      <c r="B29" s="141"/>
+      <c r="C29" s="122" t="s">
+        <v>39</v>
+      </c>
+      <c r="D29" s="146"/>
+      <c r="E29" s="147"/>
     </row>
     <row r="30" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="61">
+      <c r="B30" s="89">
         <v>10</v>
       </c>
-      <c r="C30" s="62" t="s">
-        <v>56</v>
-      </c>
-      <c r="D30" s="42"/>
-      <c r="E30" s="63"/>
+      <c r="C30" s="123" t="s">
+        <v>40</v>
+      </c>
+      <c r="D30" s="99"/>
+      <c r="E30" s="124"/>
     </row>
     <row r="31" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="32" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D32" s="64" t="s">
-        <v>57</v>
+      <c r="D32" s="40" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="33" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D33" s="65" t="s">
-        <v>58</v>
-      </c>
-      <c r="E33" s="54">
+      <c r="D33" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="E33" s="39">
         <f>D22</f>
         <v>0</v>
       </c>
-      <c r="F33" s="104"/>
+      <c r="F33" s="80"/>
     </row>
     <row r="34" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="33"/>
+      <c r="B34" s="92"/>
       <c r="C34" s="33"/>
-      <c r="D34" s="140" t="s">
-        <v>31</v>
-      </c>
-      <c r="E34" s="140"/>
+      <c r="D34" s="135" t="s">
+        <v>25</v>
+      </c>
+      <c r="E34" s="135"/>
     </row>
     <row r="35" spans="2:6" s="33" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D35" s="66"/>
+      <c r="B35" s="92"/>
+      <c r="D35" s="42"/>
     </row>
     <row r="36" spans="2:6" s="33" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D36" s="66"/>
+      <c r="B36" s="92"/>
+      <c r="D36" s="42"/>
     </row>
     <row r="37" spans="2:6" s="33" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D37" s="66"/>
+      <c r="B37" s="92"/>
+      <c r="D37" s="42"/>
     </row>
     <row r="38" spans="2:6" s="33" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D38" s="123" t="s">
+      <c r="B38" s="92"/>
+      <c r="D38" s="134" t="s">
         <v>19</v>
       </c>
-      <c r="E38" s="123"/>
+      <c r="E38" s="134"/>
     </row>
     <row r="39" spans="2:6" s="33" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D39" s="120" t="s">
+      <c r="B39" s="92"/>
+      <c r="D39" s="132" t="s">
         <v>20</v>
       </c>
-      <c r="E39" s="120"/>
+      <c r="E39" s="132"/>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="A7:E7"/>
+    <mergeCell ref="A8:E8"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="D21:E21"/>
     <mergeCell ref="D34:E34"/>
     <mergeCell ref="D38:E38"/>
     <mergeCell ref="D39:E39"/>
@@ -3061,16 +2961,6 @@
     <mergeCell ref="D27:E27"/>
     <mergeCell ref="D28:E28"/>
     <mergeCell ref="D29:E29"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="B21:B23"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="A7:E7"/>
-    <mergeCell ref="A8:E8"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="B13:B16"/>
-    <mergeCell ref="D18:E18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.45" top="0.25" bottom="1.5" header="0.3" footer="0.3"/>
   <pageSetup paperSize="5" scale="92" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
@@ -3082,8 +2972,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:G82"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="86" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7:D7"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A49" zoomScale="86" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3105,553 +2995,553 @@
     <row r="3" spans="2:7" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="2:7" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="33" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="2:7" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E5" s="33" t="str">
         <f>data!B8</f>
-        <v>Nomor : 449.1/        /UKM/2023</v>
+        <v>Nomor : 449.1/        /UKM/2024</v>
       </c>
     </row>
     <row r="6" spans="2:7" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E6" s="64" t="s">
-        <v>60</v>
+      <c r="E6" s="40" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="2:7" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E7" s="64" t="s">
-        <v>89</v>
-      </c>
-      <c r="F7" s="67"/>
+      <c r="E7" s="40" t="s">
+        <v>72</v>
+      </c>
+      <c r="F7" s="43"/>
     </row>
     <row r="8" spans="2:7" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="68"/>
-      <c r="D8" s="68"/>
-      <c r="E8" s="64" t="s">
-        <v>61</v>
-      </c>
-      <c r="F8" s="150">
+      <c r="C8" s="44"/>
+      <c r="D8" s="44"/>
+      <c r="E8" s="40" t="s">
+        <v>45</v>
+      </c>
+      <c r="F8" s="165">
         <f>data!B7</f>
         <v>0</v>
       </c>
-      <c r="G8" s="150"/>
+      <c r="G8" s="165"/>
     </row>
     <row r="9" spans="2:7" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E9" s="69"/>
+      <c r="E9" s="45"/>
     </row>
     <row r="10" spans="2:7" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E10" s="66"/>
+      <c r="E10" s="42"/>
     </row>
     <row r="11" spans="2:7" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="70" t="s">
-        <v>62</v>
-      </c>
-      <c r="C11" s="71" t="s">
-        <v>63</v>
-      </c>
-      <c r="D11" s="71"/>
-      <c r="E11" s="72" t="s">
-        <v>64</v>
-      </c>
-      <c r="F11" s="73"/>
+      <c r="B11" s="46" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" s="47" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" s="47"/>
+      <c r="E11" s="48" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" s="49"/>
     </row>
     <row r="12" spans="2:7" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="74"/>
-      <c r="C12" s="151">
+      <c r="B12" s="50"/>
+      <c r="C12" s="166">
         <f>F8</f>
         <v>0</v>
       </c>
-      <c r="D12" s="151"/>
-      <c r="E12" s="152">
+      <c r="D12" s="166"/>
+      <c r="E12" s="167">
         <f>C12</f>
         <v>0</v>
       </c>
-      <c r="F12" s="153"/>
+      <c r="F12" s="168"/>
     </row>
     <row r="13" spans="2:7" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="74"/>
-      <c r="C13" s="64" t="str">
+      <c r="B13" s="50"/>
+      <c r="C13" s="40" t="str">
         <f>E7</f>
         <v>Pada Tanggal</v>
       </c>
-      <c r="D13" s="67">
+      <c r="D13" s="43">
         <f>F7</f>
         <v>0</v>
       </c>
-      <c r="E13" s="48" t="str">
+      <c r="E13" s="37" t="str">
         <f>E7</f>
         <v>Pada Tanggal</v>
       </c>
-      <c r="F13" s="75">
+      <c r="F13" s="51">
         <f>D13</f>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="2:7" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="74"/>
-      <c r="C14" s="64"/>
-      <c r="D14" s="64"/>
-      <c r="E14" s="48" t="s">
-        <v>65</v>
-      </c>
-      <c r="F14" s="76"/>
+      <c r="B14" s="50"/>
+      <c r="C14" s="40"/>
+      <c r="D14" s="40"/>
+      <c r="E14" s="37" t="s">
+        <v>49</v>
+      </c>
+      <c r="F14" s="52"/>
     </row>
     <row r="15" spans="2:7" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="74"/>
-      <c r="C15" s="140" t="s">
-        <v>66</v>
-      </c>
-      <c r="D15" s="140"/>
-      <c r="E15" s="154" t="s">
-        <v>66</v>
-      </c>
-      <c r="F15" s="155"/>
+      <c r="B15" s="50"/>
+      <c r="C15" s="135" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15" s="135"/>
+      <c r="E15" s="163" t="s">
+        <v>50</v>
+      </c>
+      <c r="F15" s="162"/>
     </row>
     <row r="16" spans="2:7" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="74"/>
-      <c r="E16" s="48"/>
-      <c r="F16" s="77"/>
+      <c r="B16" s="50"/>
+      <c r="E16" s="37"/>
+      <c r="F16" s="53"/>
     </row>
     <row r="17" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="74"/>
+      <c r="B17" s="50"/>
       <c r="D17" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="E17" s="48"/>
-      <c r="F17" s="77"/>
+      <c r="E17" s="37"/>
+      <c r="F17" s="53"/>
     </row>
     <row r="18" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="74"/>
-      <c r="E18" s="48"/>
-      <c r="F18" s="77"/>
+      <c r="B18" s="50"/>
+      <c r="E18" s="37"/>
+      <c r="F18" s="53"/>
     </row>
     <row r="19" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="74"/>
-      <c r="C19" s="147" t="s">
-        <v>67</v>
-      </c>
-      <c r="D19" s="147"/>
-      <c r="E19" s="148" t="s">
-        <v>67</v>
-      </c>
-      <c r="F19" s="149"/>
+      <c r="B19" s="50"/>
+      <c r="C19" s="157" t="s">
+        <v>51</v>
+      </c>
+      <c r="D19" s="157"/>
+      <c r="E19" s="164" t="s">
+        <v>51</v>
+      </c>
+      <c r="F19" s="161"/>
     </row>
     <row r="20" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="78"/>
-      <c r="C20" s="79" t="s">
-        <v>68</v>
-      </c>
-      <c r="D20" s="80"/>
-      <c r="E20" s="81" t="s">
-        <v>68</v>
-      </c>
-      <c r="F20" s="82"/>
+      <c r="B20" s="54"/>
+      <c r="C20" s="55" t="s">
+        <v>52</v>
+      </c>
+      <c r="D20" s="56"/>
+      <c r="E20" s="57" t="s">
+        <v>52</v>
+      </c>
+      <c r="F20" s="58"/>
     </row>
     <row r="21" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="70" t="s">
-        <v>69</v>
-      </c>
-      <c r="C21" s="71"/>
-      <c r="D21" s="73"/>
-      <c r="E21" s="72" t="s">
-        <v>64</v>
-      </c>
-      <c r="F21" s="73"/>
+      <c r="B21" s="46" t="s">
+        <v>53</v>
+      </c>
+      <c r="C21" s="47"/>
+      <c r="D21" s="49"/>
+      <c r="E21" s="48" t="s">
+        <v>48</v>
+      </c>
+      <c r="F21" s="49"/>
     </row>
     <row r="22" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="74"/>
-      <c r="C22" s="64" t="s">
-        <v>70</v>
-      </c>
-      <c r="D22" s="83">
+      <c r="B22" s="50"/>
+      <c r="C22" s="40" t="s">
+        <v>54</v>
+      </c>
+      <c r="D22" s="59">
         <f>C12</f>
         <v>0</v>
       </c>
-      <c r="E22" s="111" t="s">
-        <v>70</v>
-      </c>
-      <c r="F22" s="84"/>
+      <c r="E22" s="85" t="s">
+        <v>54</v>
+      </c>
+      <c r="F22" s="60"/>
     </row>
     <row r="23" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="74"/>
-      <c r="C23" s="64" t="s">
-        <v>71</v>
-      </c>
-      <c r="D23" s="85"/>
-      <c r="E23" s="48" t="s">
-        <v>71</v>
-      </c>
-      <c r="F23" s="85"/>
+      <c r="B23" s="50"/>
+      <c r="C23" s="40" t="s">
+        <v>55</v>
+      </c>
+      <c r="D23" s="61"/>
+      <c r="E23" s="37" t="s">
+        <v>55</v>
+      </c>
+      <c r="F23" s="61"/>
     </row>
     <row r="24" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="74"/>
-      <c r="C24" s="64"/>
-      <c r="D24" s="76"/>
-      <c r="E24" s="48" t="s">
-        <v>72</v>
-      </c>
-      <c r="F24" s="76"/>
+      <c r="B24" s="50"/>
+      <c r="C24" s="40"/>
+      <c r="D24" s="52"/>
+      <c r="E24" s="37" t="s">
+        <v>56</v>
+      </c>
+      <c r="F24" s="52"/>
     </row>
     <row r="25" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="74"/>
-      <c r="C25" s="140" t="s">
-        <v>66</v>
-      </c>
-      <c r="D25" s="155"/>
-      <c r="E25" s="154" t="s">
-        <v>66</v>
-      </c>
-      <c r="F25" s="155"/>
+      <c r="B25" s="50"/>
+      <c r="C25" s="135" t="s">
+        <v>50</v>
+      </c>
+      <c r="D25" s="162"/>
+      <c r="E25" s="163" t="s">
+        <v>50</v>
+      </c>
+      <c r="F25" s="162"/>
     </row>
     <row r="26" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="74"/>
-      <c r="D26" s="77"/>
-      <c r="E26" s="48"/>
-      <c r="F26" s="77"/>
+      <c r="B26" s="50"/>
+      <c r="D26" s="53"/>
+      <c r="E26" s="37"/>
+      <c r="F26" s="53"/>
     </row>
     <row r="27" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="74"/>
-      <c r="D27" s="77"/>
-      <c r="E27" s="48"/>
-      <c r="F27" s="77"/>
+      <c r="B27" s="50"/>
+      <c r="D27" s="53"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="53"/>
     </row>
     <row r="28" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="74"/>
-      <c r="D28" s="77"/>
-      <c r="E28" s="48"/>
-      <c r="F28" s="77"/>
+      <c r="B28" s="50"/>
+      <c r="D28" s="53"/>
+      <c r="E28" s="37"/>
+      <c r="F28" s="53"/>
     </row>
     <row r="29" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="74"/>
-      <c r="C29" s="147" t="s">
-        <v>67</v>
-      </c>
-      <c r="D29" s="149"/>
-      <c r="E29" s="147" t="s">
-        <v>67</v>
-      </c>
-      <c r="F29" s="149"/>
+      <c r="B29" s="50"/>
+      <c r="C29" s="157" t="s">
+        <v>51</v>
+      </c>
+      <c r="D29" s="161"/>
+      <c r="E29" s="157" t="s">
+        <v>51</v>
+      </c>
+      <c r="F29" s="161"/>
     </row>
     <row r="30" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="78"/>
-      <c r="C30" s="79" t="s">
-        <v>68</v>
-      </c>
-      <c r="D30" s="82"/>
-      <c r="E30" s="81" t="s">
-        <v>68</v>
-      </c>
-      <c r="F30" s="82"/>
+      <c r="B30" s="54"/>
+      <c r="C30" s="55" t="s">
+        <v>52</v>
+      </c>
+      <c r="D30" s="58"/>
+      <c r="E30" s="57" t="s">
+        <v>52</v>
+      </c>
+      <c r="F30" s="58"/>
     </row>
     <row r="31" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="70" t="s">
-        <v>73</v>
-      </c>
-      <c r="C31" s="71"/>
-      <c r="D31" s="73"/>
-      <c r="E31" s="72" t="s">
-        <v>64</v>
-      </c>
-      <c r="F31" s="73"/>
+      <c r="B31" s="46" t="s">
+        <v>57</v>
+      </c>
+      <c r="C31" s="47"/>
+      <c r="D31" s="49"/>
+      <c r="E31" s="48" t="s">
+        <v>48</v>
+      </c>
+      <c r="F31" s="49"/>
     </row>
     <row r="32" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="74"/>
-      <c r="C32" s="64" t="s">
-        <v>74</v>
-      </c>
-      <c r="D32" s="87"/>
-      <c r="E32" s="110" t="s">
-        <v>74</v>
-      </c>
-      <c r="F32" s="88"/>
+      <c r="B32" s="50"/>
+      <c r="C32" s="40" t="s">
+        <v>58</v>
+      </c>
+      <c r="D32" s="63"/>
+      <c r="E32" s="84" t="s">
+        <v>58</v>
+      </c>
+      <c r="F32" s="64"/>
     </row>
     <row r="33" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="74"/>
-      <c r="C33" s="64" t="s">
-        <v>71</v>
-      </c>
-      <c r="D33" s="89"/>
-      <c r="E33" s="109" t="s">
-        <v>71</v>
-      </c>
-      <c r="F33" s="89"/>
+      <c r="B33" s="50"/>
+      <c r="C33" s="40" t="s">
+        <v>55</v>
+      </c>
+      <c r="D33" s="65"/>
+      <c r="E33" s="83" t="s">
+        <v>55</v>
+      </c>
+      <c r="F33" s="65"/>
     </row>
     <row r="34" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="74"/>
-      <c r="C34" s="64"/>
-      <c r="E34" s="48" t="s">
-        <v>72</v>
-      </c>
-      <c r="F34" s="90"/>
+      <c r="B34" s="50"/>
+      <c r="C34" s="40"/>
+      <c r="E34" s="37" t="s">
+        <v>56</v>
+      </c>
+      <c r="F34" s="66"/>
     </row>
     <row r="35" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="74"/>
-      <c r="C35" s="140" t="s">
-        <v>66</v>
-      </c>
-      <c r="D35" s="155"/>
-      <c r="E35" s="154" t="s">
-        <v>66</v>
-      </c>
-      <c r="F35" s="155"/>
+      <c r="B35" s="50"/>
+      <c r="C35" s="135" t="s">
+        <v>50</v>
+      </c>
+      <c r="D35" s="162"/>
+      <c r="E35" s="163" t="s">
+        <v>50</v>
+      </c>
+      <c r="F35" s="162"/>
     </row>
     <row r="36" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="74"/>
-      <c r="D36" s="77"/>
-      <c r="E36" s="48"/>
-      <c r="F36" s="77"/>
+      <c r="B36" s="50"/>
+      <c r="D36" s="53"/>
+      <c r="E36" s="37"/>
+      <c r="F36" s="53"/>
     </row>
     <row r="37" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="74"/>
-      <c r="D37" s="77"/>
-      <c r="E37" s="48"/>
-      <c r="F37" s="77"/>
+      <c r="B37" s="50"/>
+      <c r="D37" s="53"/>
+      <c r="E37" s="37"/>
+      <c r="F37" s="53"/>
     </row>
     <row r="38" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="74"/>
-      <c r="D38" s="77"/>
-      <c r="E38" s="48"/>
-      <c r="F38" s="77"/>
+      <c r="B38" s="50"/>
+      <c r="D38" s="53"/>
+      <c r="E38" s="37"/>
+      <c r="F38" s="53"/>
     </row>
     <row r="39" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="74"/>
-      <c r="C39" s="147" t="s">
-        <v>67</v>
-      </c>
-      <c r="D39" s="149"/>
-      <c r="E39" s="147" t="s">
-        <v>67</v>
-      </c>
-      <c r="F39" s="149"/>
+      <c r="B39" s="50"/>
+      <c r="C39" s="157" t="s">
+        <v>51</v>
+      </c>
+      <c r="D39" s="161"/>
+      <c r="E39" s="157" t="s">
+        <v>51</v>
+      </c>
+      <c r="F39" s="161"/>
     </row>
     <row r="40" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="78"/>
-      <c r="C40" s="79" t="s">
-        <v>68</v>
-      </c>
-      <c r="D40" s="82"/>
-      <c r="E40" s="81" t="s">
-        <v>68</v>
-      </c>
-      <c r="F40" s="82"/>
+      <c r="B40" s="54"/>
+      <c r="C40" s="55" t="s">
+        <v>52</v>
+      </c>
+      <c r="D40" s="58"/>
+      <c r="E40" s="57" t="s">
+        <v>52</v>
+      </c>
+      <c r="F40" s="58"/>
     </row>
     <row r="41" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="70" t="s">
-        <v>75</v>
-      </c>
-      <c r="C41" s="71"/>
-      <c r="D41" s="73"/>
-      <c r="E41" s="72" t="s">
-        <v>64</v>
-      </c>
-      <c r="F41" s="73"/>
+      <c r="B41" s="46" t="s">
+        <v>59</v>
+      </c>
+      <c r="C41" s="47"/>
+      <c r="D41" s="49"/>
+      <c r="E41" s="48" t="s">
+        <v>48</v>
+      </c>
+      <c r="F41" s="49"/>
     </row>
     <row r="42" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="74"/>
-      <c r="C42" s="64" t="s">
-        <v>74</v>
-      </c>
-      <c r="D42" s="91"/>
-      <c r="E42" s="92"/>
-      <c r="F42" s="93"/>
+      <c r="B42" s="50"/>
+      <c r="C42" s="40" t="s">
+        <v>58</v>
+      </c>
+      <c r="D42" s="67"/>
+      <c r="E42" s="68"/>
+      <c r="F42" s="69"/>
     </row>
     <row r="43" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="74"/>
-      <c r="C43" s="64" t="s">
-        <v>71</v>
-      </c>
-      <c r="D43" s="85"/>
-      <c r="E43" s="86"/>
-      <c r="F43" s="85"/>
+      <c r="B43" s="50"/>
+      <c r="C43" s="40" t="s">
+        <v>55</v>
+      </c>
+      <c r="D43" s="61"/>
+      <c r="E43" s="62"/>
+      <c r="F43" s="61"/>
     </row>
     <row r="44" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="74"/>
-      <c r="C44" s="64"/>
-      <c r="E44" s="48" t="s">
-        <v>72</v>
-      </c>
-      <c r="F44" s="90"/>
+      <c r="B44" s="50"/>
+      <c r="C44" s="40"/>
+      <c r="E44" s="37" t="s">
+        <v>56</v>
+      </c>
+      <c r="F44" s="66"/>
     </row>
     <row r="45" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="74"/>
-      <c r="C45" s="140" t="s">
-        <v>66</v>
-      </c>
-      <c r="D45" s="155"/>
-      <c r="E45" s="154" t="s">
-        <v>66</v>
-      </c>
-      <c r="F45" s="155"/>
+      <c r="B45" s="50"/>
+      <c r="C45" s="135" t="s">
+        <v>50</v>
+      </c>
+      <c r="D45" s="162"/>
+      <c r="E45" s="163" t="s">
+        <v>50</v>
+      </c>
+      <c r="F45" s="162"/>
     </row>
     <row r="46" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="74"/>
-      <c r="D46" s="77"/>
-      <c r="E46" s="48"/>
-      <c r="F46" s="77"/>
+      <c r="B46" s="50"/>
+      <c r="D46" s="53"/>
+      <c r="E46" s="37"/>
+      <c r="F46" s="53"/>
     </row>
     <row r="47" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="74"/>
-      <c r="D47" s="77"/>
-      <c r="E47" s="48"/>
-      <c r="F47" s="77"/>
+      <c r="B47" s="50"/>
+      <c r="D47" s="53"/>
+      <c r="E47" s="37"/>
+      <c r="F47" s="53"/>
     </row>
     <row r="48" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="74"/>
-      <c r="D48" s="77"/>
-      <c r="E48" s="48"/>
-      <c r="F48" s="77"/>
+      <c r="B48" s="50"/>
+      <c r="D48" s="53"/>
+      <c r="E48" s="37"/>
+      <c r="F48" s="53"/>
     </row>
     <row r="49" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="74"/>
-      <c r="C49" s="147" t="s">
-        <v>67</v>
-      </c>
-      <c r="D49" s="149"/>
-      <c r="E49" s="148" t="s">
-        <v>67</v>
-      </c>
-      <c r="F49" s="149"/>
+      <c r="B49" s="50"/>
+      <c r="C49" s="157" t="s">
+        <v>51</v>
+      </c>
+      <c r="D49" s="161"/>
+      <c r="E49" s="164" t="s">
+        <v>51</v>
+      </c>
+      <c r="F49" s="161"/>
     </row>
     <row r="50" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="78"/>
-      <c r="C50" s="79" t="s">
-        <v>68</v>
-      </c>
-      <c r="D50" s="82"/>
-      <c r="E50" s="81" t="s">
-        <v>68</v>
-      </c>
-      <c r="F50" s="82"/>
+      <c r="B50" s="54"/>
+      <c r="C50" s="55" t="s">
+        <v>52</v>
+      </c>
+      <c r="D50" s="58"/>
+      <c r="E50" s="57" t="s">
+        <v>52</v>
+      </c>
+      <c r="F50" s="58"/>
     </row>
     <row r="51" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="74" t="s">
-        <v>76</v>
-      </c>
-      <c r="C51" s="94" t="s">
-        <v>77</v>
-      </c>
-      <c r="D51" s="94"/>
-      <c r="E51" s="94"/>
-      <c r="F51" s="95"/>
+      <c r="B51" s="50" t="s">
+        <v>60</v>
+      </c>
+      <c r="C51" s="70" t="s">
+        <v>61</v>
+      </c>
+      <c r="D51" s="70"/>
+      <c r="E51" s="70"/>
+      <c r="F51" s="71"/>
     </row>
     <row r="52" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="74"/>
+      <c r="B52" s="50"/>
       <c r="C52" s="33" t="s">
-        <v>78</v>
-      </c>
-      <c r="F52" s="77"/>
+        <v>62</v>
+      </c>
+      <c r="F52" s="53"/>
     </row>
     <row r="53" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="74"/>
+      <c r="B53" s="50"/>
       <c r="C53" s="33" t="s">
-        <v>79</v>
-      </c>
-      <c r="F53" s="96"/>
+        <v>63</v>
+      </c>
+      <c r="F53" s="72"/>
     </row>
     <row r="54" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="74"/>
-      <c r="C54" s="147"/>
-      <c r="D54" s="147"/>
-      <c r="E54" s="147"/>
-      <c r="F54" s="97"/>
+      <c r="B54" s="50"/>
+      <c r="C54" s="157"/>
+      <c r="D54" s="157"/>
+      <c r="E54" s="157"/>
+      <c r="F54" s="73"/>
     </row>
     <row r="55" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="74"/>
-      <c r="F55" s="77"/>
+      <c r="B55" s="50"/>
+      <c r="F55" s="53"/>
     </row>
     <row r="56" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="74"/>
-      <c r="C56" s="122" t="s">
-        <v>31</v>
-      </c>
-      <c r="D56" s="122"/>
-      <c r="E56" s="122"/>
-      <c r="F56" s="156"/>
+      <c r="B56" s="50"/>
+      <c r="C56" s="133" t="s">
+        <v>25</v>
+      </c>
+      <c r="D56" s="133"/>
+      <c r="E56" s="133"/>
+      <c r="F56" s="158"/>
     </row>
     <row r="57" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="74"/>
+      <c r="B57" s="50"/>
       <c r="C57" s="3"/>
       <c r="D57" s="3"/>
       <c r="E57" s="15"/>
-      <c r="F57" s="98"/>
+      <c r="F57" s="74"/>
     </row>
     <row r="58" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="74"/>
+      <c r="B58" s="50"/>
       <c r="C58" s="3"/>
       <c r="D58" s="3"/>
       <c r="E58" s="3"/>
-      <c r="F58" s="98"/>
+      <c r="F58" s="74"/>
     </row>
     <row r="59" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="74"/>
+      <c r="B59" s="50"/>
       <c r="C59" s="3"/>
       <c r="D59" s="3"/>
       <c r="E59" s="3"/>
-      <c r="F59" s="98"/>
+      <c r="F59" s="74"/>
     </row>
     <row r="60" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="74"/>
-      <c r="C60" s="157" t="s">
+      <c r="B60" s="50"/>
+      <c r="C60" s="159" t="s">
         <v>19</v>
       </c>
-      <c r="D60" s="157"/>
-      <c r="E60" s="157"/>
-      <c r="F60" s="158"/>
+      <c r="D60" s="159"/>
+      <c r="E60" s="159"/>
+      <c r="F60" s="160"/>
     </row>
     <row r="61" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="74"/>
-      <c r="C61" s="122" t="s">
+      <c r="B61" s="50"/>
+      <c r="C61" s="133" t="s">
         <v>20</v>
       </c>
-      <c r="D61" s="122"/>
-      <c r="E61" s="122"/>
-      <c r="F61" s="156"/>
+      <c r="D61" s="133"/>
+      <c r="E61" s="133"/>
+      <c r="F61" s="158"/>
     </row>
     <row r="62" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="78"/>
-      <c r="C62" s="79"/>
-      <c r="D62" s="79"/>
-      <c r="E62" s="79"/>
-      <c r="F62" s="99"/>
+      <c r="B62" s="54"/>
+      <c r="C62" s="55"/>
+      <c r="D62" s="55"/>
+      <c r="E62" s="55"/>
+      <c r="F62" s="75"/>
     </row>
     <row r="63" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="100" t="s">
-        <v>80</v>
-      </c>
-      <c r="C63" s="101" t="s">
-        <v>81</v>
-      </c>
-      <c r="D63" s="101"/>
-      <c r="E63" s="102"/>
-      <c r="F63" s="103"/>
+      <c r="B63" s="76" t="s">
+        <v>64</v>
+      </c>
+      <c r="C63" s="77" t="s">
+        <v>65</v>
+      </c>
+      <c r="D63" s="77"/>
+      <c r="E63" s="78"/>
+      <c r="F63" s="79"/>
     </row>
     <row r="64" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B64" s="33" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
     </row>
     <row r="65" spans="2:3" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B65" s="33" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="C65" s="33" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
     </row>
     <row r="66" spans="2:3" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C66" s="33" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
     </row>
     <row r="67" spans="2:3" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C67" s="33" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
     </row>
     <row r="68" spans="2:3" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C68" s="33" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
     </row>
     <row r="69" spans="2:3" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3665,7 +3555,7 @@
     <row r="77" spans="2:3" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="78" spans="2:3" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C78" s="33" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
     </row>
     <row r="79" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3674,6 +3564,19 @@
     <row r="82" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="E35:F35"/>
     <mergeCell ref="C54:E54"/>
     <mergeCell ref="C56:F56"/>
     <mergeCell ref="C60:F60"/>
@@ -3684,19 +3587,6 @@
     <mergeCell ref="E45:F45"/>
     <mergeCell ref="C49:D49"/>
     <mergeCell ref="E49:F49"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="E15:F15"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.43307086614173229" top="0.23622047244094491" bottom="1.4960629921259843" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="5" scale="86" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
refactor: fix missing border
</commit_message>
<xml_diff>
--- a/src/assets/sppd.xlsx
+++ b/src/assets/sppd.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B25FD93B-D5C1-46DE-98E9-EC463EE860CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8EBAA5C-CF54-4492-AC46-96295D073A32}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="94">
   <si>
     <t>SURAT TUGAS</t>
   </si>
@@ -205,12 +205,6 @@
     <t>`</t>
   </si>
   <si>
-    <t>Berangkat dari UPTD Puskesmas Lerep</t>
-  </si>
-  <si>
-    <t>Ke                     :</t>
-  </si>
-  <si>
     <t>I</t>
   </si>
   <si>
@@ -478,6 +472,18 @@
   </si>
   <si>
     <t>Nomor : 449.1/        /UKM/2024</t>
+  </si>
+  <si>
+    <t>Nomor</t>
+  </si>
+  <si>
+    <t>: UPTD Puskesmas Lerep</t>
+  </si>
+  <si>
+    <t>Ke</t>
+  </si>
+  <si>
+    <t>: 449.1/        /UKM/2024</t>
   </si>
 </sst>
 </file>
@@ -1004,7 +1010,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="169">
+  <cellXfs count="168">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1289,9 +1295,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1934,46 +1937,46 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B5" s="86"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -2016,28 +2019,28 @@
     <row r="2" spans="1:8" s="6" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="C2" s="7"/>
-      <c r="D2" s="126"/>
-      <c r="E2" s="126"/>
-      <c r="F2" s="126"/>
-      <c r="G2" s="126"/>
+      <c r="D2" s="125"/>
+      <c r="E2" s="125"/>
+      <c r="F2" s="125"/>
+      <c r="G2" s="125"/>
       <c r="H2" s="5"/>
     </row>
     <row r="3" spans="1:8" s="6" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="C3" s="7"/>
-      <c r="D3" s="127"/>
-      <c r="E3" s="127"/>
-      <c r="F3" s="127"/>
-      <c r="G3" s="127"/>
+      <c r="D3" s="126"/>
+      <c r="E3" s="126"/>
+      <c r="F3" s="126"/>
+      <c r="G3" s="126"/>
       <c r="H3" s="8"/>
     </row>
     <row r="4" spans="1:8" s="6" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="C4" s="7"/>
-      <c r="D4" s="128"/>
-      <c r="E4" s="128"/>
-      <c r="F4" s="128"/>
-      <c r="G4" s="128"/>
+      <c r="D4" s="127"/>
+      <c r="E4" s="127"/>
+      <c r="F4" s="127"/>
+      <c r="G4" s="127"/>
       <c r="H4" s="8"/>
     </row>
     <row r="5" spans="1:8" s="9" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2051,70 +2054,70 @@
     </row>
     <row r="6" spans="1:8" s="14" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
-      <c r="B6" s="129" t="s">
+      <c r="B6" s="128" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="129"/>
-      <c r="D6" s="129"/>
-      <c r="E6" s="129"/>
-      <c r="F6" s="129"/>
-      <c r="G6" s="129"/>
+      <c r="C6" s="128"/>
+      <c r="D6" s="128"/>
+      <c r="E6" s="128"/>
+      <c r="F6" s="128"/>
+      <c r="G6" s="128"/>
     </row>
     <row r="7" spans="1:8" s="14" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
-      <c r="B7" s="125" t="str">
+      <c r="B7" s="124" t="str">
         <f>data!B8</f>
         <v>Nomor : 449.1/        /UKM/2024</v>
       </c>
-      <c r="C7" s="125"/>
-      <c r="D7" s="125"/>
-      <c r="E7" s="125"/>
-      <c r="F7" s="125"/>
-      <c r="G7" s="125"/>
+      <c r="C7" s="124"/>
+      <c r="D7" s="124"/>
+      <c r="E7" s="124"/>
+      <c r="F7" s="124"/>
+      <c r="G7" s="124"/>
     </row>
     <row r="8" spans="1:8" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="131" t="s">
-        <v>81</v>
-      </c>
-      <c r="F8" s="131"/>
-      <c r="G8" s="131"/>
+      <c r="E8" s="130" t="s">
+        <v>79</v>
+      </c>
+      <c r="F8" s="130"/>
+      <c r="G8" s="130"/>
     </row>
     <row r="9" spans="1:8" s="14" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9"/>
       <c r="C9"/>
       <c r="D9"/>
-      <c r="E9" s="131"/>
-      <c r="F9" s="131"/>
-      <c r="G9" s="131"/>
+      <c r="E9" s="130"/>
+      <c r="F9" s="130"/>
+      <c r="G9" s="130"/>
     </row>
     <row r="10" spans="1:8" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
-      <c r="B10" s="130"/>
-      <c r="C10" s="130"/>
-      <c r="D10" s="130"/>
-      <c r="E10" s="130"/>
-      <c r="F10" s="130"/>
-      <c r="G10" s="130"/>
+      <c r="B10" s="129"/>
+      <c r="C10" s="129"/>
+      <c r="D10" s="129"/>
+      <c r="E10" s="129"/>
+      <c r="F10" s="129"/>
+      <c r="G10" s="129"/>
     </row>
     <row r="11" spans="1:8" s="17" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="16"/>
-      <c r="B11" s="125" t="s">
+      <c r="B11" s="124" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="125"/>
-      <c r="D11" s="125"/>
-      <c r="E11" s="125"/>
-      <c r="F11" s="125"/>
-      <c r="G11" s="125"/>
+      <c r="C11" s="124"/>
+      <c r="D11" s="124"/>
+      <c r="E11" s="124"/>
+      <c r="F11" s="124"/>
+      <c r="G11" s="124"/>
     </row>
     <row r="12" spans="1:8" s="17" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="16"/>
@@ -2122,8 +2125,8 @@
       <c r="C12" s="16"/>
       <c r="D12" s="19"/>
       <c r="E12" s="20"/>
-      <c r="F12" s="125"/>
-      <c r="G12" s="125"/>
+      <c r="F12" s="124"/>
+      <c r="G12" s="124"/>
     </row>
     <row r="13" spans="1:8" s="17" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="16"/>
@@ -2140,8 +2143,8 @@
         <f>data!B1</f>
         <v>0</v>
       </c>
-      <c r="F13" s="125"/>
-      <c r="G13" s="125"/>
+      <c r="F13" s="124"/>
+      <c r="G13" s="124"/>
     </row>
     <row r="14" spans="1:8" s="17" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16"/>
@@ -2156,8 +2159,8 @@
         <f>data!B2</f>
         <v>0</v>
       </c>
-      <c r="F14" s="125"/>
-      <c r="G14" s="125"/>
+      <c r="F14" s="124"/>
+      <c r="G14" s="124"/>
     </row>
     <row r="15" spans="1:8" s="17" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="16"/>
@@ -2208,10 +2211,10 @@
         <f>data!C1</f>
         <v>0</v>
       </c>
-      <c r="F17" s="125" t="s">
+      <c r="F17" s="124" t="s">
         <v>10</v>
       </c>
-      <c r="G17" s="125"/>
+      <c r="G17" s="124"/>
     </row>
     <row r="18" spans="1:7" s="17" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="16"/>
@@ -2226,8 +2229,8 @@
         <f>data!C2</f>
         <v>0</v>
       </c>
-      <c r="F18" s="125"/>
-      <c r="G18" s="125"/>
+      <c r="F18" s="124"/>
+      <c r="G18" s="124"/>
     </row>
     <row r="19" spans="1:7" s="17" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="16"/>
@@ -2357,10 +2360,10 @@
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
       <c r="E28" s="27"/>
-      <c r="F28" s="133" t="s">
+      <c r="F28" s="132" t="s">
         <v>17</v>
       </c>
-      <c r="G28" s="133"/>
+      <c r="G28" s="132"/>
     </row>
     <row r="29" spans="1:7" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
@@ -2368,10 +2371,10 @@
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
       <c r="E29" s="27"/>
-      <c r="F29" s="133" t="s">
+      <c r="F29" s="132" t="s">
         <v>18</v>
       </c>
-      <c r="G29" s="133"/>
+      <c r="G29" s="132"/>
     </row>
     <row r="30" spans="1:7" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
@@ -2404,10 +2407,10 @@
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
       <c r="E33" s="27"/>
-      <c r="F33" s="134" t="s">
+      <c r="F33" s="133" t="s">
         <v>19</v>
       </c>
-      <c r="G33" s="134"/>
+      <c r="G33" s="133"/>
       <c r="H33" s="31"/>
     </row>
     <row r="34" spans="1:8" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -2416,10 +2419,10 @@
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
       <c r="E34" s="27"/>
-      <c r="F34" s="132" t="s">
+      <c r="F34" s="131" t="s">
         <v>20</v>
       </c>
-      <c r="G34" s="132"/>
+      <c r="G34" s="131"/>
       <c r="H34" s="32"/>
     </row>
     <row r="35" spans="1:8" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -2566,8 +2569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K39"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="90" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A15" zoomScale="90" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27:E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2619,24 +2622,23 @@
       <c r="B6" s="95"/>
     </row>
     <row r="7" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="152" t="s">
+      <c r="A7" s="151" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="152"/>
-      <c r="C7" s="152"/>
-      <c r="D7" s="152"/>
-      <c r="E7" s="152"/>
+      <c r="B7" s="151"/>
+      <c r="C7" s="151"/>
+      <c r="D7" s="151"/>
+      <c r="E7" s="151"/>
       <c r="I7" s="35"/>
     </row>
     <row r="8" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="133" t="str">
-        <f>data!B8</f>
-        <v>Nomor : 449.1/        /UKM/2024</v>
-      </c>
-      <c r="B8" s="133"/>
-      <c r="C8" s="133"/>
-      <c r="D8" s="133"/>
-      <c r="E8" s="133"/>
+      <c r="A8" s="132" t="s">
+        <v>89</v>
+      </c>
+      <c r="B8" s="132"/>
+      <c r="C8" s="132"/>
+      <c r="D8" s="132"/>
+      <c r="E8" s="132"/>
       <c r="I8" s="35"/>
     </row>
     <row r="9" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -2653,10 +2655,10 @@
       <c r="C10" s="99" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="138" t="s">
+      <c r="D10" s="137" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="139"/>
+      <c r="E10" s="138"/>
     </row>
     <row r="11" spans="1:11" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="93">
@@ -2684,11 +2686,11 @@
     </row>
     <row r="13" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="38"/>
-      <c r="B13" s="153">
+      <c r="B13" s="152">
         <v>3</v>
       </c>
       <c r="C13" s="105" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D13" s="106">
         <f>data!B3</f>
@@ -2700,9 +2702,9 @@
     </row>
     <row r="14" spans="1:11" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="38"/>
-      <c r="B14" s="153"/>
+      <c r="B14" s="152"/>
       <c r="C14" s="100" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D14" s="108">
         <f>data!C3</f>
@@ -2712,9 +2714,9 @@
     </row>
     <row r="15" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="38"/>
-      <c r="B15" s="154"/>
+      <c r="B15" s="153"/>
       <c r="C15" s="100" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D15" s="110">
         <f>data!B4</f>
@@ -2752,143 +2754,143 @@
       <c r="C18" s="99" t="s">
         <v>28</v>
       </c>
-      <c r="D18" s="155" t="s">
+      <c r="D18" s="154" t="s">
         <v>29</v>
       </c>
-      <c r="E18" s="156"/>
+      <c r="E18" s="155"/>
       <c r="H18" s="35"/>
     </row>
     <row r="19" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="38"/>
-      <c r="B19" s="141">
+      <c r="B19" s="140">
         <v>6</v>
       </c>
       <c r="C19" s="114" t="s">
-        <v>86</v>
-      </c>
-      <c r="D19" s="138" t="s">
+        <v>84</v>
+      </c>
+      <c r="D19" s="137" t="s">
         <v>30</v>
       </c>
-      <c r="E19" s="139"/>
+      <c r="E19" s="138"/>
     </row>
     <row r="20" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="38"/>
-      <c r="B20" s="141"/>
+      <c r="B20" s="140"/>
       <c r="C20" s="115" t="s">
-        <v>87</v>
-      </c>
-      <c r="D20" s="148">
+        <v>85</v>
+      </c>
+      <c r="D20" s="147">
         <f>data!B7</f>
         <v>0</v>
       </c>
-      <c r="E20" s="149"/>
+      <c r="E20" s="148"/>
     </row>
     <row r="21" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="38"/>
-      <c r="B21" s="141">
+      <c r="B21" s="140">
         <v>7</v>
       </c>
       <c r="C21" s="114" t="s">
-        <v>88</v>
-      </c>
-      <c r="D21" s="138" t="s">
+        <v>86</v>
+      </c>
+      <c r="D21" s="137" t="s">
         <v>31</v>
       </c>
-      <c r="E21" s="139"/>
+      <c r="E21" s="138"/>
     </row>
     <row r="22" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="150"/>
+      <c r="B22" s="149"/>
       <c r="C22" s="100" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D22" s="98"/>
       <c r="E22" s="116"/>
     </row>
     <row r="23" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="38"/>
-      <c r="B23" s="151"/>
+      <c r="B23" s="150"/>
       <c r="C23" s="100" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D23" s="98">
         <f>D22</f>
         <v>0</v>
       </c>
-      <c r="E23" s="117"/>
+      <c r="E23" s="116"/>
     </row>
     <row r="24" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="38"/>
-      <c r="B24" s="136">
+      <c r="B24" s="135">
         <v>8</v>
       </c>
       <c r="C24" s="88" t="s">
         <v>32</v>
       </c>
-      <c r="D24" s="138" t="s">
+      <c r="D24" s="137" t="s">
         <v>6</v>
       </c>
-      <c r="E24" s="139"/>
+      <c r="E24" s="138"/>
     </row>
     <row r="25" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="38"/>
-      <c r="B25" s="137"/>
+      <c r="B25" s="136"/>
       <c r="C25" s="110"/>
-      <c r="D25" s="118"/>
+      <c r="D25" s="117"/>
       <c r="E25" s="111"/>
     </row>
     <row r="26" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="38"/>
       <c r="B26" s="90"/>
-      <c r="C26" s="119" t="s">
+      <c r="C26" s="118" t="s">
         <v>33</v>
       </c>
-      <c r="D26" s="120" t="s">
+      <c r="D26" s="119" t="s">
         <v>34</v>
       </c>
       <c r="E26" s="111"/>
     </row>
     <row r="27" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="38"/>
-      <c r="B27" s="140">
+      <c r="B27" s="139">
         <v>9</v>
       </c>
-      <c r="C27" s="121" t="s">
+      <c r="C27" s="120" t="s">
         <v>35</v>
       </c>
-      <c r="D27" s="142" t="s">
+      <c r="D27" s="141" t="s">
         <v>36</v>
       </c>
-      <c r="E27" s="143"/>
+      <c r="E27" s="142"/>
     </row>
     <row r="28" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="38"/>
-      <c r="B28" s="141"/>
-      <c r="C28" s="121" t="s">
+      <c r="B28" s="140"/>
+      <c r="C28" s="120" t="s">
         <v>37</v>
       </c>
-      <c r="D28" s="144" t="s">
+      <c r="D28" s="143" t="s">
         <v>38</v>
       </c>
-      <c r="E28" s="145"/>
+      <c r="E28" s="144"/>
     </row>
     <row r="29" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="38"/>
-      <c r="B29" s="141"/>
-      <c r="C29" s="122" t="s">
+      <c r="B29" s="140"/>
+      <c r="C29" s="121" t="s">
         <v>39</v>
       </c>
-      <c r="D29" s="146"/>
-      <c r="E29" s="147"/>
+      <c r="D29" s="145"/>
+      <c r="E29" s="146"/>
     </row>
     <row r="30" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="89">
         <v>10</v>
       </c>
-      <c r="C30" s="123" t="s">
+      <c r="C30" s="122" t="s">
         <v>40</v>
       </c>
       <c r="D30" s="99"/>
-      <c r="E30" s="124"/>
+      <c r="E30" s="123"/>
     </row>
     <row r="31" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="32" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -2909,10 +2911,10 @@
     <row r="34" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="92"/>
       <c r="C34" s="33"/>
-      <c r="D34" s="135" t="s">
+      <c r="D34" s="134" t="s">
         <v>25</v>
       </c>
-      <c r="E34" s="135"/>
+      <c r="E34" s="134"/>
     </row>
     <row r="35" spans="2:6" s="33" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="92"/>
@@ -2928,17 +2930,17 @@
     </row>
     <row r="38" spans="2:6" s="33" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="92"/>
-      <c r="D38" s="134" t="s">
+      <c r="D38" s="133" t="s">
         <v>19</v>
       </c>
-      <c r="E38" s="134"/>
+      <c r="E38" s="133"/>
     </row>
     <row r="39" spans="2:6" s="33" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="92"/>
-      <c r="D39" s="132" t="s">
+      <c r="D39" s="131" t="s">
         <v>20</v>
       </c>
-      <c r="E39" s="132"/>
+      <c r="E39" s="131"/>
     </row>
   </sheetData>
   <mergeCells count="19">
@@ -2972,8 +2974,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:G82"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A49" zoomScale="86" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A51" zoomScale="86" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D75" sqref="D75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2999,65 +3001,72 @@
       </c>
     </row>
     <row r="5" spans="2:7" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E5" s="33" t="str">
-        <f>data!B8</f>
-        <v>Nomor : 449.1/        /UKM/2024</v>
+      <c r="E5" s="33" t="s">
+        <v>90</v>
+      </c>
+      <c r="F5" s="33" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="2:7" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E6" s="40" t="s">
-        <v>44</v>
+        <v>46</v>
+      </c>
+      <c r="F6" s="33" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="7" spans="2:7" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E7" s="40" t="s">
-        <v>72</v>
-      </c>
-      <c r="F7" s="43"/>
+        <v>70</v>
+      </c>
+      <c r="F7" s="43" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="8" spans="2:7" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C8" s="44"/>
       <c r="D8" s="44"/>
       <c r="E8" s="40" t="s">
+        <v>92</v>
+      </c>
+      <c r="F8" s="164" t="str">
+        <f>": "&amp;data!B7</f>
+        <v xml:space="preserve">: </v>
+      </c>
+      <c r="G8" s="164"/>
+    </row>
+    <row r="9" spans="2:7" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E9" s="45"/>
+    </row>
+    <row r="10" spans="2:7" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E10" s="42"/>
+    </row>
+    <row r="11" spans="2:7" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="46" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="47" t="s">
         <v>45</v>
       </c>
-      <c r="F8" s="165">
+      <c r="D11" s="47"/>
+      <c r="E11" s="48" t="s">
+        <v>46</v>
+      </c>
+      <c r="F11" s="49"/>
+    </row>
+    <row r="12" spans="2:7" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="50"/>
+      <c r="C12" s="165">
         <f>data!B7</f>
         <v>0</v>
       </c>
-      <c r="G8" s="165"/>
-    </row>
-    <row r="9" spans="2:7" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E9" s="45"/>
-    </row>
-    <row r="10" spans="2:7" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E10" s="42"/>
-    </row>
-    <row r="11" spans="2:7" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="46" t="s">
-        <v>46</v>
-      </c>
-      <c r="C11" s="47" t="s">
-        <v>47</v>
-      </c>
-      <c r="D11" s="47"/>
-      <c r="E11" s="48" t="s">
-        <v>48</v>
-      </c>
-      <c r="F11" s="49"/>
-    </row>
-    <row r="12" spans="2:7" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="50"/>
-      <c r="C12" s="166">
-        <f>F8</f>
-        <v>0</v>
-      </c>
-      <c r="D12" s="166"/>
-      <c r="E12" s="167">
+      <c r="D12" s="165"/>
+      <c r="E12" s="166">
         <f>C12</f>
         <v>0</v>
       </c>
-      <c r="F12" s="168"/>
+      <c r="F12" s="167"/>
     </row>
     <row r="13" spans="2:7" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="50"/>
@@ -3065,10 +3074,7 @@
         <f>E7</f>
         <v>Pada Tanggal</v>
       </c>
-      <c r="D13" s="43">
-        <f>F7</f>
-        <v>0</v>
-      </c>
+      <c r="D13" s="43"/>
       <c r="E13" s="37" t="str">
         <f>E7</f>
         <v>Pada Tanggal</v>
@@ -3083,20 +3089,20 @@
       <c r="C14" s="40"/>
       <c r="D14" s="40"/>
       <c r="E14" s="37" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F14" s="52"/>
     </row>
     <row r="15" spans="2:7" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="50"/>
-      <c r="C15" s="135" t="s">
-        <v>50</v>
-      </c>
-      <c r="D15" s="135"/>
-      <c r="E15" s="163" t="s">
-        <v>50</v>
-      </c>
-      <c r="F15" s="162"/>
+      <c r="C15" s="134" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" s="134"/>
+      <c r="E15" s="162" t="s">
+        <v>48</v>
+      </c>
+      <c r="F15" s="161"/>
     </row>
     <row r="16" spans="2:7" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="50"/>
@@ -3118,59 +3124,59 @@
     </row>
     <row r="19" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="50"/>
-      <c r="C19" s="157" t="s">
-        <v>51</v>
-      </c>
-      <c r="D19" s="157"/>
-      <c r="E19" s="164" t="s">
-        <v>51</v>
-      </c>
-      <c r="F19" s="161"/>
+      <c r="C19" s="156" t="s">
+        <v>49</v>
+      </c>
+      <c r="D19" s="156"/>
+      <c r="E19" s="163" t="s">
+        <v>49</v>
+      </c>
+      <c r="F19" s="160"/>
     </row>
     <row r="20" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="54"/>
       <c r="C20" s="55" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D20" s="56"/>
       <c r="E20" s="57" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F20" s="58"/>
     </row>
     <row r="21" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="46" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C21" s="47"/>
       <c r="D21" s="49"/>
       <c r="E21" s="48" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F21" s="49"/>
     </row>
     <row r="22" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="50"/>
       <c r="C22" s="40" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D22" s="59">
         <f>C12</f>
         <v>0</v>
       </c>
       <c r="E22" s="85" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F22" s="60"/>
     </row>
     <row r="23" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="50"/>
       <c r="C23" s="40" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D23" s="61"/>
       <c r="E23" s="37" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F23" s="61"/>
     </row>
@@ -3179,20 +3185,20 @@
       <c r="C24" s="40"/>
       <c r="D24" s="52"/>
       <c r="E24" s="37" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F24" s="52"/>
     </row>
     <row r="25" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="50"/>
-      <c r="C25" s="135" t="s">
-        <v>50</v>
-      </c>
-      <c r="D25" s="162"/>
-      <c r="E25" s="163" t="s">
-        <v>50</v>
-      </c>
-      <c r="F25" s="162"/>
+      <c r="C25" s="134" t="s">
+        <v>48</v>
+      </c>
+      <c r="D25" s="161"/>
+      <c r="E25" s="162" t="s">
+        <v>48</v>
+      </c>
+      <c r="F25" s="161"/>
     </row>
     <row r="26" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="50"/>
@@ -3214,56 +3220,56 @@
     </row>
     <row r="29" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="50"/>
-      <c r="C29" s="157" t="s">
-        <v>51</v>
-      </c>
-      <c r="D29" s="161"/>
-      <c r="E29" s="157" t="s">
-        <v>51</v>
-      </c>
-      <c r="F29" s="161"/>
+      <c r="C29" s="156" t="s">
+        <v>49</v>
+      </c>
+      <c r="D29" s="160"/>
+      <c r="E29" s="156" t="s">
+        <v>49</v>
+      </c>
+      <c r="F29" s="160"/>
     </row>
     <row r="30" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="54"/>
       <c r="C30" s="55" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D30" s="58"/>
       <c r="E30" s="57" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F30" s="58"/>
     </row>
     <row r="31" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="46" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C31" s="47"/>
       <c r="D31" s="49"/>
       <c r="E31" s="48" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F31" s="49"/>
     </row>
     <row r="32" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="50"/>
       <c r="C32" s="40" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D32" s="63"/>
       <c r="E32" s="84" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F32" s="64"/>
     </row>
     <row r="33" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="50"/>
       <c r="C33" s="40" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D33" s="65"/>
       <c r="E33" s="83" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F33" s="65"/>
     </row>
@@ -3271,20 +3277,20 @@
       <c r="B34" s="50"/>
       <c r="C34" s="40"/>
       <c r="E34" s="37" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F34" s="66"/>
     </row>
     <row r="35" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="50"/>
-      <c r="C35" s="135" t="s">
-        <v>50</v>
-      </c>
-      <c r="D35" s="162"/>
-      <c r="E35" s="163" t="s">
-        <v>50</v>
-      </c>
-      <c r="F35" s="162"/>
+      <c r="C35" s="134" t="s">
+        <v>48</v>
+      </c>
+      <c r="D35" s="161"/>
+      <c r="E35" s="162" t="s">
+        <v>48</v>
+      </c>
+      <c r="F35" s="161"/>
     </row>
     <row r="36" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="50"/>
@@ -3306,41 +3312,41 @@
     </row>
     <row r="39" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="50"/>
-      <c r="C39" s="157" t="s">
-        <v>51</v>
-      </c>
-      <c r="D39" s="161"/>
-      <c r="E39" s="157" t="s">
-        <v>51</v>
-      </c>
-      <c r="F39" s="161"/>
+      <c r="C39" s="156" t="s">
+        <v>49</v>
+      </c>
+      <c r="D39" s="160"/>
+      <c r="E39" s="156" t="s">
+        <v>49</v>
+      </c>
+      <c r="F39" s="160"/>
     </row>
     <row r="40" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="54"/>
       <c r="C40" s="55" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D40" s="58"/>
       <c r="E40" s="57" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F40" s="58"/>
     </row>
     <row r="41" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="46" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C41" s="47"/>
       <c r="D41" s="49"/>
       <c r="E41" s="48" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F41" s="49"/>
     </row>
     <row r="42" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="50"/>
       <c r="C42" s="40" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D42" s="67"/>
       <c r="E42" s="68"/>
@@ -3349,7 +3355,7 @@
     <row r="43" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="50"/>
       <c r="C43" s="40" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D43" s="61"/>
       <c r="E43" s="62"/>
@@ -3359,20 +3365,20 @@
       <c r="B44" s="50"/>
       <c r="C44" s="40"/>
       <c r="E44" s="37" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F44" s="66"/>
     </row>
     <row r="45" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="50"/>
-      <c r="C45" s="135" t="s">
-        <v>50</v>
-      </c>
-      <c r="D45" s="162"/>
-      <c r="E45" s="163" t="s">
-        <v>50</v>
-      </c>
-      <c r="F45" s="162"/>
+      <c r="C45" s="134" t="s">
+        <v>48</v>
+      </c>
+      <c r="D45" s="161"/>
+      <c r="E45" s="162" t="s">
+        <v>48</v>
+      </c>
+      <c r="F45" s="161"/>
     </row>
     <row r="46" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="50"/>
@@ -3394,32 +3400,32 @@
     </row>
     <row r="49" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="50"/>
-      <c r="C49" s="157" t="s">
-        <v>51</v>
-      </c>
-      <c r="D49" s="161"/>
-      <c r="E49" s="164" t="s">
-        <v>51</v>
-      </c>
-      <c r="F49" s="161"/>
+      <c r="C49" s="156" t="s">
+        <v>49</v>
+      </c>
+      <c r="D49" s="160"/>
+      <c r="E49" s="163" t="s">
+        <v>49</v>
+      </c>
+      <c r="F49" s="160"/>
     </row>
     <row r="50" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="54"/>
       <c r="C50" s="55" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D50" s="58"/>
       <c r="E50" s="57" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F50" s="58"/>
     </row>
     <row r="51" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="50" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C51" s="70" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D51" s="70"/>
       <c r="E51" s="70"/>
@@ -3428,22 +3434,22 @@
     <row r="52" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="50"/>
       <c r="C52" s="33" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F52" s="53"/>
     </row>
     <row r="53" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="50"/>
       <c r="C53" s="33" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F53" s="72"/>
     </row>
     <row r="54" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B54" s="50"/>
-      <c r="C54" s="157"/>
-      <c r="D54" s="157"/>
-      <c r="E54" s="157"/>
+      <c r="C54" s="156"/>
+      <c r="D54" s="156"/>
+      <c r="E54" s="156"/>
       <c r="F54" s="73"/>
     </row>
     <row r="55" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3452,12 +3458,12 @@
     </row>
     <row r="56" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B56" s="50"/>
-      <c r="C56" s="133" t="s">
+      <c r="C56" s="132" t="s">
         <v>25</v>
       </c>
-      <c r="D56" s="133"/>
-      <c r="E56" s="133"/>
-      <c r="F56" s="158"/>
+      <c r="D56" s="132"/>
+      <c r="E56" s="132"/>
+      <c r="F56" s="157"/>
     </row>
     <row r="57" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B57" s="50"/>
@@ -3482,21 +3488,21 @@
     </row>
     <row r="60" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B60" s="50"/>
-      <c r="C60" s="159" t="s">
+      <c r="C60" s="158" t="s">
         <v>19</v>
       </c>
-      <c r="D60" s="159"/>
-      <c r="E60" s="159"/>
-      <c r="F60" s="160"/>
+      <c r="D60" s="158"/>
+      <c r="E60" s="158"/>
+      <c r="F60" s="159"/>
     </row>
     <row r="61" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B61" s="50"/>
-      <c r="C61" s="133" t="s">
+      <c r="C61" s="132" t="s">
         <v>20</v>
       </c>
-      <c r="D61" s="133"/>
-      <c r="E61" s="133"/>
-      <c r="F61" s="158"/>
+      <c r="D61" s="132"/>
+      <c r="E61" s="132"/>
+      <c r="F61" s="157"/>
     </row>
     <row r="62" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B62" s="54"/>
@@ -3507,10 +3513,10 @@
     </row>
     <row r="63" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B63" s="76" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C63" s="77" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D63" s="77"/>
       <c r="E63" s="78"/>
@@ -3518,30 +3524,30 @@
     </row>
     <row r="64" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B64" s="33" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="65" spans="2:3" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B65" s="33" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C65" s="33" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="66" spans="2:3" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C66" s="33" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="67" spans="2:3" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C67" s="33" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="68" spans="2:3" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C68" s="33" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="69" spans="2:3" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
feat: auto creating nomer surat tugas
</commit_message>
<xml_diff>
--- a/src/assets/sppd.xlsx
+++ b/src/assets/sppd.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8EBAA5C-CF54-4492-AC46-96295D073A32}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{651BC6C0-473D-473D-B35D-87E1E1378A6F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="94">
   <si>
     <t>SURAT TUGAS</t>
   </si>
@@ -1010,7 +1010,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="168">
+  <cellXfs count="170">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1196,9 +1196,6 @@
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1321,9 +1318,18 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1342,14 +1348,41 @@
     <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="27" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="26" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="24" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1360,18 +1393,9 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1390,36 +1414,33 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="24" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="27" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="26" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1429,29 +1450,14 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1927,7 +1933,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection sqref="A1:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1959,7 +1965,7 @@
       <c r="A5" t="s">
         <v>75</v>
       </c>
-      <c r="B5" s="86"/>
+      <c r="B5" s="85"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -1990,7 +1996,7 @@
   <dimension ref="A1:H52"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+      <selection activeCell="E8" sqref="E8:G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2019,28 +2025,28 @@
     <row r="2" spans="1:8" s="6" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="C2" s="7"/>
-      <c r="D2" s="125"/>
-      <c r="E2" s="125"/>
-      <c r="F2" s="125"/>
-      <c r="G2" s="125"/>
+      <c r="D2" s="127"/>
+      <c r="E2" s="127"/>
+      <c r="F2" s="127"/>
+      <c r="G2" s="127"/>
       <c r="H2" s="5"/>
     </row>
     <row r="3" spans="1:8" s="6" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="C3" s="7"/>
-      <c r="D3" s="126"/>
-      <c r="E3" s="126"/>
-      <c r="F3" s="126"/>
-      <c r="G3" s="126"/>
+      <c r="D3" s="128"/>
+      <c r="E3" s="128"/>
+      <c r="F3" s="128"/>
+      <c r="G3" s="128"/>
       <c r="H3" s="8"/>
     </row>
     <row r="4" spans="1:8" s="6" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="C4" s="7"/>
-      <c r="D4" s="127"/>
-      <c r="E4" s="127"/>
-      <c r="F4" s="127"/>
-      <c r="G4" s="127"/>
+      <c r="D4" s="129"/>
+      <c r="E4" s="129"/>
+      <c r="F4" s="129"/>
+      <c r="G4" s="129"/>
       <c r="H4" s="8"/>
     </row>
     <row r="5" spans="1:8" s="9" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2054,20 +2060,19 @@
     </row>
     <row r="6" spans="1:8" s="14" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
-      <c r="B6" s="128" t="s">
+      <c r="B6" s="130" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="128"/>
-      <c r="D6" s="128"/>
-      <c r="E6" s="128"/>
-      <c r="F6" s="128"/>
-      <c r="G6" s="128"/>
+      <c r="C6" s="130"/>
+      <c r="D6" s="130"/>
+      <c r="E6" s="130"/>
+      <c r="F6" s="130"/>
+      <c r="G6" s="130"/>
     </row>
     <row r="7" spans="1:8" s="14" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
-      <c r="B7" s="124" t="str">
-        <f>data!B8</f>
-        <v>Nomor : 449.1/        /UKM/2024</v>
+      <c r="B7" s="124" t="s">
+        <v>89</v>
       </c>
       <c r="C7" s="124"/>
       <c r="D7" s="124"/>
@@ -2084,29 +2089,29 @@
       <c r="D8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="130" t="s">
+      <c r="E8" s="132" t="s">
         <v>79</v>
       </c>
-      <c r="F8" s="130"/>
-      <c r="G8" s="130"/>
+      <c r="F8" s="132"/>
+      <c r="G8" s="132"/>
     </row>
     <row r="9" spans="1:8" s="14" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9"/>
       <c r="C9"/>
       <c r="D9"/>
-      <c r="E9" s="130"/>
-      <c r="F9" s="130"/>
-      <c r="G9" s="130"/>
+      <c r="E9" s="132"/>
+      <c r="F9" s="132"/>
+      <c r="G9" s="132"/>
     </row>
     <row r="10" spans="1:8" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
-      <c r="B10" s="129"/>
-      <c r="C10" s="129"/>
-      <c r="D10" s="129"/>
-      <c r="E10" s="129"/>
-      <c r="F10" s="129"/>
-      <c r="G10" s="129"/>
+      <c r="B10" s="131"/>
+      <c r="C10" s="131"/>
+      <c r="D10" s="131"/>
+      <c r="E10" s="131"/>
+      <c r="F10" s="131"/>
+      <c r="G10" s="131"/>
     </row>
     <row r="11" spans="1:8" s="17" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="16"/>
@@ -2139,7 +2144,7 @@
       <c r="D13" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="E13" s="81">
+      <c r="E13" s="167">
         <f>data!B1</f>
         <v>0</v>
       </c>
@@ -2155,7 +2160,7 @@
       <c r="D14" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="E14" s="81">
+      <c r="E14" s="167">
         <f>data!B2</f>
         <v>0</v>
       </c>
@@ -2171,7 +2176,7 @@
       <c r="D15" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="E15" s="81">
+      <c r="E15" s="167">
         <f>data!B3</f>
         <v>0</v>
       </c>
@@ -2189,7 +2194,7 @@
       <c r="D16" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="E16" s="81">
+      <c r="E16" s="167">
         <f>data!B4</f>
         <v>0</v>
       </c>
@@ -2207,7 +2212,7 @@
       <c r="D17" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="E17" s="81">
+      <c r="E17" s="167">
         <f>data!C1</f>
         <v>0</v>
       </c>
@@ -2225,7 +2230,7 @@
       <c r="D18" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="E18" s="81">
+      <c r="E18" s="167">
         <f>data!C2</f>
         <v>0</v>
       </c>
@@ -2241,7 +2246,7 @@
       <c r="D19" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="E19" s="81">
+      <c r="E19" s="167">
         <f>data!C3</f>
         <v>0</v>
       </c>
@@ -2259,7 +2264,7 @@
       <c r="D20" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="E20" s="81">
+      <c r="E20" s="167">
         <f>data!C4</f>
         <v>0</v>
       </c>
@@ -2295,11 +2300,11 @@
       <c r="D23" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="E23" s="26"/>
+      <c r="E23" s="168"/>
       <c r="F23" s="26"/>
       <c r="G23" s="4"/>
     </row>
-    <row r="24" spans="1:7" s="17" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" s="17" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="16"/>
       <c r="B24" s="16"/>
       <c r="C24" s="16" t="s">
@@ -2308,12 +2313,12 @@
       <c r="D24" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="E24" s="87">
+      <c r="E24" s="86">
         <f>data!B6</f>
         <v>0</v>
       </c>
       <c r="F24" s="20"/>
-      <c r="G24" s="82"/>
+      <c r="G24" s="81"/>
     </row>
     <row r="25" spans="1:7" s="14" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
@@ -2324,7 +2329,7 @@
       <c r="D25" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="E25" s="87">
+      <c r="E25" s="169">
         <f>data!B7</f>
         <v>0</v>
       </c>
@@ -2360,10 +2365,10 @@
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
       <c r="E28" s="27"/>
-      <c r="F28" s="132" t="s">
+      <c r="F28" s="125" t="s">
         <v>17</v>
       </c>
-      <c r="G28" s="132"/>
+      <c r="G28" s="125"/>
     </row>
     <row r="29" spans="1:7" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
@@ -2371,10 +2376,10 @@
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
       <c r="E29" s="27"/>
-      <c r="F29" s="132" t="s">
+      <c r="F29" s="125" t="s">
         <v>18</v>
       </c>
-      <c r="G29" s="132"/>
+      <c r="G29" s="125"/>
     </row>
     <row r="30" spans="1:7" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
@@ -2407,10 +2412,10 @@
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
       <c r="E33" s="27"/>
-      <c r="F33" s="133" t="s">
+      <c r="F33" s="126" t="s">
         <v>19</v>
       </c>
-      <c r="G33" s="133"/>
+      <c r="G33" s="126"/>
       <c r="H33" s="31"/>
     </row>
     <row r="34" spans="1:8" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -2419,10 +2424,10 @@
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
       <c r="E34" s="27"/>
-      <c r="F34" s="131" t="s">
+      <c r="F34" s="123" t="s">
         <v>20</v>
       </c>
-      <c r="G34" s="131"/>
+      <c r="G34" s="123"/>
       <c r="H34" s="32"/>
     </row>
     <row r="35" spans="1:8" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -2541,11 +2546,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="F33:G33"/>
     <mergeCell ref="F17:G17"/>
     <mergeCell ref="D2:G2"/>
     <mergeCell ref="D3:G3"/>
@@ -2558,6 +2558,11 @@
     <mergeCell ref="F13:G13"/>
     <mergeCell ref="F14:G14"/>
     <mergeCell ref="E8:G9"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="F33:G33"/>
   </mergeCells>
   <pageMargins left="0.59055118110236227" right="0.39370078740157483" top="0.59055118110236227" bottom="1.7716535433070868" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="5" scale="86" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
@@ -2569,14 +2574,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K39"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A15" zoomScale="90" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView view="pageBreakPreview" zoomScale="90" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D27" sqref="D27:E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.85546875" style="5" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" style="96" customWidth="1"/>
+    <col min="2" max="2" width="5.140625" style="95" customWidth="1"/>
     <col min="3" max="3" width="40.7109375" style="5" customWidth="1"/>
     <col min="4" max="4" width="15.5703125" style="5" customWidth="1"/>
     <col min="5" max="5" width="24.85546875" style="5" customWidth="1"/>
@@ -2585,179 +2590,179 @@
   <sheetData>
     <row r="1" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1"/>
-      <c r="B1" s="94"/>
+      <c r="B1" s="93"/>
       <c r="C1"/>
       <c r="D1"/>
       <c r="E1"/>
     </row>
     <row r="2" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2"/>
-      <c r="B2" s="94"/>
+      <c r="B2" s="93"/>
       <c r="C2"/>
       <c r="D2"/>
       <c r="E2"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3"/>
-      <c r="B3" s="94"/>
+      <c r="B3" s="93"/>
       <c r="C3"/>
       <c r="D3"/>
       <c r="E3"/>
     </row>
     <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4"/>
-      <c r="B4" s="94"/>
+      <c r="B4" s="93"/>
       <c r="C4"/>
       <c r="D4"/>
       <c r="E4"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5"/>
-      <c r="B5" s="94"/>
+      <c r="B5" s="93"/>
       <c r="C5"/>
       <c r="D5"/>
       <c r="E5"/>
     </row>
     <row r="6" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="95"/>
+      <c r="B6" s="94"/>
     </row>
     <row r="7" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="151" t="s">
+      <c r="A7" s="133" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="151"/>
-      <c r="C7" s="151"/>
-      <c r="D7" s="151"/>
-      <c r="E7" s="151"/>
+      <c r="B7" s="133"/>
+      <c r="C7" s="133"/>
+      <c r="D7" s="133"/>
+      <c r="E7" s="133"/>
       <c r="I7" s="35"/>
     </row>
     <row r="8" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="132" t="s">
+      <c r="A8" s="125" t="s">
         <v>89</v>
       </c>
-      <c r="B8" s="132"/>
-      <c r="C8" s="132"/>
-      <c r="D8" s="132"/>
-      <c r="E8" s="132"/>
+      <c r="B8" s="125"/>
+      <c r="C8" s="125"/>
+      <c r="D8" s="125"/>
+      <c r="E8" s="125"/>
       <c r="I8" s="35"/>
     </row>
     <row r="9" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="36"/>
-      <c r="B9" s="92"/>
+      <c r="B9" s="91"/>
       <c r="C9" s="36"/>
       <c r="D9" s="36"/>
       <c r="I9" s="35"/>
     </row>
     <row r="10" spans="1:11" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="89">
+      <c r="B10" s="88">
         <v>1</v>
       </c>
-      <c r="C10" s="99" t="s">
+      <c r="C10" s="98" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="137" t="s">
+      <c r="D10" s="134" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="138"/>
+      <c r="E10" s="135"/>
     </row>
     <row r="11" spans="1:11" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="93">
+      <c r="B11" s="92">
         <v>2</v>
       </c>
-      <c r="C11" s="100" t="s">
+      <c r="C11" s="99" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="101">
+      <c r="D11" s="100">
         <f>data!B1</f>
         <v>0</v>
       </c>
-      <c r="E11" s="102"/>
+      <c r="E11" s="101"/>
     </row>
     <row r="12" spans="1:11" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="93"/>
-      <c r="C12" s="100"/>
-      <c r="D12" s="103">
+      <c r="B12" s="92"/>
+      <c r="C12" s="99"/>
+      <c r="D12" s="102">
         <f>data!C1</f>
         <v>0</v>
       </c>
-      <c r="E12" s="104"/>
+      <c r="E12" s="103"/>
       <c r="H12" s="35"/>
       <c r="K12" s="35"/>
     </row>
     <row r="13" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="38"/>
-      <c r="B13" s="152">
+      <c r="B13" s="136">
         <v>3</v>
       </c>
-      <c r="C13" s="105" t="s">
+      <c r="C13" s="104" t="s">
         <v>81</v>
       </c>
-      <c r="D13" s="106">
+      <c r="D13" s="105">
         <f>data!B3</f>
         <v>0</v>
       </c>
-      <c r="E13" s="107"/>
+      <c r="E13" s="106"/>
       <c r="H13" s="35"/>
       <c r="K13" s="35"/>
     </row>
     <row r="14" spans="1:11" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="38"/>
-      <c r="B14" s="152"/>
-      <c r="C14" s="100" t="s">
+      <c r="B14" s="136"/>
+      <c r="C14" s="99" t="s">
         <v>82</v>
       </c>
-      <c r="D14" s="108">
+      <c r="D14" s="107">
         <f>data!C3</f>
         <v>0</v>
       </c>
-      <c r="E14" s="109"/>
+      <c r="E14" s="108"/>
     </row>
     <row r="15" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="38"/>
-      <c r="B15" s="153"/>
-      <c r="C15" s="100" t="s">
+      <c r="B15" s="137"/>
+      <c r="C15" s="99" t="s">
         <v>83</v>
       </c>
-      <c r="D15" s="110">
+      <c r="D15" s="109">
         <f>data!B4</f>
         <v>0</v>
       </c>
-      <c r="E15" s="111"/>
+      <c r="E15" s="110"/>
     </row>
     <row r="16" spans="1:11" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="38"/>
-      <c r="B16" s="97"/>
-      <c r="C16" s="100"/>
-      <c r="D16" s="110"/>
-      <c r="E16" s="111"/>
+      <c r="B16" s="96"/>
+      <c r="C16" s="99"/>
+      <c r="D16" s="109"/>
+      <c r="E16" s="110"/>
     </row>
     <row r="17" spans="1:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="38"/>
-      <c r="B17" s="91">
+      <c r="B17" s="90">
         <v>4</v>
       </c>
-      <c r="C17" s="99" t="s">
+      <c r="C17" s="98" t="s">
         <v>27</v>
       </c>
-      <c r="D17" s="112">
+      <c r="D17" s="111">
         <f>data!B6</f>
         <v>0</v>
       </c>
-      <c r="E17" s="113"/>
+      <c r="E17" s="112"/>
       <c r="H17" s="35"/>
     </row>
     <row r="18" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="38"/>
-      <c r="B18" s="91">
+      <c r="B18" s="90">
         <v>5</v>
       </c>
-      <c r="C18" s="99" t="s">
+      <c r="C18" s="98" t="s">
         <v>28</v>
       </c>
-      <c r="D18" s="154" t="s">
+      <c r="D18" s="138" t="s">
         <v>29</v>
       </c>
-      <c r="E18" s="155"/>
+      <c r="E18" s="139"/>
       <c r="H18" s="35"/>
     </row>
     <row r="19" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -2765,132 +2770,132 @@
       <c r="B19" s="140">
         <v>6</v>
       </c>
-      <c r="C19" s="114" t="s">
+      <c r="C19" s="113" t="s">
         <v>84</v>
       </c>
-      <c r="D19" s="137" t="s">
+      <c r="D19" s="134" t="s">
         <v>30</v>
       </c>
-      <c r="E19" s="138"/>
+      <c r="E19" s="135"/>
     </row>
     <row r="20" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="38"/>
       <c r="B20" s="140"/>
-      <c r="C20" s="115" t="s">
+      <c r="C20" s="114" t="s">
         <v>85</v>
       </c>
-      <c r="D20" s="147">
+      <c r="D20" s="141">
         <f>data!B7</f>
         <v>0</v>
       </c>
-      <c r="E20" s="148"/>
+      <c r="E20" s="142"/>
     </row>
     <row r="21" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="38"/>
       <c r="B21" s="140">
         <v>7</v>
       </c>
-      <c r="C21" s="114" t="s">
+      <c r="C21" s="113" t="s">
         <v>86</v>
       </c>
-      <c r="D21" s="137" t="s">
+      <c r="D21" s="134" t="s">
         <v>31</v>
       </c>
-      <c r="E21" s="138"/>
+      <c r="E21" s="135"/>
     </row>
     <row r="22" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="149"/>
-      <c r="C22" s="100" t="s">
+      <c r="B22" s="143"/>
+      <c r="C22" s="99" t="s">
         <v>87</v>
       </c>
-      <c r="D22" s="98"/>
-      <c r="E22" s="116"/>
+      <c r="D22" s="97"/>
+      <c r="E22" s="115"/>
     </row>
     <row r="23" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="38"/>
-      <c r="B23" s="150"/>
-      <c r="C23" s="100" t="s">
+      <c r="B23" s="144"/>
+      <c r="C23" s="99" t="s">
         <v>88</v>
       </c>
-      <c r="D23" s="98">
+      <c r="D23" s="97">
         <f>D22</f>
         <v>0</v>
       </c>
-      <c r="E23" s="116"/>
+      <c r="E23" s="115"/>
     </row>
     <row r="24" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="38"/>
-      <c r="B24" s="135">
+      <c r="B24" s="146">
         <v>8</v>
       </c>
-      <c r="C24" s="88" t="s">
+      <c r="C24" s="87" t="s">
         <v>32</v>
       </c>
-      <c r="D24" s="137" t="s">
+      <c r="D24" s="134" t="s">
         <v>6</v>
       </c>
-      <c r="E24" s="138"/>
+      <c r="E24" s="135"/>
     </row>
     <row r="25" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="38"/>
-      <c r="B25" s="136"/>
-      <c r="C25" s="110"/>
-      <c r="D25" s="117"/>
-      <c r="E25" s="111"/>
+      <c r="B25" s="147"/>
+      <c r="C25" s="109"/>
+      <c r="D25" s="116"/>
+      <c r="E25" s="110"/>
     </row>
     <row r="26" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="38"/>
-      <c r="B26" s="90"/>
-      <c r="C26" s="118" t="s">
+      <c r="B26" s="89"/>
+      <c r="C26" s="117" t="s">
         <v>33</v>
       </c>
-      <c r="D26" s="119" t="s">
+      <c r="D26" s="118" t="s">
         <v>34</v>
       </c>
-      <c r="E26" s="111"/>
+      <c r="E26" s="110"/>
     </row>
     <row r="27" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="38"/>
-      <c r="B27" s="139">
+      <c r="B27" s="148">
         <v>9</v>
       </c>
-      <c r="C27" s="120" t="s">
+      <c r="C27" s="119" t="s">
         <v>35</v>
       </c>
-      <c r="D27" s="141" t="s">
+      <c r="D27" s="149" t="s">
         <v>36</v>
       </c>
-      <c r="E27" s="142"/>
+      <c r="E27" s="150"/>
     </row>
     <row r="28" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="38"/>
       <c r="B28" s="140"/>
-      <c r="C28" s="120" t="s">
+      <c r="C28" s="119" t="s">
         <v>37</v>
       </c>
-      <c r="D28" s="143" t="s">
+      <c r="D28" s="151" t="s">
         <v>38</v>
       </c>
-      <c r="E28" s="144"/>
+      <c r="E28" s="152"/>
     </row>
     <row r="29" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="38"/>
       <c r="B29" s="140"/>
-      <c r="C29" s="121" t="s">
+      <c r="C29" s="120" t="s">
         <v>39</v>
       </c>
-      <c r="D29" s="145"/>
-      <c r="E29" s="146"/>
+      <c r="D29" s="153"/>
+      <c r="E29" s="154"/>
     </row>
     <row r="30" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="89">
+      <c r="B30" s="88">
         <v>10</v>
       </c>
-      <c r="C30" s="122" t="s">
+      <c r="C30" s="121" t="s">
         <v>40</v>
       </c>
-      <c r="D30" s="99"/>
-      <c r="E30" s="123"/>
+      <c r="D30" s="98"/>
+      <c r="E30" s="122"/>
     </row>
     <row r="31" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="32" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -2909,51 +2914,41 @@
       <c r="F33" s="80"/>
     </row>
     <row r="34" spans="2:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="92"/>
+      <c r="B34" s="91"/>
       <c r="C34" s="33"/>
-      <c r="D34" s="134" t="s">
+      <c r="D34" s="145" t="s">
         <v>25</v>
       </c>
-      <c r="E34" s="134"/>
+      <c r="E34" s="145"/>
     </row>
     <row r="35" spans="2:6" s="33" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="92"/>
+      <c r="B35" s="91"/>
       <c r="D35" s="42"/>
     </row>
     <row r="36" spans="2:6" s="33" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="92"/>
+      <c r="B36" s="91"/>
       <c r="D36" s="42"/>
     </row>
     <row r="37" spans="2:6" s="33" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="92"/>
+      <c r="B37" s="91"/>
       <c r="D37" s="42"/>
     </row>
     <row r="38" spans="2:6" s="33" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="92"/>
-      <c r="D38" s="133" t="s">
+      <c r="B38" s="91"/>
+      <c r="D38" s="126" t="s">
         <v>19</v>
       </c>
-      <c r="E38" s="133"/>
+      <c r="E38" s="126"/>
     </row>
     <row r="39" spans="2:6" s="33" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="92"/>
-      <c r="D39" s="131" t="s">
+      <c r="B39" s="91"/>
+      <c r="D39" s="123" t="s">
         <v>20</v>
       </c>
-      <c r="E39" s="131"/>
+      <c r="E39" s="123"/>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="A7:E7"/>
-    <mergeCell ref="A8:E8"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="B13:B15"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="B21:B23"/>
-    <mergeCell ref="D21:E21"/>
     <mergeCell ref="D34:E34"/>
     <mergeCell ref="D38:E38"/>
     <mergeCell ref="D39:E39"/>
@@ -2963,6 +2958,16 @@
     <mergeCell ref="D27:E27"/>
     <mergeCell ref="D28:E28"/>
     <mergeCell ref="D29:E29"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="A7:E7"/>
+    <mergeCell ref="A8:E8"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="D18:E18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.45" top="0.25" bottom="1.5" header="0.3" footer="0.3"/>
   <pageSetup paperSize="5" scale="92" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
@@ -2974,7 +2979,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:G82"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A51" zoomScale="86" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView view="pageBreakPreview" zoomScale="86" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D75" sqref="D75"/>
     </sheetView>
   </sheetViews>
@@ -3030,11 +3035,11 @@
       <c r="E8" s="40" t="s">
         <v>92</v>
       </c>
-      <c r="F8" s="164" t="str">
+      <c r="F8" s="158" t="str">
         <f>": "&amp;data!B7</f>
         <v xml:space="preserve">: </v>
       </c>
-      <c r="G8" s="164"/>
+      <c r="G8" s="158"/>
     </row>
     <row r="9" spans="2:7" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E9" s="45"/>
@@ -3057,16 +3062,16 @@
     </row>
     <row r="12" spans="2:7" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="50"/>
-      <c r="C12" s="165">
+      <c r="C12" s="159">
         <f>data!B7</f>
         <v>0</v>
       </c>
-      <c r="D12" s="165"/>
-      <c r="E12" s="166">
+      <c r="D12" s="159"/>
+      <c r="E12" s="160">
         <f>C12</f>
         <v>0</v>
       </c>
-      <c r="F12" s="167"/>
+      <c r="F12" s="161"/>
     </row>
     <row r="13" spans="2:7" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="50"/>
@@ -3095,14 +3100,14 @@
     </row>
     <row r="15" spans="2:7" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="50"/>
-      <c r="C15" s="134" t="s">
+      <c r="C15" s="145" t="s">
         <v>48</v>
       </c>
-      <c r="D15" s="134"/>
+      <c r="D15" s="145"/>
       <c r="E15" s="162" t="s">
         <v>48</v>
       </c>
-      <c r="F15" s="161"/>
+      <c r="F15" s="163"/>
     </row>
     <row r="16" spans="2:7" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="50"/>
@@ -3124,14 +3129,14 @@
     </row>
     <row r="19" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="50"/>
-      <c r="C19" s="156" t="s">
+      <c r="C19" s="155" t="s">
         <v>49</v>
       </c>
-      <c r="D19" s="156"/>
-      <c r="E19" s="163" t="s">
+      <c r="D19" s="155"/>
+      <c r="E19" s="156" t="s">
         <v>49</v>
       </c>
-      <c r="F19" s="160"/>
+      <c r="F19" s="157"/>
     </row>
     <row r="20" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="54"/>
@@ -3164,7 +3169,7 @@
         <f>C12</f>
         <v>0</v>
       </c>
-      <c r="E22" s="85" t="s">
+      <c r="E22" s="84" t="s">
         <v>52</v>
       </c>
       <c r="F22" s="60"/>
@@ -3191,14 +3196,14 @@
     </row>
     <row r="25" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="50"/>
-      <c r="C25" s="134" t="s">
+      <c r="C25" s="145" t="s">
         <v>48</v>
       </c>
-      <c r="D25" s="161"/>
+      <c r="D25" s="163"/>
       <c r="E25" s="162" t="s">
         <v>48</v>
       </c>
-      <c r="F25" s="161"/>
+      <c r="F25" s="163"/>
     </row>
     <row r="26" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="50"/>
@@ -3220,14 +3225,14 @@
     </row>
     <row r="29" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="50"/>
-      <c r="C29" s="156" t="s">
+      <c r="C29" s="155" t="s">
         <v>49</v>
       </c>
-      <c r="D29" s="160"/>
-      <c r="E29" s="156" t="s">
+      <c r="D29" s="157"/>
+      <c r="E29" s="155" t="s">
         <v>49</v>
       </c>
-      <c r="F29" s="160"/>
+      <c r="F29" s="157"/>
     </row>
     <row r="30" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="54"/>
@@ -3257,7 +3262,7 @@
         <v>56</v>
       </c>
       <c r="D32" s="63"/>
-      <c r="E32" s="84" t="s">
+      <c r="E32" s="83" t="s">
         <v>56</v>
       </c>
       <c r="F32" s="64"/>
@@ -3268,7 +3273,7 @@
         <v>53</v>
       </c>
       <c r="D33" s="65"/>
-      <c r="E33" s="83" t="s">
+      <c r="E33" s="82" t="s">
         <v>53</v>
       </c>
       <c r="F33" s="65"/>
@@ -3283,14 +3288,14 @@
     </row>
     <row r="35" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="50"/>
-      <c r="C35" s="134" t="s">
+      <c r="C35" s="145" t="s">
         <v>48</v>
       </c>
-      <c r="D35" s="161"/>
+      <c r="D35" s="163"/>
       <c r="E35" s="162" t="s">
         <v>48</v>
       </c>
-      <c r="F35" s="161"/>
+      <c r="F35" s="163"/>
     </row>
     <row r="36" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="50"/>
@@ -3312,14 +3317,14 @@
     </row>
     <row r="39" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="50"/>
-      <c r="C39" s="156" t="s">
+      <c r="C39" s="155" t="s">
         <v>49</v>
       </c>
-      <c r="D39" s="160"/>
-      <c r="E39" s="156" t="s">
+      <c r="D39" s="157"/>
+      <c r="E39" s="155" t="s">
         <v>49</v>
       </c>
-      <c r="F39" s="160"/>
+      <c r="F39" s="157"/>
     </row>
     <row r="40" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="54"/>
@@ -3371,14 +3376,14 @@
     </row>
     <row r="45" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="50"/>
-      <c r="C45" s="134" t="s">
+      <c r="C45" s="145" t="s">
         <v>48</v>
       </c>
-      <c r="D45" s="161"/>
+      <c r="D45" s="163"/>
       <c r="E45" s="162" t="s">
         <v>48</v>
       </c>
-      <c r="F45" s="161"/>
+      <c r="F45" s="163"/>
     </row>
     <row r="46" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="50"/>
@@ -3400,14 +3405,14 @@
     </row>
     <row r="49" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="50"/>
-      <c r="C49" s="156" t="s">
+      <c r="C49" s="155" t="s">
         <v>49</v>
       </c>
-      <c r="D49" s="160"/>
-      <c r="E49" s="163" t="s">
+      <c r="D49" s="157"/>
+      <c r="E49" s="156" t="s">
         <v>49</v>
       </c>
-      <c r="F49" s="160"/>
+      <c r="F49" s="157"/>
     </row>
     <row r="50" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="54"/>
@@ -3447,9 +3452,9 @@
     </row>
     <row r="54" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B54" s="50"/>
-      <c r="C54" s="156"/>
-      <c r="D54" s="156"/>
-      <c r="E54" s="156"/>
+      <c r="C54" s="155"/>
+      <c r="D54" s="155"/>
+      <c r="E54" s="155"/>
       <c r="F54" s="73"/>
     </row>
     <row r="55" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3458,12 +3463,12 @@
     </row>
     <row r="56" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B56" s="50"/>
-      <c r="C56" s="132" t="s">
+      <c r="C56" s="125" t="s">
         <v>25</v>
       </c>
-      <c r="D56" s="132"/>
-      <c r="E56" s="132"/>
-      <c r="F56" s="157"/>
+      <c r="D56" s="125"/>
+      <c r="E56" s="125"/>
+      <c r="F56" s="164"/>
     </row>
     <row r="57" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B57" s="50"/>
@@ -3488,21 +3493,21 @@
     </row>
     <row r="60" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B60" s="50"/>
-      <c r="C60" s="158" t="s">
+      <c r="C60" s="165" t="s">
         <v>19</v>
       </c>
-      <c r="D60" s="158"/>
-      <c r="E60" s="158"/>
-      <c r="F60" s="159"/>
+      <c r="D60" s="165"/>
+      <c r="E60" s="165"/>
+      <c r="F60" s="166"/>
     </row>
     <row r="61" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B61" s="50"/>
-      <c r="C61" s="132" t="s">
+      <c r="C61" s="125" t="s">
         <v>20</v>
       </c>
-      <c r="D61" s="132"/>
-      <c r="E61" s="132"/>
-      <c r="F61" s="157"/>
+      <c r="D61" s="125"/>
+      <c r="E61" s="125"/>
+      <c r="F61" s="164"/>
     </row>
     <row r="62" spans="2:6" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B62" s="54"/>
@@ -3570,19 +3575,6 @@
     <row r="82" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="E35:F35"/>
     <mergeCell ref="C54:E54"/>
     <mergeCell ref="C56:F56"/>
     <mergeCell ref="C60:F60"/>
@@ -3593,6 +3585,19 @@
     <mergeCell ref="E45:F45"/>
     <mergeCell ref="C49:D49"/>
     <mergeCell ref="E49:F49"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="E15:F15"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.43307086614173229" top="0.23622047244094491" bottom="1.4960629921259843" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="5" scale="86" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>

</xml_diff>